<commit_message>
Added working munchmo driver
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giorg\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\github_javaemus\arcadeflex-037b7\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
   </bookViews>
   <sheets>
     <sheet name="Playable" sheetId="2" r:id="rId1"/>
@@ -15986,15 +15986,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -16055,6 +16057,46 @@
       </c>
       <c r="P3" t="s">
         <v>4227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4014</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4015</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" t="s">
+        <v>4016</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4015</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" t="s">
+        <v>4018</v>
       </c>
     </row>
   </sheetData>
@@ -16066,8 +16108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1891" workbookViewId="0">
-      <selection activeCell="A1906" sqref="A1906:XFD1908"/>
+    <sheetView topLeftCell="A1801" workbookViewId="0">
+      <selection activeCell="A1815" sqref="A1815:XFD1816"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -55042,46 +55084,6 @@
         <v>4013</v>
       </c>
     </row>
-    <row r="1815" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1815" t="s">
-        <v>4014</v>
-      </c>
-      <c r="B1815" t="s">
-        <v>4015</v>
-      </c>
-      <c r="C1815" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1815" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1815" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1815" t="s">
-        <v>4016</v>
-      </c>
-    </row>
-    <row r="1816" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1816" t="s">
-        <v>4017</v>
-      </c>
-      <c r="B1816" t="s">
-        <v>4015</v>
-      </c>
-      <c r="C1816" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1816" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1816" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1816" t="s">
-        <v>4018</v>
-      </c>
-    </row>
     <row r="1817" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1817" t="s">
         <v>4019</v>

</xml_diff>

<commit_message>
Fixed astrocde issue. Now seems to work okay
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -15684,12 +15684,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -15704,9 +15716,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
@@ -22898,8 +22912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1712" workbookViewId="0">
-      <selection activeCell="A1727" sqref="A1727:XFD1735"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I188" sqref="I188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27115,7 +27129,7 @@
       <c r="E185" t="s">
         <v>533</v>
       </c>
-      <c r="F185" t="s">
+      <c r="F185" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K185" t="s">
@@ -27144,7 +27158,7 @@
       <c r="E186" t="s">
         <v>533</v>
       </c>
-      <c r="F186" t="s">
+      <c r="F186" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K186" t="s">
@@ -27173,7 +27187,7 @@
       <c r="E187" t="s">
         <v>533</v>
       </c>
-      <c r="F187" t="s">
+      <c r="F187" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K187" t="s">
@@ -27202,7 +27216,7 @@
       <c r="E188" t="s">
         <v>533</v>
       </c>
-      <c r="F188" t="s">
+      <c r="F188" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K188" t="s">
@@ -27231,7 +27245,7 @@
       <c r="E189" t="s">
         <v>533</v>
       </c>
-      <c r="F189" t="s">
+      <c r="F189" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K189" t="s">
@@ -27260,7 +27274,7 @@
       <c r="E190" t="s">
         <v>533</v>
       </c>
-      <c r="F190" t="s">
+      <c r="F190" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K190" t="s">
@@ -27289,7 +27303,7 @@
       <c r="E191" t="s">
         <v>533</v>
       </c>
-      <c r="F191" t="s">
+      <c r="F191" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K191" t="s">
@@ -27318,7 +27332,7 @@
       <c r="E192" t="s">
         <v>533</v>
       </c>
-      <c r="F192" t="s">
+      <c r="F192" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K192" t="s">
@@ -27347,7 +27361,7 @@
       <c r="E193" t="s">
         <v>533</v>
       </c>
-      <c r="F193" t="s">
+      <c r="F193" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K193" t="s">
@@ -27376,7 +27390,7 @@
       <c r="E194" t="s">
         <v>533</v>
       </c>
-      <c r="F194" t="s">
+      <c r="F194" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K194" t="s">
@@ -27405,7 +27419,7 @@
       <c r="E195" t="s">
         <v>533</v>
       </c>
-      <c r="F195" t="s">
+      <c r="F195" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K195" t="s">
@@ -27434,7 +27448,7 @@
       <c r="E196" t="s">
         <v>533</v>
       </c>
-      <c r="F196" t="s">
+      <c r="F196" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K196" t="s">
@@ -27463,7 +27477,7 @@
       <c r="E197" t="s">
         <v>533</v>
       </c>
-      <c r="F197" t="s">
+      <c r="F197" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K197" t="s">
@@ -27492,7 +27506,7 @@
       <c r="E198" t="s">
         <v>533</v>
       </c>
-      <c r="F198" t="s">
+      <c r="F198" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K198" t="s">
@@ -27521,7 +27535,7 @@
       <c r="E199" t="s">
         <v>533</v>
       </c>
-      <c r="F199" t="s">
+      <c r="F199" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K199" t="s">
@@ -27550,7 +27564,7 @@
       <c r="E200" t="s">
         <v>533</v>
       </c>
-      <c r="F200" t="s">
+      <c r="F200" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K200" t="s">
@@ -27579,7 +27593,7 @@
       <c r="E201" t="s">
         <v>533</v>
       </c>
-      <c r="F201" t="s">
+      <c r="F201" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K201" t="s">
@@ -27608,7 +27622,7 @@
       <c r="E202" t="s">
         <v>533</v>
       </c>
-      <c r="F202" t="s">
+      <c r="F202" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K202" t="s">
@@ -27637,7 +27651,7 @@
       <c r="E203" t="s">
         <v>533</v>
       </c>
-      <c r="F203" t="s">
+      <c r="F203" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K203" t="s">
@@ -27666,7 +27680,7 @@
       <c r="E204" t="s">
         <v>533</v>
       </c>
-      <c r="F204" t="s">
+      <c r="F204" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K204" t="s">
@@ -27695,7 +27709,7 @@
       <c r="E205" t="s">
         <v>533</v>
       </c>
-      <c r="F205" t="s">
+      <c r="F205" s="3" t="s">
         <v>698</v>
       </c>
       <c r="K205" t="s">
@@ -34097,7 +34111,7 @@
       <c r="E520" t="s">
         <v>1177</v>
       </c>
-      <c r="F520" t="s">
+      <c r="F520" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K520" t="s">
@@ -34123,7 +34137,7 @@
       <c r="E521" t="s">
         <v>1177</v>
       </c>
-      <c r="F521" t="s">
+      <c r="F521" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K521" t="s">
@@ -34149,7 +34163,7 @@
       <c r="E522" t="s">
         <v>1177</v>
       </c>
-      <c r="F522" t="s">
+      <c r="F522" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K522" t="s">
@@ -34175,7 +34189,7 @@
       <c r="E523" t="s">
         <v>1177</v>
       </c>
-      <c r="F523" t="s">
+      <c r="F523" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K523" t="s">
@@ -34201,7 +34215,7 @@
       <c r="E524" t="s">
         <v>1177</v>
       </c>
-      <c r="F524" t="s">
+      <c r="F524" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K524" t="s">
@@ -34227,7 +34241,7 @@
       <c r="E525" t="s">
         <v>1177</v>
       </c>
-      <c r="F525" t="s">
+      <c r="F525" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K525" t="s">
@@ -34253,7 +34267,7 @@
       <c r="E526" t="s">
         <v>1177</v>
       </c>
-      <c r="F526" t="s">
+      <c r="F526" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K526" t="s">
@@ -34279,7 +34293,7 @@
       <c r="E527" t="s">
         <v>1177</v>
       </c>
-      <c r="F527" t="s">
+      <c r="F527" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K527" t="s">
@@ -34509,7 +34523,7 @@
       <c r="D537" t="s">
         <v>23</v>
       </c>
-      <c r="E537" t="s">
+      <c r="E537" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K537" t="s">
@@ -34535,7 +34549,7 @@
       <c r="D538" t="s">
         <v>23</v>
       </c>
-      <c r="E538" t="s">
+      <c r="E538" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K538" t="s">
@@ -34584,7 +34598,7 @@
       <c r="D540" t="s">
         <v>23</v>
       </c>
-      <c r="E540" t="s">
+      <c r="E540" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K540" t="s">
@@ -34679,7 +34693,7 @@
       <c r="D544" t="s">
         <v>23</v>
       </c>
-      <c r="E544" t="s">
+      <c r="E544" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K544" t="s">
@@ -34705,7 +34719,7 @@
       <c r="D545" t="s">
         <v>23</v>
       </c>
-      <c r="E545" t="s">
+      <c r="E545" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K545" t="s">
@@ -34731,7 +34745,7 @@
       <c r="D546" t="s">
         <v>23</v>
       </c>
-      <c r="E546" t="s">
+      <c r="E546" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K546" t="s">
@@ -34918,7 +34932,7 @@
       <c r="D554" t="s">
         <v>23</v>
       </c>
-      <c r="E554" t="s">
+      <c r="E554" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K554" t="s">
@@ -34941,7 +34955,7 @@
       <c r="D555" t="s">
         <v>23</v>
       </c>
-      <c r="E555" t="s">
+      <c r="E555" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K555" t="s">
@@ -35016,7 +35030,7 @@
       <c r="D558" t="s">
         <v>23</v>
       </c>
-      <c r="E558" t="s">
+      <c r="E558" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K558" t="s">
@@ -35039,7 +35053,7 @@
       <c r="D559" t="s">
         <v>23</v>
       </c>
-      <c r="E559" t="s">
+      <c r="E559" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K559" t="s">
@@ -35111,7 +35125,7 @@
       <c r="E562" t="s">
         <v>23</v>
       </c>
-      <c r="F562" t="s">
+      <c r="F562" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K562" t="s">
@@ -35140,7 +35154,7 @@
       <c r="E563" t="s">
         <v>23</v>
       </c>
-      <c r="F563" t="s">
+      <c r="F563" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K563" t="s">
@@ -35169,7 +35183,7 @@
       <c r="E564" t="s">
         <v>23</v>
       </c>
-      <c r="F564" t="s">
+      <c r="F564" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K564" t="s">
@@ -35247,7 +35261,7 @@
       <c r="D567" t="s">
         <v>10</v>
       </c>
-      <c r="E567" t="s">
+      <c r="E567" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K567" t="s">
@@ -35270,7 +35284,7 @@
       <c r="D568" t="s">
         <v>10</v>
       </c>
-      <c r="E568" t="s">
+      <c r="E568" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K568" t="s">
@@ -35293,7 +35307,7 @@
       <c r="D569" t="s">
         <v>10</v>
       </c>
-      <c r="E569" t="s">
+      <c r="E569" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K569" t="s">
@@ -35465,7 +35479,7 @@
       <c r="C577" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D577" t="s">
+      <c r="D577" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K577" t="s">
@@ -35485,7 +35499,7 @@
       <c r="C578" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D578" t="s">
+      <c r="D578" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K578" t="s">
@@ -35505,7 +35519,7 @@
       <c r="C579" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D579" t="s">
+      <c r="D579" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K579" t="s">
@@ -35525,7 +35539,7 @@
       <c r="C580" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D580" t="s">
+      <c r="D580" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K580" t="s">
@@ -35596,7 +35610,7 @@
       <c r="C584" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D584" t="s">
+      <c r="D584" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K584" t="s">
@@ -58533,7 +58547,7 @@
       <c r="D1638" t="s">
         <v>579</v>
       </c>
-      <c r="E1638" t="s">
+      <c r="E1638" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K1638" t="s">
@@ -58559,7 +58573,7 @@
       <c r="D1639" t="s">
         <v>579</v>
       </c>
-      <c r="E1639" t="s">
+      <c r="E1639" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="K1639" t="s">

</xml_diff>

<commit_message>
Added working lsasquad,arkanoid driver
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
   </bookViews>
   <sheets>
     <sheet name="Playable" sheetId="2" r:id="rId1"/>
@@ -15993,10 +15993,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P401"/>
+  <dimension ref="A1:P410"/>
   <sheetViews>
-    <sheetView topLeftCell="A377" workbookViewId="0">
-      <selection activeCell="A406" sqref="A406"/>
+    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
+      <selection activeCell="A411" sqref="A411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24128,6 +24128,183 @@
         <v>1534</v>
       </c>
     </row>
+    <row r="402" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A402" s="4" t="s">
+        <v>1573</v>
+      </c>
+      <c r="B402" s="4" t="s">
+        <v>1574</v>
+      </c>
+      <c r="C402" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D402" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E402" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K402" s="4" t="s">
+        <v>1546</v>
+      </c>
+      <c r="P402" s="4" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="403" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A403" s="4" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B403" s="4" t="s">
+        <v>1574</v>
+      </c>
+      <c r="C403" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D403" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E403" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K403" s="4" t="s">
+        <v>1546</v>
+      </c>
+      <c r="P403" s="4" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="404" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A404" s="4" t="s">
+        <v>1617</v>
+      </c>
+      <c r="B404" s="4" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C404" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D404" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K404" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="P404" s="4" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="405" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A405" s="4" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B405" s="4" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C405" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D405" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K405" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="P405" s="4" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="406" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A406" s="4" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B406" s="4" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C406" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D406" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K406" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="P406" s="4" t="s">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="407" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A407" s="4" t="s">
+        <v>1626</v>
+      </c>
+      <c r="B407" s="4" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C407" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K407" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="P407" s="4" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="408" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A408" s="4" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B408" s="4" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C408" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K408" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="P408" s="4" t="s">
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="409" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A409" s="4" t="s">
+        <v>1630</v>
+      </c>
+      <c r="B409" s="4" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C409" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K409" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="P409" s="4" t="s">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="410" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A410" s="4" t="s">
+        <v>1632</v>
+      </c>
+      <c r="B410" s="4" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C410" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D410" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K410" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="P410" s="4" t="s">
+        <v>1633</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -24136,10 +24313,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24340,6 +24517,26 @@
         <v>1536</v>
       </c>
     </row>
+    <row r="10" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>1624</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>1625</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24347,10 +24544,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P285"/>
+  <dimension ref="A1:P275"/>
   <sheetViews>
-    <sheetView topLeftCell="A280" workbookViewId="0">
-      <selection activeCell="A303" sqref="A303:XFD303"/>
+    <sheetView topLeftCell="A257" workbookViewId="0">
+      <selection activeCell="A276" sqref="A276:XFD282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30117,203 +30314,6 @@
       </c>
       <c r="P275" t="s">
         <v>856</v>
-      </c>
-    </row>
-    <row r="276" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A276" s="4" t="s">
-        <v>1573</v>
-      </c>
-      <c r="B276" s="4" t="s">
-        <v>1574</v>
-      </c>
-      <c r="C276" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D276" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E276" s="4" t="s">
-        <v>1483</v>
-      </c>
-      <c r="K276" s="4" t="s">
-        <v>1546</v>
-      </c>
-      <c r="P276" s="4" t="s">
-        <v>1575</v>
-      </c>
-    </row>
-    <row r="277" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A277" s="4" t="s">
-        <v>1576</v>
-      </c>
-      <c r="B277" s="4" t="s">
-        <v>1574</v>
-      </c>
-      <c r="C277" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D277" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E277" s="4" t="s">
-        <v>1483</v>
-      </c>
-      <c r="K277" s="4" t="s">
-        <v>1546</v>
-      </c>
-      <c r="P277" s="4" t="s">
-        <v>1577</v>
-      </c>
-    </row>
-    <row r="278" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A278" s="4" t="s">
-        <v>1617</v>
-      </c>
-      <c r="B278" s="4" t="s">
-        <v>1618</v>
-      </c>
-      <c r="C278" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D278" s="4" t="s">
-        <v>1483</v>
-      </c>
-      <c r="K278" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="P278" s="4" t="s">
-        <v>1619</v>
-      </c>
-    </row>
-    <row r="279" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A279" s="4" t="s">
-        <v>1620</v>
-      </c>
-      <c r="B279" s="4" t="s">
-        <v>1618</v>
-      </c>
-      <c r="C279" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D279" s="4" t="s">
-        <v>1483</v>
-      </c>
-      <c r="K279" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="P279" s="4" t="s">
-        <v>1621</v>
-      </c>
-    </row>
-    <row r="280" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A280" s="4" t="s">
-        <v>1622</v>
-      </c>
-      <c r="B280" s="4" t="s">
-        <v>1618</v>
-      </c>
-      <c r="C280" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D280" s="4" t="s">
-        <v>1483</v>
-      </c>
-      <c r="K280" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="P280" s="4" t="s">
-        <v>1623</v>
-      </c>
-    </row>
-    <row r="281" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A281" s="4" t="s">
-        <v>1624</v>
-      </c>
-      <c r="B281" s="4" t="s">
-        <v>1618</v>
-      </c>
-      <c r="C281" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D281" s="4" t="s">
-        <v>1483</v>
-      </c>
-      <c r="K281" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="P281" s="4" t="s">
-        <v>1625</v>
-      </c>
-    </row>
-    <row r="282" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A282" s="4" t="s">
-        <v>1626</v>
-      </c>
-      <c r="B282" s="4" t="s">
-        <v>1618</v>
-      </c>
-      <c r="C282" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K282" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="P282" s="4" t="s">
-        <v>1627</v>
-      </c>
-    </row>
-    <row r="283" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A283" s="4" t="s">
-        <v>1628</v>
-      </c>
-      <c r="B283" s="4" t="s">
-        <v>1618</v>
-      </c>
-      <c r="C283" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K283" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="P283" s="4" t="s">
-        <v>1629</v>
-      </c>
-    </row>
-    <row r="284" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A284" s="4" t="s">
-        <v>1630</v>
-      </c>
-      <c r="B284" s="4" t="s">
-        <v>1618</v>
-      </c>
-      <c r="C284" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K284" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="P284" s="4" t="s">
-        <v>1631</v>
-      </c>
-    </row>
-    <row r="285" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A285" s="4" t="s">
-        <v>1632</v>
-      </c>
-      <c r="B285" s="4" t="s">
-        <v>1618</v>
-      </c>
-      <c r="C285" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D285" s="4" t="s">
-        <v>1483</v>
-      </c>
-      <c r="K285" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="P285" s="4" t="s">
-        <v>1633</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added working spacefb driver
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Playable" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Φύλλο1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="compatibility_list" localSheetId="3">Φύλλο1!$A$1:$P$1645</definedName>
+    <definedName name="compatibility_list" localSheetId="3">Φύλλο1!$A$1:$P$1640</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -15993,10 +15993,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P410"/>
+  <dimension ref="A1:P415"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
-      <selection activeCell="A411" sqref="A411"/>
+    <sheetView topLeftCell="A388" workbookViewId="0">
+      <selection activeCell="A416" sqref="A416"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24303,6 +24303,106 @@
       </c>
       <c r="P410" s="4" t="s">
         <v>1633</v>
+      </c>
+    </row>
+    <row r="411" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A411" t="s">
+        <v>4825</v>
+      </c>
+      <c r="B411" t="s">
+        <v>4826</v>
+      </c>
+      <c r="C411" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D411" t="s">
+        <v>814</v>
+      </c>
+      <c r="K411" t="s">
+        <v>200</v>
+      </c>
+      <c r="P411" t="s">
+        <v>4827</v>
+      </c>
+    </row>
+    <row r="412" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A412" t="s">
+        <v>4828</v>
+      </c>
+      <c r="B412" t="s">
+        <v>4826</v>
+      </c>
+      <c r="C412" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D412" t="s">
+        <v>814</v>
+      </c>
+      <c r="K412" t="s">
+        <v>200</v>
+      </c>
+      <c r="P412" t="s">
+        <v>4829</v>
+      </c>
+    </row>
+    <row r="413" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A413" t="s">
+        <v>4830</v>
+      </c>
+      <c r="B413" t="s">
+        <v>4826</v>
+      </c>
+      <c r="C413" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D413" t="s">
+        <v>814</v>
+      </c>
+      <c r="K413" t="s">
+        <v>200</v>
+      </c>
+      <c r="P413" t="s">
+        <v>4831</v>
+      </c>
+    </row>
+    <row r="414" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A414" t="s">
+        <v>4832</v>
+      </c>
+      <c r="B414" t="s">
+        <v>4826</v>
+      </c>
+      <c r="C414" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D414" t="s">
+        <v>814</v>
+      </c>
+      <c r="K414" t="s">
+        <v>200</v>
+      </c>
+      <c r="P414" t="s">
+        <v>4833</v>
+      </c>
+    </row>
+    <row r="415" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A415" t="s">
+        <v>4834</v>
+      </c>
+      <c r="B415" t="s">
+        <v>4826</v>
+      </c>
+      <c r="C415" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D415" t="s">
+        <v>814</v>
+      </c>
+      <c r="K415" t="s">
+        <v>200</v>
+      </c>
+      <c r="P415" t="s">
+        <v>4835</v>
       </c>
     </row>
   </sheetData>
@@ -30323,10 +30423,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1645"/>
+  <dimension ref="A1:P1640"/>
   <sheetViews>
-    <sheetView topLeftCell="A1622" workbookViewId="0">
-      <selection activeCell="H416" sqref="H416"/>
+    <sheetView tabSelected="1" topLeftCell="A1486" workbookViewId="0">
+      <selection activeCell="F1497" sqref="F1497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -63155,295 +63255,292 @@
     </row>
     <row r="1501" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1501" t="s">
-        <v>4825</v>
+        <v>4843</v>
       </c>
       <c r="B1501" t="s">
-        <v>4826</v>
+        <v>4844</v>
       </c>
       <c r="C1501" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D1501" t="s">
-        <v>814</v>
+        <v>23</v>
       </c>
       <c r="K1501" t="s">
-        <v>200</v>
+        <v>24</v>
       </c>
       <c r="P1501" t="s">
-        <v>4827</v>
+        <v>4845</v>
       </c>
     </row>
     <row r="1502" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1502" t="s">
-        <v>4828</v>
+        <v>4851</v>
       </c>
       <c r="B1502" t="s">
-        <v>4826</v>
+        <v>4852</v>
       </c>
       <c r="C1502" s="1" t="s">
-        <v>10</v>
+        <v>458</v>
       </c>
       <c r="D1502" t="s">
-        <v>814</v>
+        <v>1274</v>
       </c>
       <c r="K1502" t="s">
-        <v>200</v>
+        <v>105</v>
       </c>
       <c r="P1502" t="s">
-        <v>4829</v>
+        <v>4853</v>
       </c>
     </row>
     <row r="1503" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1503" t="s">
-        <v>4830</v>
+        <v>4854</v>
       </c>
       <c r="B1503" t="s">
-        <v>4826</v>
+        <v>4852</v>
       </c>
       <c r="C1503" s="1" t="s">
-        <v>10</v>
+        <v>458</v>
       </c>
       <c r="D1503" t="s">
-        <v>814</v>
+        <v>1274</v>
       </c>
       <c r="K1503" t="s">
-        <v>200</v>
+        <v>105</v>
       </c>
       <c r="P1503" t="s">
-        <v>4831</v>
+        <v>4855</v>
       </c>
     </row>
     <row r="1504" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1504" t="s">
-        <v>4832</v>
+        <v>4859</v>
       </c>
       <c r="B1504" t="s">
-        <v>4826</v>
+        <v>4860</v>
       </c>
       <c r="C1504" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1504" t="s">
-        <v>814</v>
+        <v>533</v>
       </c>
       <c r="K1504" t="s">
-        <v>200</v>
+        <v>3697</v>
       </c>
       <c r="P1504" t="s">
-        <v>4833</v>
+        <v>4861</v>
       </c>
     </row>
     <row r="1505" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1505" t="s">
-        <v>4834</v>
+        <v>4862</v>
       </c>
       <c r="B1505" t="s">
-        <v>4826</v>
+        <v>4863</v>
       </c>
       <c r="C1505" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1505" t="s">
-        <v>814</v>
-      </c>
-      <c r="K1505" t="s">
-        <v>200</v>
+        <v>533</v>
       </c>
       <c r="P1505" t="s">
-        <v>4835</v>
+        <v>4864</v>
       </c>
     </row>
     <row r="1506" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1506" t="s">
-        <v>4843</v>
+        <v>4865</v>
       </c>
       <c r="B1506" t="s">
-        <v>4844</v>
+        <v>4863</v>
       </c>
       <c r="C1506" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1506" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1506" t="s">
-        <v>24</v>
+        <v>533</v>
       </c>
       <c r="P1506" t="s">
-        <v>4845</v>
+        <v>4866</v>
       </c>
     </row>
     <row r="1507" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1507" t="s">
-        <v>4851</v>
+        <v>4867</v>
       </c>
       <c r="B1507" t="s">
-        <v>4852</v>
-      </c>
-      <c r="C1507" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="D1507" t="s">
-        <v>1274</v>
-      </c>
-      <c r="K1507" t="s">
-        <v>105</v>
+        <v>4868</v>
+      </c>
+      <c r="C1507" s="1">
+        <v>8080</v>
       </c>
       <c r="P1507" t="s">
-        <v>4853</v>
+        <v>4869</v>
       </c>
     </row>
     <row r="1508" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1508" t="s">
-        <v>4854</v>
+        <v>4870</v>
       </c>
       <c r="B1508" t="s">
-        <v>4852</v>
+        <v>4871</v>
       </c>
       <c r="C1508" s="1" t="s">
-        <v>458</v>
+        <v>4285</v>
       </c>
       <c r="D1508" t="s">
+        <v>4285</v>
+      </c>
+      <c r="E1508" t="s">
         <v>1274</v>
       </c>
+      <c r="F1508" t="s">
+        <v>1274</v>
+      </c>
       <c r="K1508" t="s">
-        <v>105</v>
+        <v>372</v>
+      </c>
+      <c r="L1508" t="s">
+        <v>621</v>
       </c>
       <c r="P1508" t="s">
-        <v>4855</v>
+        <v>4872</v>
       </c>
     </row>
     <row r="1509" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1509" t="s">
-        <v>4859</v>
+        <v>4891</v>
       </c>
       <c r="B1509" t="s">
-        <v>4860</v>
-      </c>
-      <c r="C1509" s="1" t="s">
-        <v>533</v>
+        <v>4892</v>
+      </c>
+      <c r="C1509" s="1">
+        <v>8080</v>
       </c>
       <c r="K1509" t="s">
-        <v>3697</v>
+        <v>459</v>
       </c>
       <c r="P1509" t="s">
-        <v>4861</v>
+        <v>4893</v>
       </c>
     </row>
     <row r="1510" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1510" t="s">
-        <v>4862</v>
+        <v>4896</v>
       </c>
       <c r="B1510" t="s">
-        <v>4863</v>
+        <v>4897</v>
       </c>
       <c r="C1510" s="1" t="s">
-        <v>533</v>
+        <v>4898</v>
+      </c>
+      <c r="D1510" t="s">
+        <v>814</v>
+      </c>
+      <c r="K1510" t="s">
+        <v>2675</v>
       </c>
       <c r="P1510" t="s">
-        <v>4864</v>
+        <v>4899</v>
       </c>
     </row>
     <row r="1511" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1511" t="s">
-        <v>4865</v>
+        <v>4900</v>
       </c>
       <c r="B1511" t="s">
-        <v>4863</v>
-      </c>
-      <c r="C1511" s="1" t="s">
-        <v>533</v>
+        <v>4901</v>
+      </c>
+      <c r="C1511" s="1">
+        <v>68000</v>
+      </c>
+      <c r="D1511" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1511" t="s">
+        <v>1501</v>
       </c>
       <c r="P1511" t="s">
-        <v>4866</v>
+        <v>4902</v>
       </c>
     </row>
     <row r="1512" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1512" t="s">
-        <v>4867</v>
+        <v>4903</v>
       </c>
       <c r="B1512" t="s">
-        <v>4868</v>
-      </c>
-      <c r="C1512" s="1">
-        <v>8080</v>
+        <v>4904</v>
+      </c>
+      <c r="C1512" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="K1512" t="s">
+        <v>105</v>
       </c>
       <c r="P1512" t="s">
-        <v>4869</v>
+        <v>4905</v>
       </c>
     </row>
     <row r="1513" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1513" t="s">
-        <v>4870</v>
+        <v>4926</v>
       </c>
       <c r="B1513" t="s">
-        <v>4871</v>
-      </c>
-      <c r="C1513" s="1" t="s">
-        <v>4285</v>
+        <v>4927</v>
+      </c>
+      <c r="C1513" s="1">
+        <v>68000</v>
       </c>
       <c r="D1513" t="s">
-        <v>4285</v>
-      </c>
-      <c r="E1513" t="s">
-        <v>1274</v>
-      </c>
-      <c r="F1513" t="s">
-        <v>1274</v>
+        <v>23</v>
       </c>
       <c r="K1513" t="s">
-        <v>372</v>
-      </c>
-      <c r="L1513" t="s">
-        <v>621</v>
+        <v>1641</v>
       </c>
       <c r="P1513" t="s">
-        <v>4872</v>
+        <v>4928</v>
       </c>
     </row>
     <row r="1514" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1514" t="s">
-        <v>4891</v>
+        <v>4929</v>
       </c>
       <c r="B1514" t="s">
-        <v>4892</v>
+        <v>4927</v>
       </c>
       <c r="C1514" s="1">
-        <v>8080</v>
+        <v>68000</v>
+      </c>
+      <c r="D1514" t="s">
+        <v>23</v>
       </c>
       <c r="K1514" t="s">
-        <v>459</v>
+        <v>1641</v>
       </c>
       <c r="P1514" t="s">
-        <v>4893</v>
+        <v>4930</v>
       </c>
     </row>
     <row r="1515" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1515" t="s">
-        <v>4896</v>
+        <v>4931</v>
       </c>
       <c r="B1515" t="s">
-        <v>4897</v>
-      </c>
-      <c r="C1515" s="1" t="s">
-        <v>4898</v>
+        <v>4927</v>
+      </c>
+      <c r="C1515" s="1">
+        <v>68000</v>
       </c>
       <c r="D1515" t="s">
-        <v>814</v>
+        <v>23</v>
       </c>
       <c r="K1515" t="s">
-        <v>2675</v>
+        <v>1641</v>
       </c>
       <c r="P1515" t="s">
-        <v>4899</v>
+        <v>4932</v>
       </c>
     </row>
     <row r="1516" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1516" t="s">
-        <v>4900</v>
+        <v>4933</v>
       </c>
       <c r="B1516" t="s">
-        <v>4901</v>
+        <v>4927</v>
       </c>
       <c r="C1516" s="1">
         <v>68000</v>
@@ -63452,32 +63549,35 @@
         <v>23</v>
       </c>
       <c r="K1516" t="s">
-        <v>1501</v>
+        <v>1641</v>
       </c>
       <c r="P1516" t="s">
-        <v>4902</v>
+        <v>4934</v>
       </c>
     </row>
     <row r="1517" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1517" t="s">
-        <v>4903</v>
+        <v>4935</v>
       </c>
       <c r="B1517" t="s">
-        <v>4904</v>
-      </c>
-      <c r="C1517" s="1" t="s">
-        <v>458</v>
+        <v>4927</v>
+      </c>
+      <c r="C1517" s="1">
+        <v>68000</v>
+      </c>
+      <c r="D1517" t="s">
+        <v>23</v>
       </c>
       <c r="K1517" t="s">
-        <v>105</v>
+        <v>1641</v>
       </c>
       <c r="P1517" t="s">
-        <v>4905</v>
+        <v>4936</v>
       </c>
     </row>
     <row r="1518" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1518" t="s">
-        <v>4926</v>
+        <v>4937</v>
       </c>
       <c r="B1518" t="s">
         <v>4927</v>
@@ -63492,12 +63592,12 @@
         <v>1641</v>
       </c>
       <c r="P1518" t="s">
-        <v>4928</v>
+        <v>4938</v>
       </c>
     </row>
     <row r="1519" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1519" t="s">
-        <v>4929</v>
+        <v>4939</v>
       </c>
       <c r="B1519" t="s">
         <v>4927</v>
@@ -63512,12 +63612,12 @@
         <v>1641</v>
       </c>
       <c r="P1519" t="s">
-        <v>4930</v>
+        <v>4940</v>
       </c>
     </row>
     <row r="1520" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1520" t="s">
-        <v>4931</v>
+        <v>4941</v>
       </c>
       <c r="B1520" t="s">
         <v>4927</v>
@@ -63532,12 +63632,12 @@
         <v>1641</v>
       </c>
       <c r="P1520" t="s">
-        <v>4932</v>
+        <v>4942</v>
       </c>
     </row>
     <row r="1521" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1521" t="s">
-        <v>4933</v>
+        <v>4943</v>
       </c>
       <c r="B1521" t="s">
         <v>4927</v>
@@ -63552,12 +63652,12 @@
         <v>1641</v>
       </c>
       <c r="P1521" t="s">
-        <v>4934</v>
+        <v>4944</v>
       </c>
     </row>
     <row r="1522" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1522" t="s">
-        <v>4935</v>
+        <v>4945</v>
       </c>
       <c r="B1522" t="s">
         <v>4927</v>
@@ -63572,12 +63672,12 @@
         <v>1641</v>
       </c>
       <c r="P1522" t="s">
-        <v>4936</v>
+        <v>4946</v>
       </c>
     </row>
     <row r="1523" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1523" t="s">
-        <v>4937</v>
+        <v>4947</v>
       </c>
       <c r="B1523" t="s">
         <v>4927</v>
@@ -63592,12 +63692,12 @@
         <v>1641</v>
       </c>
       <c r="P1523" t="s">
-        <v>4938</v>
+        <v>4948</v>
       </c>
     </row>
     <row r="1524" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1524" t="s">
-        <v>4939</v>
+        <v>4949</v>
       </c>
       <c r="B1524" t="s">
         <v>4927</v>
@@ -63612,12 +63712,12 @@
         <v>1641</v>
       </c>
       <c r="P1524" t="s">
-        <v>4940</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="1525" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1525" t="s">
-        <v>4941</v>
+        <v>4951</v>
       </c>
       <c r="B1525" t="s">
         <v>4927</v>
@@ -63632,12 +63732,12 @@
         <v>1641</v>
       </c>
       <c r="P1525" t="s">
-        <v>4942</v>
+        <v>4952</v>
       </c>
     </row>
     <row r="1526" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1526" t="s">
-        <v>4943</v>
+        <v>4953</v>
       </c>
       <c r="B1526" t="s">
         <v>4927</v>
@@ -63652,12 +63752,12 @@
         <v>1641</v>
       </c>
       <c r="P1526" t="s">
-        <v>4944</v>
+        <v>4954</v>
       </c>
     </row>
     <row r="1527" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1527" t="s">
-        <v>4945</v>
+        <v>4955</v>
       </c>
       <c r="B1527" t="s">
         <v>4927</v>
@@ -63672,12 +63772,12 @@
         <v>1641</v>
       </c>
       <c r="P1527" t="s">
-        <v>4946</v>
+        <v>4956</v>
       </c>
     </row>
     <row r="1528" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1528" t="s">
-        <v>4947</v>
+        <v>4957</v>
       </c>
       <c r="B1528" t="s">
         <v>4927</v>
@@ -63692,12 +63792,12 @@
         <v>1641</v>
       </c>
       <c r="P1528" t="s">
-        <v>4948</v>
+        <v>4958</v>
       </c>
     </row>
     <row r="1529" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1529" t="s">
-        <v>4949</v>
+        <v>4959</v>
       </c>
       <c r="B1529" t="s">
         <v>4927</v>
@@ -63712,12 +63812,12 @@
         <v>1641</v>
       </c>
       <c r="P1529" t="s">
-        <v>4950</v>
+        <v>4960</v>
       </c>
     </row>
     <row r="1530" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1530" t="s">
-        <v>4951</v>
+        <v>4961</v>
       </c>
       <c r="B1530" t="s">
         <v>4927</v>
@@ -63732,12 +63832,12 @@
         <v>1641</v>
       </c>
       <c r="P1530" t="s">
-        <v>4952</v>
+        <v>4962</v>
       </c>
     </row>
     <row r="1531" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1531" t="s">
-        <v>4953</v>
+        <v>4963</v>
       </c>
       <c r="B1531" t="s">
         <v>4927</v>
@@ -63752,12 +63852,12 @@
         <v>1641</v>
       </c>
       <c r="P1531" t="s">
-        <v>4954</v>
+        <v>4964</v>
       </c>
     </row>
     <row r="1532" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1532" t="s">
-        <v>4955</v>
+        <v>4965</v>
       </c>
       <c r="B1532" t="s">
         <v>4927</v>
@@ -63772,12 +63872,12 @@
         <v>1641</v>
       </c>
       <c r="P1532" t="s">
-        <v>4956</v>
+        <v>4966</v>
       </c>
     </row>
     <row r="1533" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1533" t="s">
-        <v>4957</v>
+        <v>4967</v>
       </c>
       <c r="B1533" t="s">
         <v>4927</v>
@@ -63792,12 +63892,12 @@
         <v>1641</v>
       </c>
       <c r="P1533" t="s">
-        <v>4958</v>
+        <v>4968</v>
       </c>
     </row>
     <row r="1534" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1534" t="s">
-        <v>4959</v>
+        <v>4969</v>
       </c>
       <c r="B1534" t="s">
         <v>4927</v>
@@ -63812,12 +63912,12 @@
         <v>1641</v>
       </c>
       <c r="P1534" t="s">
-        <v>4960</v>
+        <v>4970</v>
       </c>
     </row>
     <row r="1535" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1535" t="s">
-        <v>4961</v>
+        <v>4971</v>
       </c>
       <c r="B1535" t="s">
         <v>4927</v>
@@ -63832,12 +63932,12 @@
         <v>1641</v>
       </c>
       <c r="P1535" t="s">
-        <v>4962</v>
+        <v>4972</v>
       </c>
     </row>
     <row r="1536" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1536" t="s">
-        <v>4963</v>
+        <v>4973</v>
       </c>
       <c r="B1536" t="s">
         <v>4927</v>
@@ -63852,12 +63952,12 @@
         <v>1641</v>
       </c>
       <c r="P1536" t="s">
-        <v>4964</v>
+        <v>4974</v>
       </c>
     </row>
     <row r="1537" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1537" t="s">
-        <v>4965</v>
+        <v>4975</v>
       </c>
       <c r="B1537" t="s">
         <v>4927</v>
@@ -63872,12 +63972,12 @@
         <v>1641</v>
       </c>
       <c r="P1537" t="s">
-        <v>4966</v>
+        <v>4976</v>
       </c>
     </row>
     <row r="1538" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1538" t="s">
-        <v>4967</v>
+        <v>4977</v>
       </c>
       <c r="B1538" t="s">
         <v>4927</v>
@@ -63892,12 +63992,12 @@
         <v>1641</v>
       </c>
       <c r="P1538" t="s">
-        <v>4968</v>
+        <v>4978</v>
       </c>
     </row>
     <row r="1539" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1539" t="s">
-        <v>4969</v>
+        <v>4979</v>
       </c>
       <c r="B1539" t="s">
         <v>4927</v>
@@ -63912,12 +64012,12 @@
         <v>1641</v>
       </c>
       <c r="P1539" t="s">
-        <v>4970</v>
+        <v>4980</v>
       </c>
     </row>
     <row r="1540" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1540" t="s">
-        <v>4971</v>
+        <v>4981</v>
       </c>
       <c r="B1540" t="s">
         <v>4927</v>
@@ -63932,12 +64032,12 @@
         <v>1641</v>
       </c>
       <c r="P1540" t="s">
-        <v>4972</v>
+        <v>4982</v>
       </c>
     </row>
     <row r="1541" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1541" t="s">
-        <v>4973</v>
+        <v>4983</v>
       </c>
       <c r="B1541" t="s">
         <v>4927</v>
@@ -63952,12 +64052,12 @@
         <v>1641</v>
       </c>
       <c r="P1541" t="s">
-        <v>4974</v>
+        <v>4984</v>
       </c>
     </row>
     <row r="1542" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1542" t="s">
-        <v>4975</v>
+        <v>4985</v>
       </c>
       <c r="B1542" t="s">
         <v>4927</v>
@@ -63972,12 +64072,12 @@
         <v>1641</v>
       </c>
       <c r="P1542" t="s">
-        <v>4976</v>
+        <v>4986</v>
       </c>
     </row>
     <row r="1543" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1543" t="s">
-        <v>4977</v>
+        <v>4987</v>
       </c>
       <c r="B1543" t="s">
         <v>4927</v>
@@ -63992,12 +64092,12 @@
         <v>1641</v>
       </c>
       <c r="P1543" t="s">
-        <v>4978</v>
+        <v>4988</v>
       </c>
     </row>
     <row r="1544" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1544" t="s">
-        <v>4979</v>
+        <v>4989</v>
       </c>
       <c r="B1544" t="s">
         <v>4927</v>
@@ -64012,12 +64112,12 @@
         <v>1641</v>
       </c>
       <c r="P1544" t="s">
-        <v>4980</v>
+        <v>4990</v>
       </c>
     </row>
     <row r="1545" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1545" t="s">
-        <v>4981</v>
+        <v>4991</v>
       </c>
       <c r="B1545" t="s">
         <v>4927</v>
@@ -64032,12 +64132,12 @@
         <v>1641</v>
       </c>
       <c r="P1545" t="s">
-        <v>4982</v>
+        <v>4992</v>
       </c>
     </row>
     <row r="1546" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1546" t="s">
-        <v>4983</v>
+        <v>4993</v>
       </c>
       <c r="B1546" t="s">
         <v>4927</v>
@@ -64052,12 +64152,12 @@
         <v>1641</v>
       </c>
       <c r="P1546" t="s">
-        <v>4984</v>
+        <v>4994</v>
       </c>
     </row>
     <row r="1547" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1547" t="s">
-        <v>4985</v>
+        <v>4995</v>
       </c>
       <c r="B1547" t="s">
         <v>4927</v>
@@ -64072,12 +64172,12 @@
         <v>1641</v>
       </c>
       <c r="P1547" t="s">
-        <v>4986</v>
+        <v>4996</v>
       </c>
     </row>
     <row r="1548" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1548" t="s">
-        <v>4987</v>
+        <v>4997</v>
       </c>
       <c r="B1548" t="s">
         <v>4927</v>
@@ -64092,12 +64192,12 @@
         <v>1641</v>
       </c>
       <c r="P1548" t="s">
-        <v>4988</v>
+        <v>4998</v>
       </c>
     </row>
     <row r="1549" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1549" t="s">
-        <v>4989</v>
+        <v>4999</v>
       </c>
       <c r="B1549" t="s">
         <v>4927</v>
@@ -64112,12 +64212,12 @@
         <v>1641</v>
       </c>
       <c r="P1549" t="s">
-        <v>4990</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="1550" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1550" t="s">
-        <v>4991</v>
+        <v>5001</v>
       </c>
       <c r="B1550" t="s">
         <v>4927</v>
@@ -64132,12 +64232,12 @@
         <v>1641</v>
       </c>
       <c r="P1550" t="s">
-        <v>4992</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="1551" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1551" t="s">
-        <v>4993</v>
+        <v>5003</v>
       </c>
       <c r="B1551" t="s">
         <v>4927</v>
@@ -64152,12 +64252,12 @@
         <v>1641</v>
       </c>
       <c r="P1551" t="s">
-        <v>4994</v>
+        <v>5004</v>
       </c>
     </row>
     <row r="1552" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1552" t="s">
-        <v>4995</v>
+        <v>5005</v>
       </c>
       <c r="B1552" t="s">
         <v>4927</v>
@@ -64172,12 +64272,12 @@
         <v>1641</v>
       </c>
       <c r="P1552" t="s">
-        <v>4996</v>
+        <v>5006</v>
       </c>
     </row>
     <row r="1553" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1553" t="s">
-        <v>4997</v>
+        <v>5007</v>
       </c>
       <c r="B1553" t="s">
         <v>4927</v>
@@ -64192,12 +64292,12 @@
         <v>1641</v>
       </c>
       <c r="P1553" t="s">
-        <v>4998</v>
+        <v>5008</v>
       </c>
     </row>
     <row r="1554" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1554" t="s">
-        <v>4999</v>
+        <v>5009</v>
       </c>
       <c r="B1554" t="s">
         <v>4927</v>
@@ -64212,12 +64312,12 @@
         <v>1641</v>
       </c>
       <c r="P1554" t="s">
-        <v>5000</v>
+        <v>5010</v>
       </c>
     </row>
     <row r="1555" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1555" t="s">
-        <v>5001</v>
+        <v>5011</v>
       </c>
       <c r="B1555" t="s">
         <v>4927</v>
@@ -64232,12 +64332,12 @@
         <v>1641</v>
       </c>
       <c r="P1555" t="s">
-        <v>5002</v>
+        <v>5012</v>
       </c>
     </row>
     <row r="1556" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1556" t="s">
-        <v>5003</v>
+        <v>5013</v>
       </c>
       <c r="B1556" t="s">
         <v>4927</v>
@@ -64252,12 +64352,12 @@
         <v>1641</v>
       </c>
       <c r="P1556" t="s">
-        <v>5004</v>
+        <v>5014</v>
       </c>
     </row>
     <row r="1557" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1557" t="s">
-        <v>5005</v>
+        <v>5015</v>
       </c>
       <c r="B1557" t="s">
         <v>4927</v>
@@ -64272,12 +64372,12 @@
         <v>1641</v>
       </c>
       <c r="P1557" t="s">
-        <v>5006</v>
+        <v>5016</v>
       </c>
     </row>
     <row r="1558" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1558" t="s">
-        <v>5007</v>
+        <v>5017</v>
       </c>
       <c r="B1558" t="s">
         <v>4927</v>
@@ -64292,12 +64392,12 @@
         <v>1641</v>
       </c>
       <c r="P1558" t="s">
-        <v>5008</v>
+        <v>5018</v>
       </c>
     </row>
     <row r="1559" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1559" t="s">
-        <v>5009</v>
+        <v>5019</v>
       </c>
       <c r="B1559" t="s">
         <v>4927</v>
@@ -64312,12 +64412,12 @@
         <v>1641</v>
       </c>
       <c r="P1559" t="s">
-        <v>5010</v>
+        <v>5020</v>
       </c>
     </row>
     <row r="1560" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1560" t="s">
-        <v>5011</v>
+        <v>5021</v>
       </c>
       <c r="B1560" t="s">
         <v>4927</v>
@@ -64332,12 +64432,12 @@
         <v>1641</v>
       </c>
       <c r="P1560" t="s">
-        <v>5012</v>
+        <v>5022</v>
       </c>
     </row>
     <row r="1561" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1561" t="s">
-        <v>5013</v>
+        <v>5023</v>
       </c>
       <c r="B1561" t="s">
         <v>4927</v>
@@ -64352,12 +64452,12 @@
         <v>1641</v>
       </c>
       <c r="P1561" t="s">
-        <v>5014</v>
+        <v>5024</v>
       </c>
     </row>
     <row r="1562" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1562" t="s">
-        <v>5015</v>
+        <v>5025</v>
       </c>
       <c r="B1562" t="s">
         <v>4927</v>
@@ -64372,12 +64472,12 @@
         <v>1641</v>
       </c>
       <c r="P1562" t="s">
-        <v>5016</v>
+        <v>5026</v>
       </c>
     </row>
     <row r="1563" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1563" t="s">
-        <v>5017</v>
+        <v>5027</v>
       </c>
       <c r="B1563" t="s">
         <v>4927</v>
@@ -64392,12 +64492,12 @@
         <v>1641</v>
       </c>
       <c r="P1563" t="s">
-        <v>5018</v>
+        <v>5028</v>
       </c>
     </row>
     <row r="1564" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1564" t="s">
-        <v>5019</v>
+        <v>5029</v>
       </c>
       <c r="B1564" t="s">
         <v>4927</v>
@@ -64412,12 +64512,12 @@
         <v>1641</v>
       </c>
       <c r="P1564" t="s">
-        <v>5020</v>
+        <v>5030</v>
       </c>
     </row>
     <row r="1565" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1565" t="s">
-        <v>5021</v>
+        <v>5031</v>
       </c>
       <c r="B1565" t="s">
         <v>4927</v>
@@ -64432,12 +64532,12 @@
         <v>1641</v>
       </c>
       <c r="P1565" t="s">
-        <v>5022</v>
+        <v>5032</v>
       </c>
     </row>
     <row r="1566" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1566" t="s">
-        <v>5023</v>
+        <v>5033</v>
       </c>
       <c r="B1566" t="s">
         <v>4927</v>
@@ -64452,12 +64552,12 @@
         <v>1641</v>
       </c>
       <c r="P1566" t="s">
-        <v>5024</v>
+        <v>5034</v>
       </c>
     </row>
     <row r="1567" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1567" t="s">
-        <v>5025</v>
+        <v>5035</v>
       </c>
       <c r="B1567" t="s">
         <v>4927</v>
@@ -64472,12 +64572,12 @@
         <v>1641</v>
       </c>
       <c r="P1567" t="s">
-        <v>5026</v>
+        <v>5036</v>
       </c>
     </row>
     <row r="1568" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1568" t="s">
-        <v>5027</v>
+        <v>5037</v>
       </c>
       <c r="B1568" t="s">
         <v>4927</v>
@@ -64492,12 +64592,12 @@
         <v>1641</v>
       </c>
       <c r="P1568" t="s">
-        <v>5028</v>
+        <v>5038</v>
       </c>
     </row>
     <row r="1569" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1569" t="s">
-        <v>5029</v>
+        <v>5039</v>
       </c>
       <c r="B1569" t="s">
         <v>4927</v>
@@ -64512,12 +64612,12 @@
         <v>1641</v>
       </c>
       <c r="P1569" t="s">
-        <v>5030</v>
+        <v>5040</v>
       </c>
     </row>
     <row r="1570" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1570" t="s">
-        <v>5031</v>
+        <v>5041</v>
       </c>
       <c r="B1570" t="s">
         <v>4927</v>
@@ -64532,12 +64632,12 @@
         <v>1641</v>
       </c>
       <c r="P1570" t="s">
-        <v>5032</v>
+        <v>5042</v>
       </c>
     </row>
     <row r="1571" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1571" t="s">
-        <v>5033</v>
+        <v>5043</v>
       </c>
       <c r="B1571" t="s">
         <v>4927</v>
@@ -64552,12 +64652,12 @@
         <v>1641</v>
       </c>
       <c r="P1571" t="s">
-        <v>5034</v>
+        <v>5044</v>
       </c>
     </row>
     <row r="1572" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1572" t="s">
-        <v>5035</v>
+        <v>5045</v>
       </c>
       <c r="B1572" t="s">
         <v>4927</v>
@@ -64572,12 +64672,12 @@
         <v>1641</v>
       </c>
       <c r="P1572" t="s">
-        <v>5036</v>
+        <v>5046</v>
       </c>
     </row>
     <row r="1573" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1573" t="s">
-        <v>5037</v>
+        <v>5047</v>
       </c>
       <c r="B1573" t="s">
         <v>4927</v>
@@ -64592,12 +64692,12 @@
         <v>1641</v>
       </c>
       <c r="P1573" t="s">
-        <v>5038</v>
+        <v>5048</v>
       </c>
     </row>
     <row r="1574" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1574" t="s">
-        <v>5039</v>
+        <v>5049</v>
       </c>
       <c r="B1574" t="s">
         <v>4927</v>
@@ -64612,12 +64712,12 @@
         <v>1641</v>
       </c>
       <c r="P1574" t="s">
-        <v>5040</v>
+        <v>5050</v>
       </c>
     </row>
     <row r="1575" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1575" t="s">
-        <v>5041</v>
+        <v>5051</v>
       </c>
       <c r="B1575" t="s">
         <v>4927</v>
@@ -64632,12 +64732,12 @@
         <v>1641</v>
       </c>
       <c r="P1575" t="s">
-        <v>5042</v>
+        <v>5052</v>
       </c>
     </row>
     <row r="1576" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1576" t="s">
-        <v>5043</v>
+        <v>5053</v>
       </c>
       <c r="B1576" t="s">
         <v>4927</v>
@@ -64652,12 +64752,12 @@
         <v>1641</v>
       </c>
       <c r="P1576" t="s">
-        <v>5044</v>
+        <v>5054</v>
       </c>
     </row>
     <row r="1577" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1577" t="s">
-        <v>5045</v>
+        <v>5055</v>
       </c>
       <c r="B1577" t="s">
         <v>4927</v>
@@ -64672,12 +64772,12 @@
         <v>1641</v>
       </c>
       <c r="P1577" t="s">
-        <v>5046</v>
+        <v>5056</v>
       </c>
     </row>
     <row r="1578" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1578" t="s">
-        <v>5047</v>
+        <v>5057</v>
       </c>
       <c r="B1578" t="s">
         <v>4927</v>
@@ -64692,12 +64792,12 @@
         <v>1641</v>
       </c>
       <c r="P1578" t="s">
-        <v>5048</v>
+        <v>5058</v>
       </c>
     </row>
     <row r="1579" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1579" t="s">
-        <v>5049</v>
+        <v>5059</v>
       </c>
       <c r="B1579" t="s">
         <v>4927</v>
@@ -64712,12 +64812,12 @@
         <v>1641</v>
       </c>
       <c r="P1579" t="s">
-        <v>5050</v>
+        <v>5060</v>
       </c>
     </row>
     <row r="1580" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1580" t="s">
-        <v>5051</v>
+        <v>5061</v>
       </c>
       <c r="B1580" t="s">
         <v>4927</v>
@@ -64732,12 +64832,12 @@
         <v>1641</v>
       </c>
       <c r="P1580" t="s">
-        <v>5052</v>
+        <v>5062</v>
       </c>
     </row>
     <row r="1581" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1581" t="s">
-        <v>5053</v>
+        <v>5063</v>
       </c>
       <c r="B1581" t="s">
         <v>4927</v>
@@ -64752,12 +64852,12 @@
         <v>1641</v>
       </c>
       <c r="P1581" t="s">
-        <v>5054</v>
+        <v>5064</v>
       </c>
     </row>
     <row r="1582" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1582" t="s">
-        <v>5055</v>
+        <v>5065</v>
       </c>
       <c r="B1582" t="s">
         <v>4927</v>
@@ -64772,12 +64872,12 @@
         <v>1641</v>
       </c>
       <c r="P1582" t="s">
-        <v>5056</v>
+        <v>5066</v>
       </c>
     </row>
     <row r="1583" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1583" t="s">
-        <v>5057</v>
+        <v>5067</v>
       </c>
       <c r="B1583" t="s">
         <v>4927</v>
@@ -64792,12 +64892,12 @@
         <v>1641</v>
       </c>
       <c r="P1583" t="s">
-        <v>5058</v>
+        <v>5068</v>
       </c>
     </row>
     <row r="1584" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1584" t="s">
-        <v>5059</v>
+        <v>5069</v>
       </c>
       <c r="B1584" t="s">
         <v>4927</v>
@@ -64812,12 +64912,12 @@
         <v>1641</v>
       </c>
       <c r="P1584" t="s">
-        <v>5060</v>
+        <v>5070</v>
       </c>
     </row>
     <row r="1585" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1585" t="s">
-        <v>5061</v>
+        <v>5071</v>
       </c>
       <c r="B1585" t="s">
         <v>4927</v>
@@ -64832,12 +64932,12 @@
         <v>1641</v>
       </c>
       <c r="P1585" t="s">
-        <v>5062</v>
+        <v>5072</v>
       </c>
     </row>
     <row r="1586" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1586" t="s">
-        <v>5063</v>
+        <v>5073</v>
       </c>
       <c r="B1586" t="s">
         <v>4927</v>
@@ -64852,12 +64952,12 @@
         <v>1641</v>
       </c>
       <c r="P1586" t="s">
-        <v>5064</v>
+        <v>5074</v>
       </c>
     </row>
     <row r="1587" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1587" t="s">
-        <v>5065</v>
+        <v>5075</v>
       </c>
       <c r="B1587" t="s">
         <v>4927</v>
@@ -64872,12 +64972,12 @@
         <v>1641</v>
       </c>
       <c r="P1587" t="s">
-        <v>5066</v>
+        <v>5076</v>
       </c>
     </row>
     <row r="1588" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1588" t="s">
-        <v>5067</v>
+        <v>5077</v>
       </c>
       <c r="B1588" t="s">
         <v>4927</v>
@@ -64892,12 +64992,12 @@
         <v>1641</v>
       </c>
       <c r="P1588" t="s">
-        <v>5068</v>
+        <v>5078</v>
       </c>
     </row>
     <row r="1589" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1589" t="s">
-        <v>5069</v>
+        <v>5079</v>
       </c>
       <c r="B1589" t="s">
         <v>4927</v>
@@ -64912,12 +65012,12 @@
         <v>1641</v>
       </c>
       <c r="P1589" t="s">
-        <v>5070</v>
+        <v>5080</v>
       </c>
     </row>
     <row r="1590" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1590" t="s">
-        <v>5071</v>
+        <v>5081</v>
       </c>
       <c r="B1590" t="s">
         <v>4927</v>
@@ -64932,12 +65032,12 @@
         <v>1641</v>
       </c>
       <c r="P1590" t="s">
-        <v>5072</v>
+        <v>5082</v>
       </c>
     </row>
     <row r="1591" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1591" t="s">
-        <v>5073</v>
+        <v>5083</v>
       </c>
       <c r="B1591" t="s">
         <v>4927</v>
@@ -64952,12 +65052,12 @@
         <v>1641</v>
       </c>
       <c r="P1591" t="s">
-        <v>5074</v>
+        <v>5084</v>
       </c>
     </row>
     <row r="1592" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1592" t="s">
-        <v>5075</v>
+        <v>5085</v>
       </c>
       <c r="B1592" t="s">
         <v>4927</v>
@@ -64972,12 +65072,12 @@
         <v>1641</v>
       </c>
       <c r="P1592" t="s">
-        <v>5076</v>
+        <v>5086</v>
       </c>
     </row>
     <row r="1593" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1593" t="s">
-        <v>5077</v>
+        <v>5087</v>
       </c>
       <c r="B1593" t="s">
         <v>4927</v>
@@ -64992,12 +65092,12 @@
         <v>1641</v>
       </c>
       <c r="P1593" t="s">
-        <v>5078</v>
+        <v>5088</v>
       </c>
     </row>
     <row r="1594" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1594" t="s">
-        <v>5079</v>
+        <v>5089</v>
       </c>
       <c r="B1594" t="s">
         <v>4927</v>
@@ -65012,12 +65112,12 @@
         <v>1641</v>
       </c>
       <c r="P1594" t="s">
-        <v>5080</v>
+        <v>5090</v>
       </c>
     </row>
     <row r="1595" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1595" t="s">
-        <v>5081</v>
+        <v>5091</v>
       </c>
       <c r="B1595" t="s">
         <v>4927</v>
@@ -65032,12 +65132,12 @@
         <v>1641</v>
       </c>
       <c r="P1595" t="s">
-        <v>5082</v>
+        <v>5092</v>
       </c>
     </row>
     <row r="1596" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1596" t="s">
-        <v>5083</v>
+        <v>5093</v>
       </c>
       <c r="B1596" t="s">
         <v>4927</v>
@@ -65052,12 +65152,12 @@
         <v>1641</v>
       </c>
       <c r="P1596" t="s">
-        <v>5084</v>
+        <v>5094</v>
       </c>
     </row>
     <row r="1597" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1597" t="s">
-        <v>5085</v>
+        <v>5095</v>
       </c>
       <c r="B1597" t="s">
         <v>4927</v>
@@ -65072,12 +65172,12 @@
         <v>1641</v>
       </c>
       <c r="P1597" t="s">
-        <v>5086</v>
+        <v>5096</v>
       </c>
     </row>
     <row r="1598" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1598" t="s">
-        <v>5087</v>
+        <v>5097</v>
       </c>
       <c r="B1598" t="s">
         <v>4927</v>
@@ -65092,12 +65192,12 @@
         <v>1641</v>
       </c>
       <c r="P1598" t="s">
-        <v>5088</v>
+        <v>5098</v>
       </c>
     </row>
     <row r="1599" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1599" t="s">
-        <v>5089</v>
+        <v>5099</v>
       </c>
       <c r="B1599" t="s">
         <v>4927</v>
@@ -65112,12 +65212,12 @@
         <v>1641</v>
       </c>
       <c r="P1599" t="s">
-        <v>5090</v>
+        <v>5100</v>
       </c>
     </row>
     <row r="1600" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1600" t="s">
-        <v>5091</v>
+        <v>5101</v>
       </c>
       <c r="B1600" t="s">
         <v>4927</v>
@@ -65132,12 +65232,12 @@
         <v>1641</v>
       </c>
       <c r="P1600" t="s">
-        <v>5092</v>
+        <v>5102</v>
       </c>
     </row>
     <row r="1601" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1601" t="s">
-        <v>5093</v>
+        <v>5103</v>
       </c>
       <c r="B1601" t="s">
         <v>4927</v>
@@ -65152,12 +65252,12 @@
         <v>1641</v>
       </c>
       <c r="P1601" t="s">
-        <v>5094</v>
+        <v>5104</v>
       </c>
     </row>
     <row r="1602" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1602" t="s">
-        <v>5095</v>
+        <v>5105</v>
       </c>
       <c r="B1602" t="s">
         <v>4927</v>
@@ -65172,12 +65272,12 @@
         <v>1641</v>
       </c>
       <c r="P1602" t="s">
-        <v>5096</v>
+        <v>5106</v>
       </c>
     </row>
     <row r="1603" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1603" t="s">
-        <v>5097</v>
+        <v>5107</v>
       </c>
       <c r="B1603" t="s">
         <v>4927</v>
@@ -65192,12 +65292,12 @@
         <v>1641</v>
       </c>
       <c r="P1603" t="s">
-        <v>5098</v>
+        <v>5108</v>
       </c>
     </row>
     <row r="1604" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1604" t="s">
-        <v>5099</v>
+        <v>5109</v>
       </c>
       <c r="B1604" t="s">
         <v>4927</v>
@@ -65212,12 +65312,12 @@
         <v>1641</v>
       </c>
       <c r="P1604" t="s">
-        <v>5100</v>
+        <v>5110</v>
       </c>
     </row>
     <row r="1605" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1605" t="s">
-        <v>5101</v>
+        <v>5111</v>
       </c>
       <c r="B1605" t="s">
         <v>4927</v>
@@ -65232,12 +65332,12 @@
         <v>1641</v>
       </c>
       <c r="P1605" t="s">
-        <v>5102</v>
+        <v>5112</v>
       </c>
     </row>
     <row r="1606" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1606" t="s">
-        <v>5103</v>
+        <v>5113</v>
       </c>
       <c r="B1606" t="s">
         <v>4927</v>
@@ -65252,12 +65352,12 @@
         <v>1641</v>
       </c>
       <c r="P1606" t="s">
-        <v>5104</v>
+        <v>5114</v>
       </c>
     </row>
     <row r="1607" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1607" t="s">
-        <v>5105</v>
+        <v>5115</v>
       </c>
       <c r="B1607" t="s">
         <v>4927</v>
@@ -65272,12 +65372,12 @@
         <v>1641</v>
       </c>
       <c r="P1607" t="s">
-        <v>5106</v>
+        <v>5116</v>
       </c>
     </row>
     <row r="1608" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1608" t="s">
-        <v>5107</v>
+        <v>5117</v>
       </c>
       <c r="B1608" t="s">
         <v>4927</v>
@@ -65292,12 +65392,12 @@
         <v>1641</v>
       </c>
       <c r="P1608" t="s">
-        <v>5108</v>
+        <v>5118</v>
       </c>
     </row>
     <row r="1609" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1609" t="s">
-        <v>5109</v>
+        <v>5119</v>
       </c>
       <c r="B1609" t="s">
         <v>4927</v>
@@ -65312,12 +65412,12 @@
         <v>1641</v>
       </c>
       <c r="P1609" t="s">
-        <v>5110</v>
+        <v>5120</v>
       </c>
     </row>
     <row r="1610" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1610" t="s">
-        <v>5111</v>
+        <v>5121</v>
       </c>
       <c r="B1610" t="s">
         <v>4927</v>
@@ -65332,12 +65432,12 @@
         <v>1641</v>
       </c>
       <c r="P1610" t="s">
-        <v>5112</v>
+        <v>5122</v>
       </c>
     </row>
     <row r="1611" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1611" t="s">
-        <v>5113</v>
+        <v>5123</v>
       </c>
       <c r="B1611" t="s">
         <v>4927</v>
@@ -65352,12 +65452,12 @@
         <v>1641</v>
       </c>
       <c r="P1611" t="s">
-        <v>5114</v>
+        <v>5124</v>
       </c>
     </row>
     <row r="1612" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1612" t="s">
-        <v>5115</v>
+        <v>5125</v>
       </c>
       <c r="B1612" t="s">
         <v>4927</v>
@@ -65372,12 +65472,12 @@
         <v>1641</v>
       </c>
       <c r="P1612" t="s">
-        <v>5116</v>
+        <v>5126</v>
       </c>
     </row>
     <row r="1613" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1613" t="s">
-        <v>5117</v>
+        <v>5127</v>
       </c>
       <c r="B1613" t="s">
         <v>4927</v>
@@ -65392,12 +65492,12 @@
         <v>1641</v>
       </c>
       <c r="P1613" t="s">
-        <v>5118</v>
+        <v>5128</v>
       </c>
     </row>
     <row r="1614" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1614" t="s">
-        <v>5119</v>
+        <v>5129</v>
       </c>
       <c r="B1614" t="s">
         <v>4927</v>
@@ -65412,12 +65512,12 @@
         <v>1641</v>
       </c>
       <c r="P1614" t="s">
-        <v>5120</v>
+        <v>5130</v>
       </c>
     </row>
     <row r="1615" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1615" t="s">
-        <v>5121</v>
+        <v>5131</v>
       </c>
       <c r="B1615" t="s">
         <v>4927</v>
@@ -65432,12 +65532,12 @@
         <v>1641</v>
       </c>
       <c r="P1615" t="s">
-        <v>5122</v>
+        <v>5132</v>
       </c>
     </row>
     <row r="1616" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1616" t="s">
-        <v>5123</v>
+        <v>5133</v>
       </c>
       <c r="B1616" t="s">
         <v>4927</v>
@@ -65452,12 +65552,12 @@
         <v>1641</v>
       </c>
       <c r="P1616" t="s">
-        <v>5124</v>
+        <v>5134</v>
       </c>
     </row>
     <row r="1617" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1617" t="s">
-        <v>5125</v>
+        <v>5135</v>
       </c>
       <c r="B1617" t="s">
         <v>4927</v>
@@ -65472,12 +65572,12 @@
         <v>1641</v>
       </c>
       <c r="P1617" t="s">
-        <v>5126</v>
+        <v>5136</v>
       </c>
     </row>
     <row r="1618" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1618" t="s">
-        <v>5127</v>
+        <v>5137</v>
       </c>
       <c r="B1618" t="s">
         <v>4927</v>
@@ -65492,12 +65592,12 @@
         <v>1641</v>
       </c>
       <c r="P1618" t="s">
-        <v>5128</v>
+        <v>5138</v>
       </c>
     </row>
     <row r="1619" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1619" t="s">
-        <v>5129</v>
+        <v>5139</v>
       </c>
       <c r="B1619" t="s">
         <v>4927</v>
@@ -65512,12 +65612,12 @@
         <v>1641</v>
       </c>
       <c r="P1619" t="s">
-        <v>5130</v>
+        <v>5140</v>
       </c>
     </row>
     <row r="1620" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1620" t="s">
-        <v>5131</v>
+        <v>5141</v>
       </c>
       <c r="B1620" t="s">
         <v>4927</v>
@@ -65532,12 +65632,12 @@
         <v>1641</v>
       </c>
       <c r="P1620" t="s">
-        <v>5132</v>
+        <v>5142</v>
       </c>
     </row>
     <row r="1621" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1621" t="s">
-        <v>5133</v>
+        <v>5143</v>
       </c>
       <c r="B1621" t="s">
         <v>4927</v>
@@ -65552,12 +65652,12 @@
         <v>1641</v>
       </c>
       <c r="P1621" t="s">
-        <v>5134</v>
+        <v>5144</v>
       </c>
     </row>
     <row r="1622" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1622" t="s">
-        <v>5135</v>
+        <v>5145</v>
       </c>
       <c r="B1622" t="s">
         <v>4927</v>
@@ -65572,12 +65672,12 @@
         <v>1641</v>
       </c>
       <c r="P1622" t="s">
-        <v>5136</v>
+        <v>5146</v>
       </c>
     </row>
     <row r="1623" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1623" t="s">
-        <v>5137</v>
+        <v>5147</v>
       </c>
       <c r="B1623" t="s">
         <v>4927</v>
@@ -65592,12 +65692,12 @@
         <v>1641</v>
       </c>
       <c r="P1623" t="s">
-        <v>5138</v>
+        <v>5148</v>
       </c>
     </row>
     <row r="1624" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1624" t="s">
-        <v>5139</v>
+        <v>5149</v>
       </c>
       <c r="B1624" t="s">
         <v>4927</v>
@@ -65612,12 +65712,12 @@
         <v>1641</v>
       </c>
       <c r="P1624" t="s">
-        <v>5140</v>
+        <v>5150</v>
       </c>
     </row>
     <row r="1625" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1625" t="s">
-        <v>5141</v>
+        <v>5151</v>
       </c>
       <c r="B1625" t="s">
         <v>4927</v>
@@ -65632,12 +65732,12 @@
         <v>1641</v>
       </c>
       <c r="P1625" t="s">
-        <v>5142</v>
+        <v>5152</v>
       </c>
     </row>
     <row r="1626" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1626" t="s">
-        <v>5143</v>
+        <v>5153</v>
       </c>
       <c r="B1626" t="s">
         <v>4927</v>
@@ -65652,12 +65752,12 @@
         <v>1641</v>
       </c>
       <c r="P1626" t="s">
-        <v>5144</v>
+        <v>5154</v>
       </c>
     </row>
     <row r="1627" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1627" t="s">
-        <v>5145</v>
+        <v>5155</v>
       </c>
       <c r="B1627" t="s">
         <v>4927</v>
@@ -65672,12 +65772,12 @@
         <v>1641</v>
       </c>
       <c r="P1627" t="s">
-        <v>5146</v>
+        <v>5156</v>
       </c>
     </row>
     <row r="1628" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1628" t="s">
-        <v>5147</v>
+        <v>5157</v>
       </c>
       <c r="B1628" t="s">
         <v>4927</v>
@@ -65692,12 +65792,12 @@
         <v>1641</v>
       </c>
       <c r="P1628" t="s">
-        <v>5148</v>
+        <v>5158</v>
       </c>
     </row>
     <row r="1629" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1629" t="s">
-        <v>5149</v>
+        <v>5159</v>
       </c>
       <c r="B1629" t="s">
         <v>4927</v>
@@ -65712,12 +65812,12 @@
         <v>1641</v>
       </c>
       <c r="P1629" t="s">
-        <v>5150</v>
+        <v>5160</v>
       </c>
     </row>
     <row r="1630" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1630" t="s">
-        <v>5151</v>
+        <v>5161</v>
       </c>
       <c r="B1630" t="s">
         <v>4927</v>
@@ -65732,12 +65832,12 @@
         <v>1641</v>
       </c>
       <c r="P1630" t="s">
-        <v>5152</v>
+        <v>5162</v>
       </c>
     </row>
     <row r="1631" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1631" t="s">
-        <v>5153</v>
+        <v>5163</v>
       </c>
       <c r="B1631" t="s">
         <v>4927</v>
@@ -65752,12 +65852,12 @@
         <v>1641</v>
       </c>
       <c r="P1631" t="s">
-        <v>5154</v>
+        <v>5164</v>
       </c>
     </row>
     <row r="1632" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1632" t="s">
-        <v>5155</v>
+        <v>5165</v>
       </c>
       <c r="B1632" t="s">
         <v>4927</v>
@@ -65772,12 +65872,12 @@
         <v>1641</v>
       </c>
       <c r="P1632" t="s">
-        <v>5156</v>
+        <v>5166</v>
       </c>
     </row>
     <row r="1633" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1633" t="s">
-        <v>5157</v>
+        <v>5167</v>
       </c>
       <c r="B1633" t="s">
         <v>4927</v>
@@ -65792,12 +65892,12 @@
         <v>1641</v>
       </c>
       <c r="P1633" t="s">
-        <v>5158</v>
+        <v>5168</v>
       </c>
     </row>
     <row r="1634" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1634" t="s">
-        <v>5159</v>
+        <v>5169</v>
       </c>
       <c r="B1634" t="s">
         <v>4927</v>
@@ -65812,12 +65912,12 @@
         <v>1641</v>
       </c>
       <c r="P1634" t="s">
-        <v>5160</v>
+        <v>5170</v>
       </c>
     </row>
     <row r="1635" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1635" t="s">
-        <v>5161</v>
+        <v>5171</v>
       </c>
       <c r="B1635" t="s">
         <v>4927</v>
@@ -65832,12 +65932,12 @@
         <v>1641</v>
       </c>
       <c r="P1635" t="s">
-        <v>5162</v>
+        <v>5172</v>
       </c>
     </row>
     <row r="1636" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1636" t="s">
-        <v>5163</v>
+        <v>5173</v>
       </c>
       <c r="B1636" t="s">
         <v>4927</v>
@@ -65852,12 +65952,12 @@
         <v>1641</v>
       </c>
       <c r="P1636" t="s">
-        <v>5164</v>
+        <v>5174</v>
       </c>
     </row>
     <row r="1637" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1637" t="s">
-        <v>5165</v>
+        <v>5175</v>
       </c>
       <c r="B1637" t="s">
         <v>4927</v>
@@ -65872,12 +65972,12 @@
         <v>1641</v>
       </c>
       <c r="P1637" t="s">
-        <v>5166</v>
+        <v>5176</v>
       </c>
     </row>
     <row r="1638" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1638" t="s">
-        <v>5167</v>
+        <v>5177</v>
       </c>
       <c r="B1638" t="s">
         <v>4927</v>
@@ -65892,12 +65992,12 @@
         <v>1641</v>
       </c>
       <c r="P1638" t="s">
-        <v>5168</v>
+        <v>5178</v>
       </c>
     </row>
     <row r="1639" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1639" t="s">
-        <v>5169</v>
+        <v>5179</v>
       </c>
       <c r="B1639" t="s">
         <v>4927</v>
@@ -65912,12 +66012,12 @@
         <v>1641</v>
       </c>
       <c r="P1639" t="s">
-        <v>5170</v>
+        <v>5180</v>
       </c>
     </row>
     <row r="1640" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1640" t="s">
-        <v>5171</v>
+        <v>5181</v>
       </c>
       <c r="B1640" t="s">
         <v>4927</v>
@@ -65932,106 +66032,6 @@
         <v>1641</v>
       </c>
       <c r="P1640" t="s">
-        <v>5172</v>
-      </c>
-    </row>
-    <row r="1641" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1641" t="s">
-        <v>5173</v>
-      </c>
-      <c r="B1641" t="s">
-        <v>4927</v>
-      </c>
-      <c r="C1641" s="1">
-        <v>68000</v>
-      </c>
-      <c r="D1641" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1641" t="s">
-        <v>1641</v>
-      </c>
-      <c r="P1641" t="s">
-        <v>5174</v>
-      </c>
-    </row>
-    <row r="1642" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1642" t="s">
-        <v>5175</v>
-      </c>
-      <c r="B1642" t="s">
-        <v>4927</v>
-      </c>
-      <c r="C1642" s="1">
-        <v>68000</v>
-      </c>
-      <c r="D1642" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1642" t="s">
-        <v>1641</v>
-      </c>
-      <c r="P1642" t="s">
-        <v>5176</v>
-      </c>
-    </row>
-    <row r="1643" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1643" t="s">
-        <v>5177</v>
-      </c>
-      <c r="B1643" t="s">
-        <v>4927</v>
-      </c>
-      <c r="C1643" s="1">
-        <v>68000</v>
-      </c>
-      <c r="D1643" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1643" t="s">
-        <v>1641</v>
-      </c>
-      <c r="P1643" t="s">
-        <v>5178</v>
-      </c>
-    </row>
-    <row r="1644" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1644" t="s">
-        <v>5179</v>
-      </c>
-      <c r="B1644" t="s">
-        <v>4927</v>
-      </c>
-      <c r="C1644" s="1">
-        <v>68000</v>
-      </c>
-      <c r="D1644" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1644" t="s">
-        <v>1641</v>
-      </c>
-      <c r="P1644" t="s">
-        <v>5180</v>
-      </c>
-    </row>
-    <row r="1645" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1645" t="s">
-        <v>5181</v>
-      </c>
-      <c r="B1645" t="s">
-        <v>4927</v>
-      </c>
-      <c r="C1645" s="1">
-        <v>68000</v>
-      </c>
-      <c r="D1645" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1645" t="s">
-        <v>1641</v>
-      </c>
-      <c r="P1645" t="s">
         <v>5182</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added working snk driver
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
   </bookViews>
   <sheets>
     <sheet name="Playable" sheetId="2" r:id="rId1"/>
@@ -16000,10 +16000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P444"/>
+  <dimension ref="A1:P467"/>
   <sheetViews>
-    <sheetView topLeftCell="A418" workbookViewId="0">
-      <selection activeCell="G434" sqref="G434"/>
+    <sheetView tabSelected="1" topLeftCell="A442" workbookViewId="0">
+      <selection activeCell="A468" sqref="A468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25016,6 +25016,541 @@
         <v>3203</v>
       </c>
     </row>
+    <row r="445" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A445" t="s">
+        <v>4027</v>
+      </c>
+      <c r="B445" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C445" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D445" t="s">
+        <v>10</v>
+      </c>
+      <c r="E445" t="s">
+        <v>23</v>
+      </c>
+      <c r="K445" t="s">
+        <v>371</v>
+      </c>
+      <c r="P445" t="s">
+        <v>4029</v>
+      </c>
+    </row>
+    <row r="446" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A446" t="s">
+        <v>4030</v>
+      </c>
+      <c r="B446" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C446" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D446" t="s">
+        <v>10</v>
+      </c>
+      <c r="E446" t="s">
+        <v>23</v>
+      </c>
+      <c r="K446" t="s">
+        <v>371</v>
+      </c>
+      <c r="P446" t="s">
+        <v>4031</v>
+      </c>
+    </row>
+    <row r="447" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A447" t="s">
+        <v>4032</v>
+      </c>
+      <c r="B447" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C447" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D447" t="s">
+        <v>10</v>
+      </c>
+      <c r="E447" t="s">
+        <v>23</v>
+      </c>
+      <c r="K447" t="s">
+        <v>4033</v>
+      </c>
+      <c r="P447" t="s">
+        <v>4034</v>
+      </c>
+    </row>
+    <row r="448" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A448" t="s">
+        <v>4035</v>
+      </c>
+      <c r="B448" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C448" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D448" t="s">
+        <v>10</v>
+      </c>
+      <c r="E448" t="s">
+        <v>23</v>
+      </c>
+      <c r="K448" t="s">
+        <v>4033</v>
+      </c>
+      <c r="P448" t="s">
+        <v>4036</v>
+      </c>
+    </row>
+    <row r="449" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A449" t="s">
+        <v>4037</v>
+      </c>
+      <c r="B449" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C449" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D449" t="s">
+        <v>10</v>
+      </c>
+      <c r="E449" t="s">
+        <v>23</v>
+      </c>
+      <c r="K449" t="s">
+        <v>4033</v>
+      </c>
+      <c r="P449" t="s">
+        <v>4038</v>
+      </c>
+    </row>
+    <row r="450" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A450" t="s">
+        <v>4039</v>
+      </c>
+      <c r="B450" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C450" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D450" t="s">
+        <v>10</v>
+      </c>
+      <c r="E450" t="s">
+        <v>23</v>
+      </c>
+      <c r="K450" t="s">
+        <v>4033</v>
+      </c>
+      <c r="P450" t="s">
+        <v>4040</v>
+      </c>
+    </row>
+    <row r="451" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A451" t="s">
+        <v>4041</v>
+      </c>
+      <c r="B451" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C451" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D451" t="s">
+        <v>10</v>
+      </c>
+      <c r="E451" t="s">
+        <v>23</v>
+      </c>
+      <c r="K451" t="s">
+        <v>4033</v>
+      </c>
+      <c r="P451" t="s">
+        <v>4042</v>
+      </c>
+    </row>
+    <row r="452" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A452" t="s">
+        <v>4043</v>
+      </c>
+      <c r="B452" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C452" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D452" t="s">
+        <v>10</v>
+      </c>
+      <c r="E452" t="s">
+        <v>23</v>
+      </c>
+      <c r="K452" t="s">
+        <v>4044</v>
+      </c>
+      <c r="P452" t="s">
+        <v>4045</v>
+      </c>
+    </row>
+    <row r="453" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A453" t="s">
+        <v>4046</v>
+      </c>
+      <c r="B453" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C453" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D453" t="s">
+        <v>10</v>
+      </c>
+      <c r="E453" t="s">
+        <v>23</v>
+      </c>
+      <c r="K453" t="s">
+        <v>4044</v>
+      </c>
+      <c r="P453" t="s">
+        <v>4047</v>
+      </c>
+    </row>
+    <row r="454" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A454" t="s">
+        <v>4048</v>
+      </c>
+      <c r="B454" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C454" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D454" t="s">
+        <v>10</v>
+      </c>
+      <c r="E454" t="s">
+        <v>23</v>
+      </c>
+      <c r="K454" t="s">
+        <v>4044</v>
+      </c>
+      <c r="P454" t="s">
+        <v>4049</v>
+      </c>
+    </row>
+    <row r="455" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A455" t="s">
+        <v>4050</v>
+      </c>
+      <c r="B455" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C455" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D455" t="s">
+        <v>10</v>
+      </c>
+      <c r="E455" t="s">
+        <v>23</v>
+      </c>
+      <c r="K455" t="s">
+        <v>4044</v>
+      </c>
+      <c r="P455" t="s">
+        <v>4051</v>
+      </c>
+    </row>
+    <row r="456" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A456" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B456" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C456" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D456" t="s">
+        <v>10</v>
+      </c>
+      <c r="E456" t="s">
+        <v>23</v>
+      </c>
+      <c r="K456" t="s">
+        <v>4044</v>
+      </c>
+      <c r="P456" t="s">
+        <v>4055</v>
+      </c>
+    </row>
+    <row r="457" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A457" t="s">
+        <v>4056</v>
+      </c>
+      <c r="B457" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C457" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D457" t="s">
+        <v>10</v>
+      </c>
+      <c r="E457" t="s">
+        <v>23</v>
+      </c>
+      <c r="K457" t="s">
+        <v>4044</v>
+      </c>
+      <c r="P457" t="s">
+        <v>4057</v>
+      </c>
+    </row>
+    <row r="458" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A458" t="s">
+        <v>4058</v>
+      </c>
+      <c r="B458" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C458" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D458" t="s">
+        <v>10</v>
+      </c>
+      <c r="E458" t="s">
+        <v>23</v>
+      </c>
+      <c r="K458" t="s">
+        <v>4044</v>
+      </c>
+      <c r="P458" t="s">
+        <v>4059</v>
+      </c>
+    </row>
+    <row r="459" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A459" t="s">
+        <v>4060</v>
+      </c>
+      <c r="B459" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C459" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D459" t="s">
+        <v>10</v>
+      </c>
+      <c r="E459" t="s">
+        <v>23</v>
+      </c>
+      <c r="K459" t="s">
+        <v>4044</v>
+      </c>
+      <c r="P459" t="s">
+        <v>4061</v>
+      </c>
+    </row>
+    <row r="460" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A460" t="s">
+        <v>4062</v>
+      </c>
+      <c r="B460" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C460" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D460" t="s">
+        <v>10</v>
+      </c>
+      <c r="E460" t="s">
+        <v>23</v>
+      </c>
+      <c r="K460" t="s">
+        <v>4044</v>
+      </c>
+      <c r="P460" t="s">
+        <v>4063</v>
+      </c>
+    </row>
+    <row r="461" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A461" t="s">
+        <v>4064</v>
+      </c>
+      <c r="B461" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C461" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D461" t="s">
+        <v>10</v>
+      </c>
+      <c r="E461" t="s">
+        <v>23</v>
+      </c>
+      <c r="K461" t="s">
+        <v>4044</v>
+      </c>
+      <c r="P461" t="s">
+        <v>4065</v>
+      </c>
+    </row>
+    <row r="462" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A462" t="s">
+        <v>4066</v>
+      </c>
+      <c r="B462" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C462" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D462" t="s">
+        <v>10</v>
+      </c>
+      <c r="E462" t="s">
+        <v>23</v>
+      </c>
+      <c r="K462" t="s">
+        <v>4044</v>
+      </c>
+      <c r="P462" t="s">
+        <v>4067</v>
+      </c>
+    </row>
+    <row r="463" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A463" t="s">
+        <v>4068</v>
+      </c>
+      <c r="B463" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C463" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D463" t="s">
+        <v>10</v>
+      </c>
+      <c r="E463" t="s">
+        <v>23</v>
+      </c>
+      <c r="K463" t="s">
+        <v>396</v>
+      </c>
+      <c r="L463" t="s">
+        <v>4069</v>
+      </c>
+      <c r="P463" t="s">
+        <v>4070</v>
+      </c>
+    </row>
+    <row r="464" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A464" t="s">
+        <v>4071</v>
+      </c>
+      <c r="B464" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C464" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D464" t="s">
+        <v>10</v>
+      </c>
+      <c r="E464" t="s">
+        <v>23</v>
+      </c>
+      <c r="K464" t="s">
+        <v>396</v>
+      </c>
+      <c r="L464" t="s">
+        <v>4069</v>
+      </c>
+      <c r="P464" t="s">
+        <v>4072</v>
+      </c>
+    </row>
+    <row r="465" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A465" t="s">
+        <v>4073</v>
+      </c>
+      <c r="B465" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C465" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D465" t="s">
+        <v>10</v>
+      </c>
+      <c r="E465" t="s">
+        <v>23</v>
+      </c>
+      <c r="K465" t="s">
+        <v>371</v>
+      </c>
+      <c r="P465" t="s">
+        <v>4074</v>
+      </c>
+    </row>
+    <row r="466" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A466" t="s">
+        <v>4075</v>
+      </c>
+      <c r="B466" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C466" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D466" t="s">
+        <v>10</v>
+      </c>
+      <c r="E466" t="s">
+        <v>23</v>
+      </c>
+      <c r="K466" t="s">
+        <v>4033</v>
+      </c>
+      <c r="P466" t="s">
+        <v>4076</v>
+      </c>
+    </row>
+    <row r="467" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A467" t="s">
+        <v>4077</v>
+      </c>
+      <c r="B467" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C467" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D467" t="s">
+        <v>10</v>
+      </c>
+      <c r="E467" t="s">
+        <v>23</v>
+      </c>
+      <c r="K467" t="s">
+        <v>4033</v>
+      </c>
+      <c r="P467" t="s">
+        <v>4078</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -25024,14 +25559,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23" bestFit="1" customWidth="1"/>
   </cols>
@@ -25248,6 +25784,29 @@
         <v>1625</v>
       </c>
     </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4052</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" t="s">
+        <v>4044</v>
+      </c>
+      <c r="P11" t="s">
+        <v>4053</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -25255,10 +25814,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P252"/>
+  <dimension ref="A1:P228"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H125" sqref="H125"/>
+      <selection activeCell="G163" sqref="G163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28289,565 +28848,487 @@
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>4027</v>
+        <v>2564</v>
       </c>
       <c r="B145" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D145" t="s">
-        <v>10</v>
-      </c>
-      <c r="E145" t="s">
         <v>23</v>
       </c>
       <c r="K145" t="s">
-        <v>371</v>
+        <v>11</v>
       </c>
       <c r="P145" t="s">
-        <v>4029</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>4030</v>
+        <v>2567</v>
       </c>
       <c r="B146" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D146" t="s">
-        <v>10</v>
-      </c>
-      <c r="E146" t="s">
         <v>23</v>
       </c>
       <c r="K146" t="s">
-        <v>371</v>
+        <v>11</v>
       </c>
       <c r="P146" t="s">
-        <v>4031</v>
+        <v>2568</v>
       </c>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>4032</v>
+        <v>2569</v>
       </c>
       <c r="B147" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D147" t="s">
-        <v>10</v>
-      </c>
-      <c r="E147" t="s">
         <v>23</v>
       </c>
       <c r="K147" t="s">
-        <v>4033</v>
+        <v>11</v>
       </c>
       <c r="P147" t="s">
-        <v>4034</v>
+        <v>2570</v>
       </c>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>4035</v>
+        <v>2571</v>
       </c>
       <c r="B148" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D148" t="s">
-        <v>10</v>
-      </c>
-      <c r="E148" t="s">
         <v>23</v>
       </c>
       <c r="K148" t="s">
-        <v>4033</v>
+        <v>11</v>
       </c>
       <c r="P148" t="s">
-        <v>4036</v>
+        <v>2572</v>
       </c>
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>4037</v>
+        <v>2573</v>
       </c>
       <c r="B149" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D149" t="s">
-        <v>10</v>
-      </c>
-      <c r="E149" t="s">
         <v>23</v>
       </c>
       <c r="K149" t="s">
-        <v>4033</v>
+        <v>11</v>
       </c>
       <c r="P149" t="s">
-        <v>4038</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>4039</v>
+        <v>2575</v>
       </c>
       <c r="B150" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D150" t="s">
-        <v>10</v>
-      </c>
-      <c r="E150" t="s">
         <v>23</v>
       </c>
       <c r="K150" t="s">
-        <v>4033</v>
+        <v>11</v>
       </c>
       <c r="P150" t="s">
-        <v>4040</v>
+        <v>2576</v>
       </c>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>4041</v>
+        <v>2577</v>
       </c>
       <c r="B151" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D151" t="s">
-        <v>10</v>
-      </c>
-      <c r="E151" t="s">
         <v>23</v>
       </c>
       <c r="K151" t="s">
-        <v>4033</v>
+        <v>11</v>
       </c>
       <c r="P151" t="s">
-        <v>4042</v>
+        <v>2578</v>
       </c>
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>4043</v>
+        <v>2579</v>
       </c>
       <c r="B152" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D152" t="s">
-        <v>10</v>
-      </c>
-      <c r="E152" t="s">
         <v>23</v>
       </c>
       <c r="K152" t="s">
-        <v>4044</v>
+        <v>11</v>
       </c>
       <c r="P152" t="s">
-        <v>4045</v>
+        <v>2580</v>
       </c>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>4046</v>
+        <v>2581</v>
       </c>
       <c r="B153" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D153" t="s">
-        <v>10</v>
-      </c>
-      <c r="E153" t="s">
         <v>23</v>
       </c>
       <c r="K153" t="s">
-        <v>4044</v>
+        <v>11</v>
       </c>
       <c r="P153" t="s">
-        <v>4047</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>4048</v>
+        <v>2583</v>
       </c>
       <c r="B154" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D154" t="s">
-        <v>10</v>
-      </c>
-      <c r="E154" t="s">
         <v>23</v>
       </c>
       <c r="K154" t="s">
-        <v>4044</v>
+        <v>11</v>
       </c>
       <c r="P154" t="s">
-        <v>4049</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>4050</v>
+        <v>2585</v>
       </c>
       <c r="B155" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D155" t="s">
-        <v>10</v>
-      </c>
-      <c r="E155" t="s">
         <v>23</v>
       </c>
       <c r="K155" t="s">
-        <v>4044</v>
+        <v>11</v>
       </c>
       <c r="P155" t="s">
-        <v>4051</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>4052</v>
+        <v>2587</v>
       </c>
       <c r="B156" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D156" t="s">
-        <v>10</v>
-      </c>
-      <c r="E156" t="s">
         <v>23</v>
       </c>
       <c r="K156" t="s">
-        <v>4044</v>
+        <v>11</v>
       </c>
       <c r="P156" t="s">
-        <v>4053</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>4054</v>
+        <v>2589</v>
       </c>
       <c r="B157" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D157" t="s">
-        <v>10</v>
-      </c>
-      <c r="E157" t="s">
         <v>23</v>
       </c>
       <c r="K157" t="s">
-        <v>4044</v>
+        <v>11</v>
       </c>
       <c r="P157" t="s">
-        <v>4055</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>4056</v>
+        <v>2591</v>
       </c>
       <c r="B158" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D158" t="s">
-        <v>10</v>
-      </c>
-      <c r="E158" t="s">
         <v>23</v>
       </c>
       <c r="K158" t="s">
-        <v>4044</v>
+        <v>11</v>
       </c>
       <c r="P158" t="s">
-        <v>4057</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>4058</v>
+        <v>2593</v>
       </c>
       <c r="B159" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D159" t="s">
-        <v>10</v>
-      </c>
-      <c r="E159" t="s">
         <v>23</v>
       </c>
       <c r="K159" t="s">
-        <v>4044</v>
+        <v>11</v>
       </c>
       <c r="P159" t="s">
-        <v>4059</v>
+        <v>2594</v>
       </c>
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>4060</v>
+        <v>2595</v>
       </c>
       <c r="B160" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D160" t="s">
-        <v>10</v>
-      </c>
-      <c r="E160" t="s">
         <v>23</v>
       </c>
       <c r="K160" t="s">
-        <v>4044</v>
+        <v>11</v>
       </c>
       <c r="P160" t="s">
-        <v>4061</v>
+        <v>2596</v>
       </c>
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>4062</v>
+        <v>2597</v>
       </c>
       <c r="B161" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D161" t="s">
-        <v>10</v>
-      </c>
-      <c r="E161" t="s">
         <v>23</v>
       </c>
       <c r="K161" t="s">
-        <v>4044</v>
+        <v>11</v>
       </c>
       <c r="P161" t="s">
-        <v>4063</v>
+        <v>2598</v>
       </c>
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>4064</v>
+        <v>2599</v>
       </c>
       <c r="B162" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D162" t="s">
-        <v>10</v>
-      </c>
-      <c r="E162" t="s">
         <v>23</v>
       </c>
       <c r="K162" t="s">
-        <v>4044</v>
+        <v>11</v>
       </c>
       <c r="P162" t="s">
-        <v>4065</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>4066</v>
+        <v>2601</v>
       </c>
       <c r="B163" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D163" t="s">
-        <v>10</v>
-      </c>
-      <c r="E163" t="s">
         <v>23</v>
       </c>
       <c r="K163" t="s">
-        <v>4044</v>
+        <v>11</v>
       </c>
       <c r="P163" t="s">
-        <v>4067</v>
+        <v>2602</v>
       </c>
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>4068</v>
+        <v>2603</v>
       </c>
       <c r="B164" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D164" t="s">
-        <v>10</v>
-      </c>
-      <c r="E164" t="s">
         <v>23</v>
       </c>
       <c r="K164" t="s">
-        <v>396</v>
-      </c>
-      <c r="L164" t="s">
-        <v>4069</v>
+        <v>11</v>
       </c>
       <c r="P164" t="s">
-        <v>4070</v>
+        <v>2604</v>
       </c>
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>4071</v>
+        <v>2605</v>
       </c>
       <c r="B165" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D165" t="s">
-        <v>10</v>
-      </c>
-      <c r="E165" t="s">
         <v>23</v>
       </c>
       <c r="K165" t="s">
-        <v>396</v>
-      </c>
-      <c r="L165" t="s">
-        <v>4069</v>
+        <v>11</v>
       </c>
       <c r="P165" t="s">
-        <v>4072</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>4073</v>
+        <v>2607</v>
       </c>
       <c r="B166" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D166" t="s">
-        <v>10</v>
-      </c>
-      <c r="E166" t="s">
         <v>23</v>
       </c>
       <c r="K166" t="s">
-        <v>371</v>
+        <v>11</v>
       </c>
       <c r="P166" t="s">
-        <v>4074</v>
+        <v>2608</v>
       </c>
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>4075</v>
+        <v>2609</v>
       </c>
       <c r="B167" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D167" t="s">
-        <v>10</v>
-      </c>
-      <c r="E167" t="s">
         <v>23</v>
       </c>
       <c r="K167" t="s">
-        <v>4033</v>
+        <v>11</v>
       </c>
       <c r="P167" t="s">
-        <v>4076</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>4077</v>
+        <v>2611</v>
       </c>
       <c r="B168" t="s">
-        <v>4028</v>
+        <v>2565</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D168" t="s">
-        <v>10</v>
-      </c>
-      <c r="E168" t="s">
         <v>23</v>
       </c>
       <c r="K168" t="s">
-        <v>4033</v>
+        <v>11</v>
       </c>
       <c r="P168" t="s">
-        <v>4078</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>2564</v>
+        <v>2613</v>
       </c>
       <c r="B169" t="s">
         <v>2565</v>
@@ -28862,12 +29343,12 @@
         <v>11</v>
       </c>
       <c r="P169" t="s">
-        <v>2566</v>
+        <v>2614</v>
       </c>
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>2567</v>
+        <v>2615</v>
       </c>
       <c r="B170" t="s">
         <v>2565</v>
@@ -28882,12 +29363,12 @@
         <v>11</v>
       </c>
       <c r="P170" t="s">
-        <v>2568</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>2569</v>
+        <v>2617</v>
       </c>
       <c r="B171" t="s">
         <v>2565</v>
@@ -28902,12 +29383,12 @@
         <v>11</v>
       </c>
       <c r="P171" t="s">
-        <v>2570</v>
+        <v>2618</v>
       </c>
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>2571</v>
+        <v>2619</v>
       </c>
       <c r="B172" t="s">
         <v>2565</v>
@@ -28922,12 +29403,12 @@
         <v>11</v>
       </c>
       <c r="P172" t="s">
-        <v>2572</v>
+        <v>2620</v>
       </c>
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>2573</v>
+        <v>2621</v>
       </c>
       <c r="B173" t="s">
         <v>2565</v>
@@ -28942,12 +29423,12 @@
         <v>11</v>
       </c>
       <c r="P173" t="s">
-        <v>2574</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>2575</v>
+        <v>2623</v>
       </c>
       <c r="B174" t="s">
         <v>2565</v>
@@ -28962,12 +29443,12 @@
         <v>11</v>
       </c>
       <c r="P174" t="s">
-        <v>2576</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>2577</v>
+        <v>2625</v>
       </c>
       <c r="B175" t="s">
         <v>2565</v>
@@ -28982,12 +29463,12 @@
         <v>11</v>
       </c>
       <c r="P175" t="s">
-        <v>2578</v>
+        <v>2626</v>
       </c>
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>2579</v>
+        <v>2627</v>
       </c>
       <c r="B176" t="s">
         <v>2565</v>
@@ -29002,12 +29483,12 @@
         <v>11</v>
       </c>
       <c r="P176" t="s">
-        <v>2580</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>2581</v>
+        <v>2629</v>
       </c>
       <c r="B177" t="s">
         <v>2565</v>
@@ -29022,12 +29503,12 @@
         <v>11</v>
       </c>
       <c r="P177" t="s">
-        <v>2582</v>
+        <v>2630</v>
       </c>
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>2583</v>
+        <v>2631</v>
       </c>
       <c r="B178" t="s">
         <v>2565</v>
@@ -29042,12 +29523,12 @@
         <v>11</v>
       </c>
       <c r="P178" t="s">
-        <v>2584</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>2585</v>
+        <v>2633</v>
       </c>
       <c r="B179" t="s">
         <v>2565</v>
@@ -29062,12 +29543,12 @@
         <v>11</v>
       </c>
       <c r="P179" t="s">
-        <v>2586</v>
+        <v>2634</v>
       </c>
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>2587</v>
+        <v>2635</v>
       </c>
       <c r="B180" t="s">
         <v>2565</v>
@@ -29082,12 +29563,12 @@
         <v>11</v>
       </c>
       <c r="P180" t="s">
-        <v>2588</v>
+        <v>2636</v>
       </c>
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>2589</v>
+        <v>2637</v>
       </c>
       <c r="B181" t="s">
         <v>2565</v>
@@ -29102,12 +29583,12 @@
         <v>11</v>
       </c>
       <c r="P181" t="s">
-        <v>2590</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>2591</v>
+        <v>2639</v>
       </c>
       <c r="B182" t="s">
         <v>2565</v>
@@ -29122,12 +29603,12 @@
         <v>11</v>
       </c>
       <c r="P182" t="s">
-        <v>2592</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>2593</v>
+        <v>2641</v>
       </c>
       <c r="B183" t="s">
         <v>2565</v>
@@ -29142,12 +29623,12 @@
         <v>11</v>
       </c>
       <c r="P183" t="s">
-        <v>2594</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>2595</v>
+        <v>2643</v>
       </c>
       <c r="B184" t="s">
         <v>2565</v>
@@ -29162,12 +29643,12 @@
         <v>11</v>
       </c>
       <c r="P184" t="s">
-        <v>2596</v>
+        <v>2644</v>
       </c>
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>2597</v>
+        <v>2645</v>
       </c>
       <c r="B185" t="s">
         <v>2565</v>
@@ -29182,12 +29663,12 @@
         <v>11</v>
       </c>
       <c r="P185" t="s">
-        <v>2598</v>
+        <v>2646</v>
       </c>
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>2599</v>
+        <v>2647</v>
       </c>
       <c r="B186" t="s">
         <v>2565</v>
@@ -29202,12 +29683,12 @@
         <v>11</v>
       </c>
       <c r="P186" t="s">
-        <v>2600</v>
+        <v>2648</v>
       </c>
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>2601</v>
+        <v>2649</v>
       </c>
       <c r="B187" t="s">
         <v>2565</v>
@@ -29222,12 +29703,12 @@
         <v>11</v>
       </c>
       <c r="P187" t="s">
-        <v>2602</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>2603</v>
+        <v>2651</v>
       </c>
       <c r="B188" t="s">
         <v>2565</v>
@@ -29242,12 +29723,12 @@
         <v>11</v>
       </c>
       <c r="P188" t="s">
-        <v>2604</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>2605</v>
+        <v>2653</v>
       </c>
       <c r="B189" t="s">
         <v>2565</v>
@@ -29262,12 +29743,12 @@
         <v>11</v>
       </c>
       <c r="P189" t="s">
-        <v>2606</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>2607</v>
+        <v>2655</v>
       </c>
       <c r="B190" t="s">
         <v>2565</v>
@@ -29282,12 +29763,12 @@
         <v>11</v>
       </c>
       <c r="P190" t="s">
-        <v>2608</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>2609</v>
+        <v>2657</v>
       </c>
       <c r="B191" t="s">
         <v>2565</v>
@@ -29302,12 +29783,12 @@
         <v>11</v>
       </c>
       <c r="P191" t="s">
-        <v>2610</v>
+        <v>2658</v>
       </c>
     </row>
     <row r="192" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>2611</v>
+        <v>2659</v>
       </c>
       <c r="B192" t="s">
         <v>2565</v>
@@ -29322,12 +29803,12 @@
         <v>11</v>
       </c>
       <c r="P192" t="s">
-        <v>2612</v>
+        <v>2660</v>
       </c>
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>2613</v>
+        <v>2661</v>
       </c>
       <c r="B193" t="s">
         <v>2565</v>
@@ -29342,75 +29823,93 @@
         <v>11</v>
       </c>
       <c r="P193" t="s">
-        <v>2614</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>2615</v>
+        <v>3117</v>
       </c>
       <c r="B194" t="s">
-        <v>2565</v>
+        <v>3118</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D194" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E194" t="s">
+        <v>10</v>
       </c>
       <c r="K194" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="L194" t="s">
+        <v>1542</v>
       </c>
       <c r="P194" t="s">
-        <v>2616</v>
+        <v>3119</v>
       </c>
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>2617</v>
+        <v>3120</v>
       </c>
       <c r="B195" t="s">
-        <v>2565</v>
+        <v>3118</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D195" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E195" t="s">
+        <v>10</v>
       </c>
       <c r="K195" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="L195" t="s">
+        <v>1542</v>
       </c>
       <c r="P195" t="s">
-        <v>2618</v>
+        <v>3121</v>
       </c>
     </row>
     <row r="196" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>2619</v>
+        <v>3122</v>
       </c>
       <c r="B196" t="s">
-        <v>2565</v>
+        <v>3118</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D196" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E196" t="s">
+        <v>10</v>
       </c>
       <c r="K196" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="L196" t="s">
+        <v>1542</v>
       </c>
       <c r="P196" t="s">
-        <v>2620</v>
+        <v>3123</v>
       </c>
     </row>
     <row r="197" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>2621</v>
+        <v>1554</v>
       </c>
       <c r="B197" t="s">
-        <v>2565</v>
+        <v>1555</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>10</v>
@@ -29418,19 +29917,25 @@
       <c r="D197" t="s">
         <v>23</v>
       </c>
+      <c r="E197" t="s">
+        <v>23</v>
+      </c>
       <c r="K197" t="s">
-        <v>11</v>
+        <v>105</v>
+      </c>
+      <c r="L197" t="s">
+        <v>372</v>
       </c>
       <c r="P197" t="s">
-        <v>2622</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="198" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>2623</v>
+        <v>1557</v>
       </c>
       <c r="B198" t="s">
-        <v>2565</v>
+        <v>1555</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>10</v>
@@ -29438,19 +29943,25 @@
       <c r="D198" t="s">
         <v>23</v>
       </c>
+      <c r="E198" t="s">
+        <v>23</v>
+      </c>
       <c r="K198" t="s">
-        <v>11</v>
+        <v>105</v>
+      </c>
+      <c r="L198" t="s">
+        <v>372</v>
       </c>
       <c r="P198" t="s">
-        <v>2624</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="199" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>2625</v>
+        <v>1559</v>
       </c>
       <c r="B199" t="s">
-        <v>2565</v>
+        <v>1555</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>10</v>
@@ -29458,19 +29969,25 @@
       <c r="D199" t="s">
         <v>23</v>
       </c>
+      <c r="E199" t="s">
+        <v>23</v>
+      </c>
       <c r="K199" t="s">
-        <v>11</v>
+        <v>105</v>
+      </c>
+      <c r="L199" t="s">
+        <v>372</v>
       </c>
       <c r="P199" t="s">
-        <v>2626</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="200" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>2627</v>
+        <v>1561</v>
       </c>
       <c r="B200" t="s">
-        <v>2565</v>
+        <v>1555</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>10</v>
@@ -29478,59 +29995,65 @@
       <c r="D200" t="s">
         <v>23</v>
       </c>
+      <c r="E200" t="s">
+        <v>23</v>
+      </c>
       <c r="K200" t="s">
-        <v>11</v>
+        <v>105</v>
+      </c>
+      <c r="L200" t="s">
+        <v>372</v>
       </c>
       <c r="P200" t="s">
-        <v>2628</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>2629</v>
+        <v>4693</v>
       </c>
       <c r="B201" t="s">
-        <v>2565</v>
+        <v>4694</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D201" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="K201" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="P201" t="s">
-        <v>2630</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>2631</v>
+        <v>4696</v>
       </c>
       <c r="B202" t="s">
-        <v>2565</v>
+        <v>4694</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D202" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="K202" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="P202" t="s">
-        <v>2632</v>
+        <v>4697</v>
       </c>
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>2633</v>
+        <v>2039</v>
       </c>
       <c r="B203" t="s">
-        <v>2565</v>
+        <v>2040</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>10</v>
@@ -29539,18 +30062,18 @@
         <v>23</v>
       </c>
       <c r="K203" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="P203" t="s">
-        <v>2634</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>2635</v>
+        <v>2042</v>
       </c>
       <c r="B204" t="s">
-        <v>2565</v>
+        <v>2040</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>10</v>
@@ -29559,18 +30082,18 @@
         <v>23</v>
       </c>
       <c r="K204" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="P204" t="s">
-        <v>2636</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>2637</v>
+        <v>2044</v>
       </c>
       <c r="B205" t="s">
-        <v>2565</v>
+        <v>2040</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>10</v>
@@ -29579,18 +30102,18 @@
         <v>23</v>
       </c>
       <c r="K205" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="P205" t="s">
-        <v>2638</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>2639</v>
+        <v>1161</v>
       </c>
       <c r="B206" t="s">
-        <v>2565</v>
+        <v>1162</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>10</v>
@@ -29599,18 +30122,18 @@
         <v>23</v>
       </c>
       <c r="K206" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="P206" t="s">
-        <v>2640</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="207" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>2641</v>
+        <v>1164</v>
       </c>
       <c r="B207" t="s">
-        <v>2565</v>
+        <v>1162</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>10</v>
@@ -29619,18 +30142,18 @@
         <v>23</v>
       </c>
       <c r="K207" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="P207" t="s">
-        <v>2642</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="208" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>2643</v>
+        <v>1166</v>
       </c>
       <c r="B208" t="s">
-        <v>2565</v>
+        <v>1162</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>10</v>
@@ -29639,18 +30162,18 @@
         <v>23</v>
       </c>
       <c r="K208" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="P208" t="s">
-        <v>2644</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="209" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>2645</v>
+        <v>1168</v>
       </c>
       <c r="B209" t="s">
-        <v>2565</v>
+        <v>1162</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>10</v>
@@ -29659,18 +30182,18 @@
         <v>23</v>
       </c>
       <c r="K209" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="P209" t="s">
-        <v>2646</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="210" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>2647</v>
+        <v>1170</v>
       </c>
       <c r="B210" t="s">
-        <v>2565</v>
+        <v>1162</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>10</v>
@@ -29679,18 +30202,18 @@
         <v>23</v>
       </c>
       <c r="K210" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="P210" t="s">
-        <v>2648</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="211" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>2649</v>
+        <v>1172</v>
       </c>
       <c r="B211" t="s">
-        <v>2565</v>
+        <v>1162</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>10</v>
@@ -29698,19 +30221,25 @@
       <c r="D211" t="s">
         <v>23</v>
       </c>
+      <c r="E211" t="s">
+        <v>1173</v>
+      </c>
       <c r="K211" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="L211" t="s">
+        <v>1174</v>
       </c>
       <c r="P211" t="s">
-        <v>2650</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="212" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>2651</v>
+        <v>1176</v>
       </c>
       <c r="B212" t="s">
-        <v>2565</v>
+        <v>1162</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>10</v>
@@ -29718,223 +30247,211 @@
       <c r="D212" t="s">
         <v>23</v>
       </c>
+      <c r="E212" t="s">
+        <v>1173</v>
+      </c>
       <c r="K212" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="L212" t="s">
+        <v>1174</v>
       </c>
       <c r="P212" t="s">
-        <v>2652</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="213" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>2653</v>
+        <v>1178</v>
       </c>
       <c r="B213" t="s">
-        <v>2565</v>
+        <v>1162</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D213" t="s">
-        <v>23</v>
+        <v>579</v>
       </c>
       <c r="K213" t="s">
-        <v>11</v>
+        <v>200</v>
       </c>
       <c r="P213" t="s">
-        <v>2654</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="214" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>2655</v>
+        <v>1180</v>
       </c>
       <c r="B214" t="s">
-        <v>2565</v>
+        <v>1162</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D214" t="s">
-        <v>23</v>
+        <v>579</v>
       </c>
       <c r="K214" t="s">
-        <v>11</v>
+        <v>200</v>
       </c>
       <c r="P214" t="s">
-        <v>2656</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="215" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>2657</v>
+        <v>1182</v>
       </c>
       <c r="B215" t="s">
-        <v>2565</v>
+        <v>1162</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D215" t="s">
-        <v>23</v>
+        <v>579</v>
       </c>
       <c r="K215" t="s">
-        <v>11</v>
+        <v>200</v>
       </c>
       <c r="P215" t="s">
-        <v>2658</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="216" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>2659</v>
+        <v>1184</v>
       </c>
       <c r="B216" t="s">
-        <v>2565</v>
+        <v>1162</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D216" t="s">
-        <v>23</v>
+        <v>1185</v>
       </c>
       <c r="K216" t="s">
-        <v>11</v>
+        <v>200</v>
       </c>
       <c r="P216" t="s">
-        <v>2660</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="217" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>2661</v>
+        <v>1187</v>
       </c>
       <c r="B217" t="s">
-        <v>2565</v>
+        <v>1162</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D217" t="s">
-        <v>23</v>
+        <v>1185</v>
       </c>
       <c r="K217" t="s">
-        <v>11</v>
+        <v>200</v>
       </c>
       <c r="P217" t="s">
-        <v>2662</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="218" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>3117</v>
+        <v>1189</v>
       </c>
       <c r="B218" t="s">
-        <v>3118</v>
+        <v>1162</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D218" t="s">
-        <v>10</v>
-      </c>
-      <c r="E218" t="s">
-        <v>10</v>
+        <v>1185</v>
       </c>
       <c r="K218" t="s">
-        <v>24</v>
-      </c>
-      <c r="L218" t="s">
-        <v>1542</v>
+        <v>200</v>
       </c>
       <c r="P218" t="s">
-        <v>3119</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="219" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>3120</v>
+        <v>1191</v>
       </c>
       <c r="B219" t="s">
-        <v>3118</v>
+        <v>1162</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D219" t="s">
-        <v>10</v>
-      </c>
-      <c r="E219" t="s">
-        <v>10</v>
+        <v>579</v>
       </c>
       <c r="K219" t="s">
-        <v>24</v>
-      </c>
-      <c r="L219" t="s">
-        <v>1542</v>
+        <v>200</v>
       </c>
       <c r="P219" t="s">
-        <v>3121</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="220" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>3122</v>
+        <v>1193</v>
       </c>
       <c r="B220" t="s">
-        <v>3118</v>
+        <v>1162</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D220" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E220" t="s">
-        <v>10</v>
+        <v>1185</v>
       </c>
       <c r="K220" t="s">
         <v>24</v>
       </c>
       <c r="L220" t="s">
-        <v>1542</v>
+        <v>200</v>
       </c>
       <c r="P220" t="s">
-        <v>3123</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="221" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>1554</v>
+        <v>1195</v>
       </c>
       <c r="B221" t="s">
-        <v>1555</v>
+        <v>1162</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D221" t="s">
-        <v>23</v>
-      </c>
-      <c r="E221" t="s">
-        <v>23</v>
+        <v>1185</v>
       </c>
       <c r="K221" t="s">
-        <v>105</v>
-      </c>
-      <c r="L221" t="s">
-        <v>372</v>
+        <v>200</v>
       </c>
       <c r="P221" t="s">
-        <v>1556</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="222" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>1557</v>
+        <v>1197</v>
       </c>
       <c r="B222" t="s">
-        <v>1555</v>
+        <v>1162</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>10</v>
@@ -29942,628 +30459,112 @@
       <c r="D222" t="s">
         <v>23</v>
       </c>
-      <c r="E222" t="s">
-        <v>23</v>
-      </c>
       <c r="K222" t="s">
-        <v>105</v>
-      </c>
-      <c r="L222" t="s">
-        <v>372</v>
+        <v>24</v>
       </c>
       <c r="P222" t="s">
-        <v>1558</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="223" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>1559</v>
+        <v>4846</v>
       </c>
       <c r="B223" t="s">
-        <v>1555</v>
+        <v>4847</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D223" t="s">
-        <v>23</v>
-      </c>
-      <c r="E223" t="s">
-        <v>23</v>
-      </c>
       <c r="K223" t="s">
-        <v>105</v>
-      </c>
-      <c r="L223" t="s">
-        <v>372</v>
+        <v>24</v>
       </c>
       <c r="P223" t="s">
-        <v>1560</v>
+        <v>4848</v>
       </c>
     </row>
     <row r="224" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>1561</v>
+        <v>4849</v>
       </c>
       <c r="B224" t="s">
-        <v>1555</v>
+        <v>4847</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D224" t="s">
-        <v>23</v>
-      </c>
-      <c r="E224" t="s">
-        <v>23</v>
-      </c>
       <c r="K224" t="s">
-        <v>105</v>
-      </c>
-      <c r="L224" t="s">
-        <v>372</v>
+        <v>24</v>
       </c>
       <c r="P224" t="s">
-        <v>1562</v>
+        <v>4850</v>
       </c>
     </row>
     <row r="225" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>4693</v>
+        <v>848</v>
       </c>
       <c r="B225" t="s">
-        <v>4694</v>
+        <v>849</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D225" t="s">
         <v>10</v>
       </c>
       <c r="K225" t="s">
         <v>105</v>
       </c>
       <c r="P225" t="s">
-        <v>4695</v>
+        <v>850</v>
       </c>
     </row>
     <row r="226" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>4696</v>
+        <v>851</v>
       </c>
       <c r="B226" t="s">
-        <v>4694</v>
+        <v>849</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D226" t="s">
         <v>10</v>
       </c>
       <c r="K226" t="s">
         <v>105</v>
       </c>
       <c r="P226" t="s">
-        <v>4697</v>
+        <v>852</v>
       </c>
     </row>
     <row r="227" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>2039</v>
+        <v>853</v>
       </c>
       <c r="B227" t="s">
-        <v>2040</v>
+        <v>849</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D227" t="s">
-        <v>23</v>
-      </c>
       <c r="K227" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="P227" t="s">
-        <v>2041</v>
+        <v>854</v>
       </c>
     </row>
     <row r="228" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>2042</v>
+        <v>855</v>
       </c>
       <c r="B228" t="s">
-        <v>2040</v>
+        <v>849</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D228" t="s">
-        <v>23</v>
-      </c>
       <c r="K228" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="P228" t="s">
-        <v>2043</v>
-      </c>
-    </row>
-    <row r="229" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A229" t="s">
-        <v>2044</v>
-      </c>
-      <c r="B229" t="s">
-        <v>2040</v>
-      </c>
-      <c r="C229" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D229" t="s">
-        <v>23</v>
-      </c>
-      <c r="K229" t="s">
-        <v>24</v>
-      </c>
-      <c r="P229" t="s">
-        <v>2045</v>
-      </c>
-    </row>
-    <row r="230" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A230" t="s">
-        <v>1161</v>
-      </c>
-      <c r="B230" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C230" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D230" t="s">
-        <v>23</v>
-      </c>
-      <c r="K230" t="s">
-        <v>24</v>
-      </c>
-      <c r="P230" t="s">
-        <v>1163</v>
-      </c>
-    </row>
-    <row r="231" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A231" t="s">
-        <v>1164</v>
-      </c>
-      <c r="B231" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C231" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D231" t="s">
-        <v>23</v>
-      </c>
-      <c r="K231" t="s">
-        <v>24</v>
-      </c>
-      <c r="P231" t="s">
-        <v>1165</v>
-      </c>
-    </row>
-    <row r="232" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A232" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B232" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C232" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D232" t="s">
-        <v>23</v>
-      </c>
-      <c r="K232" t="s">
-        <v>24</v>
-      </c>
-      <c r="P232" t="s">
-        <v>1167</v>
-      </c>
-    </row>
-    <row r="233" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A233" t="s">
-        <v>1168</v>
-      </c>
-      <c r="B233" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C233" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D233" t="s">
-        <v>23</v>
-      </c>
-      <c r="K233" t="s">
-        <v>24</v>
-      </c>
-      <c r="P233" t="s">
-        <v>1169</v>
-      </c>
-    </row>
-    <row r="234" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A234" t="s">
-        <v>1170</v>
-      </c>
-      <c r="B234" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C234" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D234" t="s">
-        <v>23</v>
-      </c>
-      <c r="K234" t="s">
-        <v>24</v>
-      </c>
-      <c r="P234" t="s">
-        <v>1171</v>
-      </c>
-    </row>
-    <row r="235" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A235" t="s">
-        <v>1172</v>
-      </c>
-      <c r="B235" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C235" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D235" t="s">
-        <v>23</v>
-      </c>
-      <c r="E235" t="s">
-        <v>1173</v>
-      </c>
-      <c r="K235" t="s">
-        <v>24</v>
-      </c>
-      <c r="L235" t="s">
-        <v>1174</v>
-      </c>
-      <c r="P235" t="s">
-        <v>1175</v>
-      </c>
-    </row>
-    <row r="236" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A236" t="s">
-        <v>1176</v>
-      </c>
-      <c r="B236" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C236" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D236" t="s">
-        <v>23</v>
-      </c>
-      <c r="E236" t="s">
-        <v>1173</v>
-      </c>
-      <c r="K236" t="s">
-        <v>24</v>
-      </c>
-      <c r="L236" t="s">
-        <v>1174</v>
-      </c>
-      <c r="P236" t="s">
-        <v>1177</v>
-      </c>
-    </row>
-    <row r="237" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A237" t="s">
-        <v>1178</v>
-      </c>
-      <c r="B237" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C237" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D237" t="s">
-        <v>579</v>
-      </c>
-      <c r="K237" t="s">
-        <v>200</v>
-      </c>
-      <c r="P237" t="s">
-        <v>1179</v>
-      </c>
-    </row>
-    <row r="238" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A238" t="s">
-        <v>1180</v>
-      </c>
-      <c r="B238" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C238" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D238" t="s">
-        <v>579</v>
-      </c>
-      <c r="K238" t="s">
-        <v>200</v>
-      </c>
-      <c r="P238" t="s">
-        <v>1181</v>
-      </c>
-    </row>
-    <row r="239" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A239" t="s">
-        <v>1182</v>
-      </c>
-      <c r="B239" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C239" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D239" t="s">
-        <v>579</v>
-      </c>
-      <c r="K239" t="s">
-        <v>200</v>
-      </c>
-      <c r="P239" t="s">
-        <v>1183</v>
-      </c>
-    </row>
-    <row r="240" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A240" t="s">
-        <v>1184</v>
-      </c>
-      <c r="B240" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C240" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D240" t="s">
-        <v>1185</v>
-      </c>
-      <c r="K240" t="s">
-        <v>200</v>
-      </c>
-      <c r="P240" t="s">
-        <v>1186</v>
-      </c>
-    </row>
-    <row r="241" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A241" t="s">
-        <v>1187</v>
-      </c>
-      <c r="B241" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C241" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D241" t="s">
-        <v>1185</v>
-      </c>
-      <c r="K241" t="s">
-        <v>200</v>
-      </c>
-      <c r="P241" t="s">
-        <v>1188</v>
-      </c>
-    </row>
-    <row r="242" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A242" t="s">
-        <v>1189</v>
-      </c>
-      <c r="B242" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C242" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D242" t="s">
-        <v>1185</v>
-      </c>
-      <c r="K242" t="s">
-        <v>200</v>
-      </c>
-      <c r="P242" t="s">
-        <v>1190</v>
-      </c>
-    </row>
-    <row r="243" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A243" t="s">
-        <v>1191</v>
-      </c>
-      <c r="B243" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C243" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D243" t="s">
-        <v>579</v>
-      </c>
-      <c r="K243" t="s">
-        <v>200</v>
-      </c>
-      <c r="P243" t="s">
-        <v>1192</v>
-      </c>
-    </row>
-    <row r="244" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A244" t="s">
-        <v>1193</v>
-      </c>
-      <c r="B244" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C244" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D244" t="s">
-        <v>23</v>
-      </c>
-      <c r="E244" t="s">
-        <v>1185</v>
-      </c>
-      <c r="K244" t="s">
-        <v>24</v>
-      </c>
-      <c r="L244" t="s">
-        <v>200</v>
-      </c>
-      <c r="P244" t="s">
-        <v>1194</v>
-      </c>
-    </row>
-    <row r="245" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A245" t="s">
-        <v>1195</v>
-      </c>
-      <c r="B245" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C245" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D245" t="s">
-        <v>1185</v>
-      </c>
-      <c r="K245" t="s">
-        <v>200</v>
-      </c>
-      <c r="P245" t="s">
-        <v>1196</v>
-      </c>
-    </row>
-    <row r="246" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A246" t="s">
-        <v>1197</v>
-      </c>
-      <c r="B246" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C246" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D246" t="s">
-        <v>23</v>
-      </c>
-      <c r="K246" t="s">
-        <v>24</v>
-      </c>
-      <c r="P246" t="s">
-        <v>1198</v>
-      </c>
-    </row>
-    <row r="247" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A247" t="s">
-        <v>4846</v>
-      </c>
-      <c r="B247" t="s">
-        <v>4847</v>
-      </c>
-      <c r="C247" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K247" t="s">
-        <v>24</v>
-      </c>
-      <c r="P247" t="s">
-        <v>4848</v>
-      </c>
-    </row>
-    <row r="248" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A248" t="s">
-        <v>4849</v>
-      </c>
-      <c r="B248" t="s">
-        <v>4847</v>
-      </c>
-      <c r="C248" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K248" t="s">
-        <v>24</v>
-      </c>
-      <c r="P248" t="s">
-        <v>4850</v>
-      </c>
-    </row>
-    <row r="249" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A249" t="s">
-        <v>848</v>
-      </c>
-      <c r="B249" t="s">
-        <v>849</v>
-      </c>
-      <c r="C249" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K249" t="s">
-        <v>105</v>
-      </c>
-      <c r="P249" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="250" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A250" t="s">
-        <v>851</v>
-      </c>
-      <c r="B250" t="s">
-        <v>849</v>
-      </c>
-      <c r="C250" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K250" t="s">
-        <v>105</v>
-      </c>
-      <c r="P250" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="251" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A251" t="s">
-        <v>853</v>
-      </c>
-      <c r="B251" t="s">
-        <v>849</v>
-      </c>
-      <c r="C251" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K251" t="s">
-        <v>105</v>
-      </c>
-      <c r="P251" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="252" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A252" t="s">
-        <v>855</v>
-      </c>
-      <c r="B252" t="s">
-        <v>849</v>
-      </c>
-      <c r="C252" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K252" t="s">
-        <v>105</v>
-      </c>
-      <c r="P252" t="s">
         <v>856</v>
       </c>
     </row>
@@ -30576,7 +30577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1634"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A787" workbookViewId="0">
+    <sheetView topLeftCell="A787" workbookViewId="0">
       <selection activeCell="G806" sqref="G806"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added skydiver driver for working on adding 6800 cpu
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -15728,7 +15728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -15737,6 +15737,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
@@ -32494,8 +32495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1538"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A404" workbookViewId="0">
-      <selection activeCell="F423" sqref="F423"/>
+    <sheetView tabSelected="1" topLeftCell="A341" workbookViewId="0">
+      <selection activeCell="D356" sqref="D356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38278,7 +38279,7 @@
       <c r="C262" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D262" t="s">
+      <c r="D262" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K262" t="s">
@@ -38301,7 +38302,7 @@
       <c r="C263" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D263" t="s">
+      <c r="D263" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K263" t="s">
@@ -38324,7 +38325,7 @@
       <c r="C264" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D264" t="s">
+      <c r="D264" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K264" t="s">
@@ -38347,7 +38348,7 @@
       <c r="C265" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D265" t="s">
+      <c r="D265" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K265" t="s">
@@ -38370,7 +38371,7 @@
       <c r="C266" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D266" t="s">
+      <c r="D266" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K266" t="s">
@@ -38393,7 +38394,7 @@
       <c r="C267" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D267" t="s">
+      <c r="D267" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K267" t="s">
@@ -38416,7 +38417,7 @@
       <c r="C268" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D268" t="s">
+      <c r="D268" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K268" t="s">
@@ -38439,7 +38440,7 @@
       <c r="C269" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D269" t="s">
+      <c r="D269" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K269" t="s">
@@ -38462,7 +38463,7 @@
       <c r="C270" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D270" t="s">
+      <c r="D270" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K270" t="s">
@@ -38485,7 +38486,7 @@
       <c r="C271" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D271" t="s">
+      <c r="D271" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K271" t="s">
@@ -38508,7 +38509,7 @@
       <c r="C272" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D272" t="s">
+      <c r="D272" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K272" t="s">
@@ -38531,7 +38532,7 @@
       <c r="C273" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D273" t="s">
+      <c r="D273" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K273" t="s">
@@ -38554,7 +38555,7 @@
       <c r="C274" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D274" t="s">
+      <c r="D274" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K274" t="s">
@@ -38577,7 +38578,7 @@
       <c r="C275" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D275" t="s">
+      <c r="D275" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K275" t="s">
@@ -38600,7 +38601,7 @@
       <c r="C276" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D276" t="s">
+      <c r="D276" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K276" t="s">
@@ -38623,7 +38624,7 @@
       <c r="C277" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D277" t="s">
+      <c r="D277" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K277" t="s">
@@ -38646,7 +38647,7 @@
       <c r="C278" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D278" t="s">
+      <c r="D278" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K278" t="s">
@@ -38669,7 +38670,7 @@
       <c r="C279" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D279" t="s">
+      <c r="D279" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K279" t="s">
@@ -38692,7 +38693,7 @@
       <c r="C280" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D280" t="s">
+      <c r="D280" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K280" t="s">
@@ -38715,7 +38716,7 @@
       <c r="C281" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D281" t="s">
+      <c r="D281" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K281" t="s">
@@ -38738,7 +38739,7 @@
       <c r="C282" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D282" t="s">
+      <c r="D282" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K282" t="s">
@@ -38761,7 +38762,7 @@
       <c r="C283" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D283" t="s">
+      <c r="D283" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K283" t="s">
@@ -38784,7 +38785,7 @@
       <c r="C284" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D284" t="s">
+      <c r="D284" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K284" t="s">
@@ -38807,7 +38808,7 @@
       <c r="C285" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D285" t="s">
+      <c r="D285" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K285" t="s">
@@ -38830,7 +38831,7 @@
       <c r="C286" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D286" t="s">
+      <c r="D286" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K286" t="s">
@@ -39909,7 +39910,7 @@
       <c r="D341" t="s">
         <v>533</v>
       </c>
-      <c r="E341" t="s">
+      <c r="E341" s="6" t="s">
         <v>1173</v>
       </c>
       <c r="K341" t="s">
@@ -39932,7 +39933,7 @@
       <c r="D342" t="s">
         <v>533</v>
       </c>
-      <c r="E342" t="s">
+      <c r="E342" s="6" t="s">
         <v>1173</v>
       </c>
       <c r="K342" t="s">
@@ -39955,7 +39956,7 @@
       <c r="D343" t="s">
         <v>533</v>
       </c>
-      <c r="E343" t="s">
+      <c r="E343" s="6" t="s">
         <v>1173</v>
       </c>
       <c r="K343" t="s">
@@ -39978,7 +39979,7 @@
       <c r="D344" t="s">
         <v>533</v>
       </c>
-      <c r="E344" t="s">
+      <c r="E344" s="6" t="s">
         <v>1173</v>
       </c>
       <c r="K344" t="s">
@@ -40001,7 +40002,7 @@
       <c r="D345" t="s">
         <v>533</v>
       </c>
-      <c r="E345" t="s">
+      <c r="E345" s="6" t="s">
         <v>1173</v>
       </c>
       <c r="F345" s="2" t="s">
@@ -40027,7 +40028,7 @@
       <c r="D346" t="s">
         <v>533</v>
       </c>
-      <c r="E346" t="s">
+      <c r="E346" s="6" t="s">
         <v>1173</v>
       </c>
       <c r="F346" s="2" t="s">
@@ -40053,7 +40054,7 @@
       <c r="D347" t="s">
         <v>533</v>
       </c>
-      <c r="E347" t="s">
+      <c r="E347" s="6" t="s">
         <v>1173</v>
       </c>
       <c r="F347" s="2" t="s">
@@ -40079,7 +40080,7 @@
       <c r="D348" t="s">
         <v>533</v>
       </c>
-      <c r="E348" t="s">
+      <c r="E348" s="6" t="s">
         <v>1173</v>
       </c>
       <c r="F348" s="2" t="s">
@@ -40105,7 +40106,7 @@
       <c r="D349" t="s">
         <v>533</v>
       </c>
-      <c r="E349" t="s">
+      <c r="E349" s="6" t="s">
         <v>1173</v>
       </c>
       <c r="F349" s="2" t="s">
@@ -40131,7 +40132,7 @@
       <c r="D350" t="s">
         <v>533</v>
       </c>
-      <c r="E350" t="s">
+      <c r="E350" s="6" t="s">
         <v>1173</v>
       </c>
       <c r="F350" s="2" t="s">
@@ -40157,7 +40158,7 @@
       <c r="D351" t="s">
         <v>533</v>
       </c>
-      <c r="E351" t="s">
+      <c r="E351" s="6" t="s">
         <v>1173</v>
       </c>
       <c r="F351" s="2" t="s">
@@ -40183,7 +40184,7 @@
       <c r="D352" t="s">
         <v>533</v>
       </c>
-      <c r="E352" t="s">
+      <c r="E352" s="6" t="s">
         <v>1173</v>
       </c>
       <c r="F352" s="2" t="s">
@@ -40275,7 +40276,7 @@
       <c r="C356" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D356" t="s">
+      <c r="D356" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K356" t="s">
@@ -40295,7 +40296,7 @@
       <c r="C357" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D357" t="s">
+      <c r="D357" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K357" t="s">
@@ -40315,7 +40316,7 @@
       <c r="C358" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D358" t="s">
+      <c r="D358" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K358" t="s">
@@ -40335,7 +40336,7 @@
       <c r="C359" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D359" t="s">
+      <c r="D359" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K359" t="s">
@@ -40355,7 +40356,7 @@
       <c r="C360" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D360" t="s">
+      <c r="D360" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K360" t="s">
@@ -40375,7 +40376,7 @@
       <c r="C361" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D361" t="s">
+      <c r="D361" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K361" t="s">
@@ -40395,7 +40396,7 @@
       <c r="C362" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D362" t="s">
+      <c r="D362" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K362" t="s">
@@ -40415,7 +40416,7 @@
       <c r="C363" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D363" t="s">
+      <c r="D363" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K363" t="s">
@@ -40435,7 +40436,7 @@
       <c r="C364" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D364" t="s">
+      <c r="D364" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K364" t="s">
@@ -40455,7 +40456,7 @@
       <c r="C365" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D365" t="s">
+      <c r="D365" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K365" t="s">
@@ -40475,7 +40476,7 @@
       <c r="C366" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D366" t="s">
+      <c r="D366" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K366" t="s">
@@ -40495,7 +40496,7 @@
       <c r="C367" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D367" t="s">
+      <c r="D367" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K367" t="s">
@@ -40515,7 +40516,7 @@
       <c r="C368" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D368" t="s">
+      <c r="D368" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K368" t="s">
@@ -40535,7 +40536,7 @@
       <c r="C369" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D369" t="s">
+      <c r="D369" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K369" t="s">
@@ -40555,7 +40556,7 @@
       <c r="C370" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D370" t="s">
+      <c r="D370" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K370" t="s">
@@ -40575,7 +40576,7 @@
       <c r="C371" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D371" t="s">
+      <c r="D371" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K371" t="s">
@@ -40595,7 +40596,7 @@
       <c r="C372" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D372" t="s">
+      <c r="D372" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K372" t="s">
@@ -40615,7 +40616,7 @@
       <c r="C373" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D373" t="s">
+      <c r="D373" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K373" t="s">
@@ -40635,7 +40636,7 @@
       <c r="C374" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D374" t="s">
+      <c r="D374" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K374" t="s">
@@ -40658,7 +40659,7 @@
       <c r="C375" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D375" t="s">
+      <c r="D375" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K375" t="s">
@@ -40681,7 +40682,7 @@
       <c r="C376" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D376" t="s">
+      <c r="D376" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K376" t="s">
@@ -40704,7 +40705,7 @@
       <c r="C377" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D377" t="s">
+      <c r="D377" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K377" t="s">
@@ -40724,7 +40725,7 @@
       <c r="C378" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D378" t="s">
+      <c r="D378" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K378" t="s">
@@ -40744,7 +40745,7 @@
       <c r="C379" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D379" t="s">
+      <c r="D379" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K379" t="s">
@@ -40764,7 +40765,7 @@
       <c r="C380" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D380" t="s">
+      <c r="D380" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K380" t="s">
@@ -40784,7 +40785,7 @@
       <c r="C381" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D381" t="s">
+      <c r="D381" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="E381" t="s">
@@ -40816,7 +40817,7 @@
       <c r="C382" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D382" t="s">
+      <c r="D382" s="6" t="s">
         <v>1985</v>
       </c>
       <c r="K382" t="s">
@@ -46646,7 +46647,7 @@
       <c r="B657" t="s">
         <v>3765</v>
       </c>
-      <c r="C657" s="1" t="s">
+      <c r="C657" s="8" t="s">
         <v>3766</v>
       </c>
       <c r="P657" t="s">
@@ -48652,10 +48653,10 @@
       <c r="C751" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D751" t="s">
+      <c r="D751" s="6" t="s">
         <v>1173</v>
       </c>
-      <c r="E751" t="s">
+      <c r="E751" s="6" t="s">
         <v>1173</v>
       </c>
       <c r="P751" t="s">
@@ -48672,10 +48673,10 @@
       <c r="C752" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D752" t="s">
+      <c r="D752" s="6" t="s">
         <v>1173</v>
       </c>
-      <c r="E752" t="s">
+      <c r="E752" s="6" t="s">
         <v>1173</v>
       </c>
       <c r="P752" t="s">
@@ -48692,10 +48693,10 @@
       <c r="C753" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D753" t="s">
+      <c r="D753" s="6" t="s">
         <v>1173</v>
       </c>
-      <c r="E753" t="s">
+      <c r="E753" s="6" t="s">
         <v>1173</v>
       </c>
       <c r="P753" t="s">
@@ -48712,10 +48713,10 @@
       <c r="C754" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D754" t="s">
+      <c r="D754" s="6" t="s">
         <v>1173</v>
       </c>
-      <c r="E754" t="s">
+      <c r="E754" s="6" t="s">
         <v>1173</v>
       </c>
       <c r="P754" t="s">
@@ -49012,7 +49013,7 @@
       <c r="C772" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D772" t="s">
+      <c r="D772" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K772" t="s">
@@ -49035,7 +49036,7 @@
       <c r="C773" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D773" t="s">
+      <c r="D773" s="6" t="s">
         <v>1282</v>
       </c>
       <c r="K773" t="s">

</xml_diff>

<commit_message>
added working asteroid,bwidow,shaolins driver
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Playable" sheetId="2" r:id="rId1"/>
@@ -15961,10 +15961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P732"/>
+  <dimension ref="A1:P634"/>
   <sheetViews>
-    <sheetView topLeftCell="A705" workbookViewId="0">
-      <selection activeCell="A734" sqref="A734"/>
+    <sheetView topLeftCell="A607" workbookViewId="0">
+      <selection activeCell="A633" sqref="A633:XFD634"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28743,2303 +28743,229 @@
     </row>
     <row r="622" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A622" s="1" t="s">
-        <v>1211</v>
+        <v>3645</v>
       </c>
       <c r="B622" t="s">
-        <v>1212</v>
+        <v>3646</v>
       </c>
       <c r="C622" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D622" t="s">
-        <v>15</v>
+        <v>450</v>
       </c>
       <c r="K622" t="s">
-        <v>1213</v>
+        <v>107</v>
       </c>
       <c r="P622" t="s">
-        <v>1214</v>
+        <v>3647</v>
       </c>
     </row>
     <row r="623" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A623" s="1" t="s">
-        <v>1215</v>
+        <v>3648</v>
       </c>
       <c r="B623" t="s">
-        <v>1212</v>
+        <v>3646</v>
       </c>
       <c r="C623" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D623" t="s">
-        <v>15</v>
+        <v>450</v>
       </c>
       <c r="K623" t="s">
-        <v>1213</v>
+        <v>107</v>
       </c>
       <c r="P623" t="s">
-        <v>1216</v>
+        <v>3649</v>
       </c>
     </row>
     <row r="624" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A624" s="1" t="s">
-        <v>1217</v>
+        <v>3650</v>
       </c>
       <c r="B624" t="s">
-        <v>1212</v>
+        <v>3646</v>
       </c>
       <c r="C624" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D624" t="s">
-        <v>15</v>
+        <v>450</v>
       </c>
       <c r="K624" t="s">
-        <v>1213</v>
+        <v>107</v>
       </c>
       <c r="P624" t="s">
-        <v>1218</v>
+        <v>3651</v>
       </c>
     </row>
     <row r="625" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A625" s="1" t="s">
-        <v>1219</v>
+        <v>3652</v>
       </c>
       <c r="B625" t="s">
-        <v>1212</v>
+        <v>3646</v>
       </c>
       <c r="C625" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D625" t="s">
-        <v>15</v>
+        <v>450</v>
       </c>
       <c r="K625" t="s">
-        <v>1213</v>
+        <v>3653</v>
+      </c>
+      <c r="L625" t="s">
+        <v>107</v>
       </c>
       <c r="P625" t="s">
-        <v>1220</v>
+        <v>3654</v>
       </c>
     </row>
     <row r="626" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A626" s="1" t="s">
-        <v>1221</v>
+        <v>3655</v>
       </c>
       <c r="B626" t="s">
-        <v>1212</v>
+        <v>3646</v>
       </c>
       <c r="C626" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D626" t="s">
-        <v>15</v>
+        <v>450</v>
       </c>
       <c r="K626" t="s">
-        <v>1213</v>
+        <v>3653</v>
+      </c>
+      <c r="L626" t="s">
+        <v>107</v>
       </c>
       <c r="P626" t="s">
-        <v>1222</v>
+        <v>3656</v>
       </c>
     </row>
     <row r="627" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A627" s="1" t="s">
-        <v>1223</v>
+        <v>3670</v>
       </c>
       <c r="B627" t="s">
-        <v>1212</v>
+        <v>3646</v>
       </c>
       <c r="C627" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D627" t="s">
-        <v>15</v>
+        <v>450</v>
       </c>
       <c r="K627" t="s">
-        <v>1213</v>
+        <v>107</v>
       </c>
       <c r="P627" t="s">
-        <v>1224</v>
+        <v>3671</v>
       </c>
     </row>
     <row r="628" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A628" s="1" t="s">
-        <v>1225</v>
+        <v>3672</v>
       </c>
       <c r="B628" t="s">
-        <v>1212</v>
+        <v>3646</v>
       </c>
       <c r="C628" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D628" t="s">
-        <v>15</v>
+        <v>450</v>
       </c>
       <c r="K628" t="s">
-        <v>1213</v>
+        <v>107</v>
       </c>
       <c r="P628" t="s">
-        <v>1226</v>
+        <v>3673</v>
       </c>
     </row>
     <row r="629" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A629" s="1" t="s">
-        <v>1227</v>
+        <v>3666</v>
       </c>
       <c r="B629" t="s">
-        <v>1212</v>
+        <v>3658</v>
       </c>
       <c r="C629" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D629" t="s">
-        <v>15</v>
+        <v>450</v>
       </c>
       <c r="K629" t="s">
-        <v>1213</v>
+        <v>3659</v>
       </c>
       <c r="P629" t="s">
-        <v>1228</v>
+        <v>3667</v>
       </c>
     </row>
     <row r="630" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A630" s="1" t="s">
-        <v>1229</v>
+        <v>3668</v>
       </c>
       <c r="B630" t="s">
-        <v>1212</v>
+        <v>3658</v>
       </c>
       <c r="C630" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D630" t="s">
-        <v>15</v>
+        <v>450</v>
       </c>
       <c r="K630" t="s">
-        <v>1213</v>
+        <v>3659</v>
       </c>
       <c r="P630" t="s">
-        <v>1230</v>
+        <v>3669</v>
       </c>
     </row>
     <row r="631" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A631" s="1" t="s">
-        <v>1231</v>
+        <v>3676</v>
       </c>
       <c r="B631" t="s">
-        <v>1212</v>
+        <v>3658</v>
       </c>
       <c r="C631" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D631" t="s">
-        <v>15</v>
+        <v>450</v>
       </c>
       <c r="K631" t="s">
-        <v>1213</v>
+        <v>3659</v>
       </c>
       <c r="P631" t="s">
-        <v>1232</v>
+        <v>3677</v>
       </c>
     </row>
     <row r="632" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A632" s="1" t="s">
-        <v>1233</v>
+        <v>3657</v>
       </c>
       <c r="B632" t="s">
-        <v>1212</v>
+        <v>3658</v>
       </c>
       <c r="C632" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D632" t="s">
-        <v>15</v>
+        <v>450</v>
       </c>
       <c r="K632" t="s">
-        <v>1213</v>
+        <v>3659</v>
       </c>
       <c r="P632" t="s">
-        <v>1234</v>
+        <v>3660</v>
       </c>
     </row>
     <row r="633" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A633" s="1" t="s">
-        <v>1235</v>
+        <v>3249</v>
       </c>
       <c r="B633" t="s">
-        <v>1212</v>
+        <v>3250</v>
       </c>
       <c r="C633" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="D633" t="s">
-        <v>15</v>
-      </c>
       <c r="K633" t="s">
-        <v>1213</v>
+        <v>3</v>
       </c>
       <c r="P633" t="s">
-        <v>1236</v>
+        <v>3251</v>
       </c>
     </row>
     <row r="634" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A634" s="1" t="s">
-        <v>1237</v>
+        <v>3252</v>
       </c>
       <c r="B634" t="s">
-        <v>1212</v>
+        <v>3250</v>
       </c>
       <c r="C634" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="D634" t="s">
-        <v>15</v>
-      </c>
       <c r="K634" t="s">
-        <v>1213</v>
+        <v>3</v>
       </c>
       <c r="P634" t="s">
-        <v>1238</v>
-      </c>
-    </row>
-    <row r="635" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A635" s="1" t="s">
-        <v>1239</v>
-      </c>
-      <c r="B635" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C635" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D635" t="s">
-        <v>15</v>
-      </c>
-      <c r="K635" t="s">
-        <v>1213</v>
-      </c>
-      <c r="P635" t="s">
-        <v>1240</v>
-      </c>
-    </row>
-    <row r="636" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A636" s="1" t="s">
-        <v>1241</v>
-      </c>
-      <c r="B636" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C636" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D636" t="s">
-        <v>15</v>
-      </c>
-      <c r="K636" t="s">
-        <v>1213</v>
-      </c>
-      <c r="P636" t="s">
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="637" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A637" s="1" t="s">
-        <v>1243</v>
-      </c>
-      <c r="B637" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C637" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D637" t="s">
-        <v>15</v>
-      </c>
-      <c r="K637" t="s">
-        <v>1213</v>
-      </c>
-      <c r="P637" t="s">
-        <v>1244</v>
-      </c>
-    </row>
-    <row r="638" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A638" s="1" t="s">
-        <v>1245</v>
-      </c>
-      <c r="B638" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C638" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D638" t="s">
-        <v>15</v>
-      </c>
-      <c r="K638" t="s">
-        <v>1213</v>
-      </c>
-      <c r="P638" t="s">
-        <v>1246</v>
-      </c>
-    </row>
-    <row r="639" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A639" s="1" t="s">
-        <v>1247</v>
-      </c>
-      <c r="B639" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C639" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D639" t="s">
-        <v>15</v>
-      </c>
-      <c r="K639" t="s">
-        <v>1213</v>
-      </c>
-      <c r="P639" t="s">
-        <v>1248</v>
-      </c>
-    </row>
-    <row r="640" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A640" s="1" t="s">
-        <v>1249</v>
-      </c>
-      <c r="B640" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C640" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D640" t="s">
-        <v>15</v>
-      </c>
-      <c r="K640" t="s">
-        <v>1213</v>
-      </c>
-      <c r="P640" t="s">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="641" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A641" s="1" t="s">
-        <v>1251</v>
-      </c>
-      <c r="B641" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C641" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D641" t="s">
-        <v>15</v>
-      </c>
-      <c r="K641" t="s">
-        <v>1213</v>
-      </c>
-      <c r="P641" t="s">
-        <v>1252</v>
-      </c>
-    </row>
-    <row r="642" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A642" s="1" t="s">
-        <v>1253</v>
-      </c>
-      <c r="B642" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C642" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D642" t="s">
-        <v>15</v>
-      </c>
-      <c r="K642" t="s">
-        <v>1213</v>
-      </c>
-      <c r="P642" t="s">
-        <v>1254</v>
-      </c>
-    </row>
-    <row r="643" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A643" s="1" t="s">
-        <v>1255</v>
-      </c>
-      <c r="B643" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C643" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D643" t="s">
-        <v>15</v>
-      </c>
-      <c r="K643" t="s">
-        <v>1213</v>
-      </c>
-      <c r="P643" t="s">
-        <v>1256</v>
-      </c>
-    </row>
-    <row r="644" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A644" s="1" t="s">
-        <v>1257</v>
-      </c>
-      <c r="B644" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C644" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D644" t="s">
-        <v>15</v>
-      </c>
-      <c r="K644" t="s">
-        <v>1213</v>
-      </c>
-      <c r="P644" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="645" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A645" s="1" t="s">
-        <v>2064</v>
-      </c>
-      <c r="B645" t="s">
-        <v>2065</v>
-      </c>
-      <c r="C645" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D645" t="s">
-        <v>15</v>
-      </c>
-      <c r="K645" t="s">
-        <v>1538</v>
-      </c>
-      <c r="P645" t="s">
-        <v>2066</v>
-      </c>
-    </row>
-    <row r="646" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A646" s="1" t="s">
-        <v>2067</v>
-      </c>
-      <c r="B646" t="s">
-        <v>2065</v>
-      </c>
-      <c r="C646" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D646" t="s">
-        <v>15</v>
-      </c>
-      <c r="K646" t="s">
-        <v>1538</v>
-      </c>
-      <c r="P646" t="s">
-        <v>2068</v>
-      </c>
-    </row>
-    <row r="647" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A647" s="1" t="s">
-        <v>2069</v>
-      </c>
-      <c r="B647" t="s">
-        <v>2065</v>
-      </c>
-      <c r="C647" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D647" t="s">
-        <v>15</v>
-      </c>
-      <c r="K647" t="s">
-        <v>1538</v>
-      </c>
-      <c r="P647" t="s">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="648" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A648" s="1" t="s">
-        <v>2071</v>
-      </c>
-      <c r="B648" t="s">
-        <v>2065</v>
-      </c>
-      <c r="C648" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D648" t="s">
-        <v>15</v>
-      </c>
-      <c r="K648" t="s">
-        <v>1538</v>
-      </c>
-      <c r="P648" t="s">
-        <v>2072</v>
-      </c>
-    </row>
-    <row r="649" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A649" s="1" t="s">
-        <v>2073</v>
-      </c>
-      <c r="B649" t="s">
-        <v>2065</v>
-      </c>
-      <c r="C649" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D649" t="s">
-        <v>15</v>
-      </c>
-      <c r="K649" t="s">
-        <v>1538</v>
-      </c>
-      <c r="P649" t="s">
-        <v>2074</v>
-      </c>
-    </row>
-    <row r="650" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A650" s="1" t="s">
-        <v>2075</v>
-      </c>
-      <c r="B650" t="s">
-        <v>2065</v>
-      </c>
-      <c r="C650" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D650" t="s">
-        <v>15</v>
-      </c>
-      <c r="K650" t="s">
-        <v>1538</v>
-      </c>
-      <c r="P650" t="s">
-        <v>2076</v>
-      </c>
-    </row>
-    <row r="651" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A651" s="1" t="s">
-        <v>2077</v>
-      </c>
-      <c r="B651" t="s">
-        <v>2065</v>
-      </c>
-      <c r="C651" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D651" t="s">
-        <v>15</v>
-      </c>
-      <c r="K651" t="s">
-        <v>1538</v>
-      </c>
-      <c r="P651" t="s">
-        <v>2078</v>
-      </c>
-    </row>
-    <row r="652" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A652" s="1" t="s">
-        <v>2385</v>
-      </c>
-      <c r="B652" t="s">
-        <v>2386</v>
-      </c>
-      <c r="C652" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D652" t="s">
-        <v>571</v>
-      </c>
-      <c r="K652" t="s">
-        <v>369</v>
-      </c>
-      <c r="L652" t="s">
-        <v>192</v>
-      </c>
-      <c r="P652" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="653" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A653" s="1" t="s">
-        <v>2388</v>
-      </c>
-      <c r="B653" t="s">
-        <v>2386</v>
-      </c>
-      <c r="C653" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D653" t="s">
-        <v>571</v>
-      </c>
-      <c r="K653" t="s">
-        <v>369</v>
-      </c>
-      <c r="L653" t="s">
-        <v>192</v>
-      </c>
-      <c r="P653" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="654" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A654" s="1" t="s">
-        <v>2390</v>
-      </c>
-      <c r="B654" t="s">
-        <v>2386</v>
-      </c>
-      <c r="C654" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D654" t="s">
-        <v>571</v>
-      </c>
-      <c r="K654" t="s">
-        <v>369</v>
-      </c>
-      <c r="L654" t="s">
-        <v>192</v>
-      </c>
-      <c r="P654" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="655" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A655" s="1" t="s">
-        <v>2392</v>
-      </c>
-      <c r="B655" t="s">
-        <v>2386</v>
-      </c>
-      <c r="C655" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D655" t="s">
-        <v>571</v>
-      </c>
-      <c r="K655" t="s">
-        <v>369</v>
-      </c>
-      <c r="L655" t="s">
-        <v>192</v>
-      </c>
-      <c r="P655" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="656" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A656" s="1" t="s">
-        <v>2844</v>
-      </c>
-      <c r="B656" t="s">
-        <v>2845</v>
-      </c>
-      <c r="C656" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D656" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K656" t="s">
-        <v>16</v>
-      </c>
-      <c r="P656" t="s">
-        <v>2846</v>
-      </c>
-    </row>
-    <row r="657" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A657" s="1" t="s">
-        <v>2847</v>
-      </c>
-      <c r="B657" t="s">
-        <v>2845</v>
-      </c>
-      <c r="C657" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D657" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K657" t="s">
-        <v>16</v>
-      </c>
-      <c r="P657" t="s">
-        <v>2848</v>
-      </c>
-    </row>
-    <row r="658" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A658" s="1" t="s">
-        <v>2849</v>
-      </c>
-      <c r="B658" t="s">
-        <v>2845</v>
-      </c>
-      <c r="C658" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D658" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K658" t="s">
-        <v>16</v>
-      </c>
-      <c r="P658" t="s">
-        <v>2850</v>
-      </c>
-    </row>
-    <row r="659" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A659" s="1" t="s">
-        <v>2851</v>
-      </c>
-      <c r="B659" t="s">
-        <v>2845</v>
-      </c>
-      <c r="C659" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D659" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K659" t="s">
-        <v>16</v>
-      </c>
-      <c r="P659" t="s">
-        <v>2852</v>
-      </c>
-    </row>
-    <row r="660" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A660" s="1" t="s">
-        <v>2853</v>
-      </c>
-      <c r="B660" t="s">
-        <v>2845</v>
-      </c>
-      <c r="C660" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D660" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K660" t="s">
-        <v>16</v>
-      </c>
-      <c r="P660" t="s">
-        <v>2854</v>
-      </c>
-    </row>
-    <row r="661" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A661" s="1" t="s">
-        <v>2855</v>
-      </c>
-      <c r="B661" t="s">
-        <v>2845</v>
-      </c>
-      <c r="C661" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D661" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K661" t="s">
-        <v>16</v>
-      </c>
-      <c r="P661" t="s">
-        <v>2856</v>
-      </c>
-    </row>
-    <row r="662" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A662" s="1" t="s">
-        <v>2857</v>
-      </c>
-      <c r="B662" t="s">
-        <v>2845</v>
-      </c>
-      <c r="C662" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D662" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K662" t="s">
-        <v>16</v>
-      </c>
-      <c r="P662" t="s">
-        <v>2858</v>
-      </c>
-    </row>
-    <row r="663" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A663" s="1" t="s">
-        <v>2859</v>
-      </c>
-      <c r="B663" t="s">
-        <v>2845</v>
-      </c>
-      <c r="C663" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D663" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K663" t="s">
-        <v>16</v>
-      </c>
-      <c r="P663" t="s">
-        <v>2860</v>
-      </c>
-    </row>
-    <row r="664" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A664" s="1" t="s">
-        <v>2861</v>
-      </c>
-      <c r="B664" t="s">
-        <v>2845</v>
-      </c>
-      <c r="C664" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D664" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K664" t="s">
-        <v>16</v>
-      </c>
-      <c r="P664" t="s">
-        <v>2862</v>
-      </c>
-    </row>
-    <row r="665" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A665" s="1" t="s">
-        <v>2863</v>
-      </c>
-      <c r="B665" t="s">
-        <v>2845</v>
-      </c>
-      <c r="C665" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D665" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K665" t="s">
-        <v>16</v>
-      </c>
-      <c r="P665" t="s">
-        <v>2864</v>
-      </c>
-    </row>
-    <row r="666" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A666" s="1" t="s">
-        <v>2865</v>
-      </c>
-      <c r="B666" t="s">
-        <v>2845</v>
-      </c>
-      <c r="C666" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D666" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K666" t="s">
-        <v>16</v>
-      </c>
-      <c r="P666" t="s">
-        <v>2866</v>
-      </c>
-    </row>
-    <row r="667" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A667" s="1" t="s">
-        <v>2867</v>
-      </c>
-      <c r="B667" t="s">
-        <v>2845</v>
-      </c>
-      <c r="C667" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D667" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K667" t="s">
-        <v>16</v>
-      </c>
-      <c r="P667" t="s">
-        <v>2868</v>
-      </c>
-    </row>
-    <row r="668" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A668" s="1" t="s">
-        <v>2915</v>
-      </c>
-      <c r="B668" t="s">
-        <v>2916</v>
-      </c>
-      <c r="C668" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D668" t="s">
-        <v>525</v>
-      </c>
-      <c r="K668" t="s">
-        <v>369</v>
-      </c>
-      <c r="L668" t="s">
-        <v>363</v>
-      </c>
-      <c r="P668" t="s">
-        <v>2917</v>
-      </c>
-    </row>
-    <row r="669" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A669" s="1" t="s">
-        <v>2918</v>
-      </c>
-      <c r="B669" t="s">
-        <v>2916</v>
-      </c>
-      <c r="C669" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D669" t="s">
-        <v>525</v>
-      </c>
-      <c r="K669" t="s">
-        <v>369</v>
-      </c>
-      <c r="L669" t="s">
-        <v>363</v>
-      </c>
-      <c r="P669" t="s">
-        <v>2919</v>
-      </c>
-    </row>
-    <row r="670" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A670" s="1" t="s">
-        <v>2920</v>
-      </c>
-      <c r="B670" t="s">
-        <v>2916</v>
-      </c>
-      <c r="C670" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D670" t="s">
-        <v>525</v>
-      </c>
-      <c r="K670" t="s">
-        <v>369</v>
-      </c>
-      <c r="L670" t="s">
-        <v>363</v>
-      </c>
-      <c r="P670" t="s">
-        <v>2921</v>
-      </c>
-    </row>
-    <row r="671" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A671" s="1" t="s">
-        <v>2933</v>
-      </c>
-      <c r="B671" t="s">
-        <v>2934</v>
-      </c>
-      <c r="C671" s="1" t="s">
-        <v>2935</v>
-      </c>
-      <c r="D671" t="s">
-        <v>5178</v>
-      </c>
-      <c r="K671" t="s">
-        <v>369</v>
-      </c>
-      <c r="L671" t="s">
-        <v>1534</v>
-      </c>
-      <c r="P671" t="s">
-        <v>2936</v>
-      </c>
-    </row>
-    <row r="672" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A672" s="1" t="s">
-        <v>2937</v>
-      </c>
-      <c r="B672" t="s">
-        <v>2934</v>
-      </c>
-      <c r="C672" s="1" t="s">
-        <v>2935</v>
-      </c>
-      <c r="D672" t="s">
-        <v>5178</v>
-      </c>
-      <c r="K672" t="s">
-        <v>369</v>
-      </c>
-      <c r="L672" t="s">
-        <v>1534</v>
-      </c>
-      <c r="P672" t="s">
-        <v>2938</v>
-      </c>
-    </row>
-    <row r="673" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A673" s="1" t="s">
-        <v>2939</v>
-      </c>
-      <c r="B673" t="s">
-        <v>2940</v>
-      </c>
-      <c r="C673" s="1" t="s">
-        <v>2935</v>
-      </c>
-      <c r="D673" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K673" t="s">
-        <v>369</v>
-      </c>
-      <c r="L673" t="s">
-        <v>388</v>
-      </c>
-      <c r="M673" t="s">
-        <v>1918</v>
-      </c>
-      <c r="P673" t="s">
-        <v>2941</v>
-      </c>
-    </row>
-    <row r="674" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A674" s="1" t="s">
-        <v>2942</v>
-      </c>
-      <c r="B674" t="s">
-        <v>2940</v>
-      </c>
-      <c r="C674" s="1" t="s">
-        <v>2935</v>
-      </c>
-      <c r="D674" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K674" t="s">
-        <v>369</v>
-      </c>
-      <c r="L674" t="s">
-        <v>388</v>
-      </c>
-      <c r="M674" t="s">
-        <v>1918</v>
-      </c>
-      <c r="P674" t="s">
-        <v>2943</v>
-      </c>
-    </row>
-    <row r="675" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A675" s="1" t="s">
-        <v>2944</v>
-      </c>
-      <c r="B675" t="s">
-        <v>2940</v>
-      </c>
-      <c r="C675" s="1" t="s">
-        <v>2935</v>
-      </c>
-      <c r="D675" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K675" t="s">
-        <v>369</v>
-      </c>
-      <c r="L675" t="s">
-        <v>388</v>
-      </c>
-      <c r="M675" t="s">
-        <v>1918</v>
-      </c>
-      <c r="P675" t="s">
-        <v>2945</v>
-      </c>
-    </row>
-    <row r="676" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A676" s="1" t="s">
-        <v>2946</v>
-      </c>
-      <c r="B676" t="s">
-        <v>2940</v>
-      </c>
-      <c r="C676" s="1" t="s">
-        <v>2935</v>
-      </c>
-      <c r="D676" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K676" t="s">
-        <v>369</v>
-      </c>
-      <c r="L676" t="s">
-        <v>388</v>
-      </c>
-      <c r="M676" t="s">
-        <v>1918</v>
-      </c>
-      <c r="P676" t="s">
-        <v>2947</v>
-      </c>
-    </row>
-    <row r="677" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A677" s="1" t="s">
-        <v>3185</v>
-      </c>
-      <c r="B677" t="s">
-        <v>3186</v>
-      </c>
-      <c r="C677" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D677" t="s">
-        <v>525</v>
-      </c>
-      <c r="E677" t="s">
-        <v>15</v>
-      </c>
-      <c r="F677" s="6" t="s">
-        <v>830</v>
-      </c>
-      <c r="K677" t="s">
-        <v>97</v>
-      </c>
-      <c r="L677" t="s">
-        <v>192</v>
-      </c>
-      <c r="P677" t="s">
-        <v>3187</v>
-      </c>
-    </row>
-    <row r="678" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A678" s="1" t="s">
-        <v>3225</v>
-      </c>
-      <c r="B678" t="s">
-        <v>3226</v>
-      </c>
-      <c r="C678" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D678" t="s">
-        <v>15</v>
-      </c>
-      <c r="K678" t="s">
-        <v>192</v>
-      </c>
-      <c r="L678" t="s">
-        <v>3198</v>
-      </c>
-      <c r="M678" t="s">
-        <v>852</v>
-      </c>
-      <c r="P678" t="s">
-        <v>3227</v>
-      </c>
-    </row>
-    <row r="679" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A679" s="1" t="s">
-        <v>3228</v>
-      </c>
-      <c r="B679" t="s">
-        <v>3226</v>
-      </c>
-      <c r="C679" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D679" t="s">
-        <v>15</v>
-      </c>
-      <c r="K679" t="s">
-        <v>192</v>
-      </c>
-      <c r="L679" t="s">
-        <v>3198</v>
-      </c>
-      <c r="M679" t="s">
-        <v>852</v>
-      </c>
-      <c r="P679" t="s">
-        <v>3229</v>
-      </c>
-    </row>
-    <row r="680" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A680" s="1" t="s">
-        <v>3240</v>
-      </c>
-      <c r="B680" t="s">
-        <v>3226</v>
-      </c>
-      <c r="C680" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D680" t="s">
-        <v>15</v>
-      </c>
-      <c r="K680" t="s">
-        <v>192</v>
-      </c>
-      <c r="L680" t="s">
-        <v>3198</v>
-      </c>
-      <c r="M680" t="s">
-        <v>852</v>
-      </c>
-      <c r="P680" t="s">
-        <v>3241</v>
-      </c>
-    </row>
-    <row r="681" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A681" s="1" t="s">
-        <v>3242</v>
-      </c>
-      <c r="B681" t="s">
-        <v>3226</v>
-      </c>
-      <c r="C681" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D681" t="s">
-        <v>15</v>
-      </c>
-      <c r="K681" t="s">
-        <v>192</v>
-      </c>
-      <c r="L681" t="s">
-        <v>3198</v>
-      </c>
-      <c r="M681" t="s">
-        <v>852</v>
-      </c>
-      <c r="P681" t="s">
-        <v>3243</v>
-      </c>
-    </row>
-    <row r="682" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A682" s="1" t="s">
-        <v>3249</v>
-      </c>
-      <c r="B682" t="s">
-        <v>3250</v>
-      </c>
-      <c r="C682" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="K682" t="s">
-        <v>3</v>
-      </c>
-      <c r="P682" t="s">
-        <v>3251</v>
-      </c>
-    </row>
-    <row r="683" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A683" s="1" t="s">
-        <v>3252</v>
-      </c>
-      <c r="B683" t="s">
-        <v>3250</v>
-      </c>
-      <c r="C683" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="K683" t="s">
-        <v>3</v>
-      </c>
-      <c r="P683" t="s">
         <v>3253</v>
-      </c>
-    </row>
-    <row r="684" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A684" s="1" t="s">
-        <v>3281</v>
-      </c>
-      <c r="B684" t="s">
-        <v>3282</v>
-      </c>
-      <c r="C684" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D684" t="s">
-        <v>525</v>
-      </c>
-      <c r="K684" t="s">
-        <v>613</v>
-      </c>
-      <c r="P684" t="s">
-        <v>3283</v>
-      </c>
-    </row>
-    <row r="685" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A685" s="1" t="s">
-        <v>3284</v>
-      </c>
-      <c r="B685" t="s">
-        <v>3282</v>
-      </c>
-      <c r="C685" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D685" t="s">
-        <v>525</v>
-      </c>
-      <c r="K685" t="s">
-        <v>613</v>
-      </c>
-      <c r="P685" t="s">
-        <v>3285</v>
-      </c>
-    </row>
-    <row r="686" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A686" s="1" t="s">
-        <v>3286</v>
-      </c>
-      <c r="B686" t="s">
-        <v>3282</v>
-      </c>
-      <c r="C686" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D686" t="s">
-        <v>525</v>
-      </c>
-      <c r="K686" t="s">
-        <v>613</v>
-      </c>
-      <c r="P686" t="s">
-        <v>3287</v>
-      </c>
-    </row>
-    <row r="687" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A687" s="1" t="s">
-        <v>3288</v>
-      </c>
-      <c r="B687" t="s">
-        <v>3282</v>
-      </c>
-      <c r="C687" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D687" t="s">
-        <v>525</v>
-      </c>
-      <c r="K687" t="s">
-        <v>613</v>
-      </c>
-      <c r="P687" t="s">
-        <v>3289</v>
-      </c>
-    </row>
-    <row r="688" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A688" s="1" t="s">
-        <v>3304</v>
-      </c>
-      <c r="B688" t="s">
-        <v>3305</v>
-      </c>
-      <c r="C688" s="1" t="s">
-        <v>2960</v>
-      </c>
-      <c r="D688" t="s">
-        <v>15</v>
-      </c>
-      <c r="K688" t="s">
-        <v>369</v>
-      </c>
-      <c r="L688" t="s">
-        <v>2681</v>
-      </c>
-      <c r="P688" t="s">
-        <v>3306</v>
-      </c>
-    </row>
-    <row r="689" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A689" s="1" t="s">
-        <v>3307</v>
-      </c>
-      <c r="B689" t="s">
-        <v>3305</v>
-      </c>
-      <c r="C689" s="1" t="s">
-        <v>2960</v>
-      </c>
-      <c r="D689" t="s">
-        <v>15</v>
-      </c>
-      <c r="K689" t="s">
-        <v>369</v>
-      </c>
-      <c r="L689" t="s">
-        <v>2681</v>
-      </c>
-      <c r="P689" t="s">
-        <v>3308</v>
-      </c>
-    </row>
-    <row r="690" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A690" s="1" t="s">
-        <v>3309</v>
-      </c>
-      <c r="B690" t="s">
-        <v>3305</v>
-      </c>
-      <c r="C690" s="1" t="s">
-        <v>2960</v>
-      </c>
-      <c r="D690" t="s">
-        <v>15</v>
-      </c>
-      <c r="K690" t="s">
-        <v>369</v>
-      </c>
-      <c r="L690" t="s">
-        <v>2681</v>
-      </c>
-      <c r="P690" t="s">
-        <v>3310</v>
-      </c>
-    </row>
-    <row r="691" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A691" s="1" t="s">
-        <v>3311</v>
-      </c>
-      <c r="B691" t="s">
-        <v>3305</v>
-      </c>
-      <c r="C691" s="1" t="s">
-        <v>2960</v>
-      </c>
-      <c r="D691" t="s">
-        <v>15</v>
-      </c>
-      <c r="K691" t="s">
-        <v>369</v>
-      </c>
-      <c r="L691" t="s">
-        <v>2681</v>
-      </c>
-      <c r="P691" t="s">
-        <v>3312</v>
-      </c>
-    </row>
-    <row r="692" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A692" s="1" t="s">
-        <v>3313</v>
-      </c>
-      <c r="B692" t="s">
-        <v>3305</v>
-      </c>
-      <c r="C692" s="1" t="s">
-        <v>2960</v>
-      </c>
-      <c r="D692" t="s">
-        <v>15</v>
-      </c>
-      <c r="K692" t="s">
-        <v>369</v>
-      </c>
-      <c r="L692" t="s">
-        <v>2681</v>
-      </c>
-      <c r="P692" t="s">
-        <v>3314</v>
-      </c>
-    </row>
-    <row r="693" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A693" s="1" t="s">
-        <v>3576</v>
-      </c>
-      <c r="B693" t="s">
-        <v>3577</v>
-      </c>
-      <c r="C693" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K693" t="s">
-        <v>107</v>
-      </c>
-      <c r="L693" t="s">
-        <v>451</v>
-      </c>
-      <c r="M693" t="s">
-        <v>192</v>
-      </c>
-      <c r="P693" t="s">
-        <v>3578</v>
-      </c>
-    </row>
-    <row r="694" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A694" s="1" t="s">
-        <v>3579</v>
-      </c>
-      <c r="B694" t="s">
-        <v>3577</v>
-      </c>
-      <c r="C694" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K694" t="s">
-        <v>107</v>
-      </c>
-      <c r="L694" t="s">
-        <v>451</v>
-      </c>
-      <c r="M694" t="s">
-        <v>192</v>
-      </c>
-      <c r="P694" t="s">
-        <v>3580</v>
-      </c>
-    </row>
-    <row r="695" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A695" s="1" t="s">
-        <v>3581</v>
-      </c>
-      <c r="B695" t="s">
-        <v>3577</v>
-      </c>
-      <c r="C695" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K695" t="s">
-        <v>107</v>
-      </c>
-      <c r="L695" t="s">
-        <v>451</v>
-      </c>
-      <c r="M695" t="s">
-        <v>192</v>
-      </c>
-      <c r="P695" t="s">
-        <v>3582</v>
-      </c>
-    </row>
-    <row r="696" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A696" s="1" t="s">
-        <v>3583</v>
-      </c>
-      <c r="B696" t="s">
-        <v>3577</v>
-      </c>
-      <c r="C696" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K696" t="s">
-        <v>107</v>
-      </c>
-      <c r="L696" t="s">
-        <v>451</v>
-      </c>
-      <c r="M696" t="s">
-        <v>192</v>
-      </c>
-      <c r="P696" t="s">
-        <v>3584</v>
-      </c>
-    </row>
-    <row r="697" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A697" s="1" t="s">
-        <v>3585</v>
-      </c>
-      <c r="B697" t="s">
-        <v>3577</v>
-      </c>
-      <c r="C697" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D697" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K697" t="s">
-        <v>107</v>
-      </c>
-      <c r="P697" t="s">
-        <v>3586</v>
-      </c>
-    </row>
-    <row r="698" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A698" s="1" t="s">
-        <v>3587</v>
-      </c>
-      <c r="B698" t="s">
-        <v>3577</v>
-      </c>
-      <c r="C698" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D698" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K698" t="s">
-        <v>107</v>
-      </c>
-      <c r="P698" t="s">
-        <v>3588</v>
-      </c>
-    </row>
-    <row r="699" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A699" s="1" t="s">
-        <v>3589</v>
-      </c>
-      <c r="B699" t="s">
-        <v>3577</v>
-      </c>
-      <c r="C699" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D699" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K699" t="s">
-        <v>107</v>
-      </c>
-      <c r="P699" t="s">
-        <v>3590</v>
-      </c>
-    </row>
-    <row r="700" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A700" s="1" t="s">
-        <v>3591</v>
-      </c>
-      <c r="B700" t="s">
-        <v>3577</v>
-      </c>
-      <c r="C700" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D700" t="s">
-        <v>1266</v>
-      </c>
-      <c r="E700" t="s">
-        <v>15</v>
-      </c>
-      <c r="K700" t="s">
-        <v>1203</v>
-      </c>
-      <c r="L700" t="s">
-        <v>107</v>
-      </c>
-      <c r="P700" t="s">
-        <v>3592</v>
-      </c>
-    </row>
-    <row r="701" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A701" s="1" t="s">
-        <v>3593</v>
-      </c>
-      <c r="B701" t="s">
-        <v>3577</v>
-      </c>
-      <c r="C701" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D701" t="s">
-        <v>1266</v>
-      </c>
-      <c r="E701" t="s">
-        <v>15</v>
-      </c>
-      <c r="K701" t="s">
-        <v>1203</v>
-      </c>
-      <c r="L701" t="s">
-        <v>107</v>
-      </c>
-      <c r="P701" t="s">
-        <v>3594</v>
-      </c>
-    </row>
-    <row r="702" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A702" s="1" t="s">
-        <v>3595</v>
-      </c>
-      <c r="B702" t="s">
-        <v>3577</v>
-      </c>
-      <c r="C702" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D702" t="s">
-        <v>1266</v>
-      </c>
-      <c r="E702" t="s">
-        <v>15</v>
-      </c>
-      <c r="K702" t="s">
-        <v>1203</v>
-      </c>
-      <c r="L702" t="s">
-        <v>107</v>
-      </c>
-      <c r="P702" t="s">
-        <v>3596</v>
-      </c>
-    </row>
-    <row r="703" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A703" s="1" t="s">
-        <v>3597</v>
-      </c>
-      <c r="B703" t="s">
-        <v>3577</v>
-      </c>
-      <c r="C703" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D703" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K703" t="s">
-        <v>107</v>
-      </c>
-      <c r="P703" t="s">
-        <v>3598</v>
-      </c>
-    </row>
-    <row r="704" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A704" s="1" t="s">
-        <v>3599</v>
-      </c>
-      <c r="B704" t="s">
-        <v>3577</v>
-      </c>
-      <c r="C704" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D704" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K704" t="s">
-        <v>107</v>
-      </c>
-      <c r="P704" t="s">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="705" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A705" s="1" t="s">
-        <v>3601</v>
-      </c>
-      <c r="B705" t="s">
-        <v>3577</v>
-      </c>
-      <c r="C705" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D705" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K705" t="s">
-        <v>107</v>
-      </c>
-      <c r="P705" t="s">
-        <v>3602</v>
-      </c>
-    </row>
-    <row r="706" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A706" s="1" t="s">
-        <v>3645</v>
-      </c>
-      <c r="B706" t="s">
-        <v>3646</v>
-      </c>
-      <c r="C706" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K706" t="s">
-        <v>107</v>
-      </c>
-      <c r="P706" t="s">
-        <v>3647</v>
-      </c>
-    </row>
-    <row r="707" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A707" s="1" t="s">
-        <v>3648</v>
-      </c>
-      <c r="B707" t="s">
-        <v>3646</v>
-      </c>
-      <c r="C707" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K707" t="s">
-        <v>107</v>
-      </c>
-      <c r="P707" t="s">
-        <v>3649</v>
-      </c>
-    </row>
-    <row r="708" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A708" s="1" t="s">
-        <v>3650</v>
-      </c>
-      <c r="B708" t="s">
-        <v>3646</v>
-      </c>
-      <c r="C708" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K708" t="s">
-        <v>107</v>
-      </c>
-      <c r="P708" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="709" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A709" s="1" t="s">
-        <v>3652</v>
-      </c>
-      <c r="B709" t="s">
-        <v>3646</v>
-      </c>
-      <c r="C709" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K709" t="s">
-        <v>3653</v>
-      </c>
-      <c r="L709" t="s">
-        <v>107</v>
-      </c>
-      <c r="P709" t="s">
-        <v>3654</v>
-      </c>
-    </row>
-    <row r="710" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A710" s="1" t="s">
-        <v>3655</v>
-      </c>
-      <c r="B710" t="s">
-        <v>3646</v>
-      </c>
-      <c r="C710" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K710" t="s">
-        <v>3653</v>
-      </c>
-      <c r="L710" t="s">
-        <v>107</v>
-      </c>
-      <c r="P710" t="s">
-        <v>3656</v>
-      </c>
-    </row>
-    <row r="711" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A711" s="1" t="s">
-        <v>3657</v>
-      </c>
-      <c r="B711" t="s">
-        <v>3658</v>
-      </c>
-      <c r="C711" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K711" t="s">
-        <v>3659</v>
-      </c>
-      <c r="P711" t="s">
-        <v>3660</v>
-      </c>
-    </row>
-    <row r="712" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A712" s="1" t="s">
-        <v>3661</v>
-      </c>
-      <c r="B712" t="s">
-        <v>3662</v>
-      </c>
-      <c r="C712" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K712" t="s">
-        <v>3653</v>
-      </c>
-      <c r="L712" t="s">
-        <v>107</v>
-      </c>
-      <c r="P712" t="s">
-        <v>3663</v>
-      </c>
-    </row>
-    <row r="713" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A713" s="1" t="s">
-        <v>3664</v>
-      </c>
-      <c r="B713" t="s">
-        <v>3662</v>
-      </c>
-      <c r="C713" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K713" t="s">
-        <v>3653</v>
-      </c>
-      <c r="L713" t="s">
-        <v>107</v>
-      </c>
-      <c r="P713" t="s">
-        <v>3665</v>
-      </c>
-    </row>
-    <row r="714" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A714" s="1" t="s">
-        <v>3666</v>
-      </c>
-      <c r="B714" t="s">
-        <v>3658</v>
-      </c>
-      <c r="C714" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K714" t="s">
-        <v>3659</v>
-      </c>
-      <c r="P714" t="s">
-        <v>3667</v>
-      </c>
-    </row>
-    <row r="715" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A715" s="1" t="s">
-        <v>3668</v>
-      </c>
-      <c r="B715" t="s">
-        <v>3658</v>
-      </c>
-      <c r="C715" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K715" t="s">
-        <v>3659</v>
-      </c>
-      <c r="P715" t="s">
-        <v>3669</v>
-      </c>
-    </row>
-    <row r="716" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A716" s="1" t="s">
-        <v>3670</v>
-      </c>
-      <c r="B716" t="s">
-        <v>3646</v>
-      </c>
-      <c r="C716" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K716" t="s">
-        <v>107</v>
-      </c>
-      <c r="P716" t="s">
-        <v>3671</v>
-      </c>
-    </row>
-    <row r="717" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A717" s="1" t="s">
-        <v>3672</v>
-      </c>
-      <c r="B717" t="s">
-        <v>3646</v>
-      </c>
-      <c r="C717" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K717" t="s">
-        <v>107</v>
-      </c>
-      <c r="P717" t="s">
-        <v>3673</v>
-      </c>
-    </row>
-    <row r="718" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A718" s="1" t="s">
-        <v>3674</v>
-      </c>
-      <c r="B718" t="s">
-        <v>3662</v>
-      </c>
-      <c r="C718" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K718" t="s">
-        <v>3653</v>
-      </c>
-      <c r="L718" t="s">
-        <v>107</v>
-      </c>
-      <c r="P718" t="s">
-        <v>3675</v>
-      </c>
-    </row>
-    <row r="719" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A719" s="1" t="s">
-        <v>3676</v>
-      </c>
-      <c r="B719" t="s">
-        <v>3658</v>
-      </c>
-      <c r="C719" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K719" t="s">
-        <v>3659</v>
-      </c>
-      <c r="P719" t="s">
-        <v>3677</v>
-      </c>
-    </row>
-    <row r="720" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A720" s="1" t="s">
-        <v>3678</v>
-      </c>
-      <c r="B720" t="s">
-        <v>3679</v>
-      </c>
-      <c r="C720" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K720" t="s">
-        <v>3659</v>
-      </c>
-      <c r="P720" t="s">
-        <v>3680</v>
-      </c>
-    </row>
-    <row r="721" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A721" s="1" t="s">
-        <v>3681</v>
-      </c>
-      <c r="B721" t="s">
-        <v>3679</v>
-      </c>
-      <c r="C721" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K721" t="s">
-        <v>3659</v>
-      </c>
-      <c r="P721" t="s">
-        <v>3682</v>
-      </c>
-    </row>
-    <row r="722" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A722" s="1" t="s">
-        <v>3683</v>
-      </c>
-      <c r="B722" t="s">
-        <v>3679</v>
-      </c>
-      <c r="C722" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K722" t="s">
-        <v>3659</v>
-      </c>
-      <c r="P722" t="s">
-        <v>3684</v>
-      </c>
-    </row>
-    <row r="723" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A723" s="1" t="s">
-        <v>3685</v>
-      </c>
-      <c r="B723" t="s">
-        <v>3679</v>
-      </c>
-      <c r="C723" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K723" t="s">
-        <v>3659</v>
-      </c>
-      <c r="P723" t="s">
-        <v>3686</v>
-      </c>
-    </row>
-    <row r="724" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A724" s="1" t="s">
-        <v>3687</v>
-      </c>
-      <c r="B724" t="s">
-        <v>3688</v>
-      </c>
-      <c r="C724" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D724" t="s">
-        <v>571</v>
-      </c>
-      <c r="K724" t="s">
-        <v>3689</v>
-      </c>
-      <c r="L724" t="s">
-        <v>1166</v>
-      </c>
-      <c r="P724" t="s">
-        <v>3690</v>
-      </c>
-    </row>
-    <row r="725" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A725" s="1" t="s">
-        <v>3691</v>
-      </c>
-      <c r="B725" t="s">
-        <v>3688</v>
-      </c>
-      <c r="C725" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D725" t="s">
-        <v>571</v>
-      </c>
-      <c r="K725" t="s">
-        <v>3689</v>
-      </c>
-      <c r="L725" t="s">
-        <v>1166</v>
-      </c>
-      <c r="P725" t="s">
-        <v>3692</v>
-      </c>
-    </row>
-    <row r="726" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A726" s="1" t="s">
-        <v>3693</v>
-      </c>
-      <c r="B726" t="s">
-        <v>3688</v>
-      </c>
-      <c r="C726" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D726" t="s">
-        <v>571</v>
-      </c>
-      <c r="K726" t="s">
-        <v>3689</v>
-      </c>
-      <c r="L726" t="s">
-        <v>1166</v>
-      </c>
-      <c r="P726" t="s">
-        <v>3694</v>
-      </c>
-    </row>
-    <row r="727" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A727" s="1" t="s">
-        <v>4214</v>
-      </c>
-      <c r="B727" t="s">
-        <v>4215</v>
-      </c>
-      <c r="C727" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D727" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K727" t="s">
-        <v>97</v>
-      </c>
-      <c r="P727" t="s">
-        <v>4216</v>
-      </c>
-    </row>
-    <row r="728" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A728" s="1" t="s">
-        <v>4217</v>
-      </c>
-      <c r="B728" t="s">
-        <v>4215</v>
-      </c>
-      <c r="C728" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D728" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K728" t="s">
-        <v>97</v>
-      </c>
-      <c r="P728" t="s">
-        <v>4218</v>
-      </c>
-    </row>
-    <row r="729" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A729" s="1" t="s">
-        <v>4219</v>
-      </c>
-      <c r="B729" t="s">
-        <v>4215</v>
-      </c>
-      <c r="C729" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D729" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K729" t="s">
-        <v>97</v>
-      </c>
-      <c r="P729" t="s">
-        <v>4220</v>
-      </c>
-    </row>
-    <row r="730" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A730" s="1" t="s">
-        <v>4221</v>
-      </c>
-      <c r="B730" t="s">
-        <v>4215</v>
-      </c>
-      <c r="C730" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D730" t="s">
-        <v>1266</v>
-      </c>
-      <c r="K730" t="s">
-        <v>97</v>
-      </c>
-      <c r="P730" t="s">
-        <v>4222</v>
-      </c>
-    </row>
-    <row r="731" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A731" s="1" t="s">
-        <v>4237</v>
-      </c>
-      <c r="B731" t="s">
-        <v>4238</v>
-      </c>
-      <c r="C731" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="P731" t="s">
-        <v>4239</v>
-      </c>
-    </row>
-    <row r="732" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A732" s="1" t="s">
-        <v>4240</v>
-      </c>
-      <c r="B732" t="s">
-        <v>4238</v>
-      </c>
-      <c r="C732" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="P732" t="s">
-        <v>4241</v>
       </c>
     </row>
   </sheetData>
@@ -31050,10 +28976,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P284"/>
+  <dimension ref="A1:P382"/>
   <sheetViews>
-    <sheetView topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="A285" sqref="A285"/>
+    <sheetView tabSelected="1" topLeftCell="A334" workbookViewId="0">
+      <selection activeCell="G354" sqref="G354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36957,6 +34883,2080 @@
       </c>
       <c r="P284" t="s">
         <v>1109</v>
+      </c>
+    </row>
+    <row r="285" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A285" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B285" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D285" t="s">
+        <v>15</v>
+      </c>
+      <c r="K285" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P285" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="286" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A286" s="1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B286" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D286" t="s">
+        <v>15</v>
+      </c>
+      <c r="K286" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P286" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="287" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A287" s="1" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B287" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D287" t="s">
+        <v>15</v>
+      </c>
+      <c r="K287" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P287" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="288" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A288" s="1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B288" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D288" t="s">
+        <v>15</v>
+      </c>
+      <c r="K288" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P288" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="289" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A289" s="1" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B289" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D289" t="s">
+        <v>15</v>
+      </c>
+      <c r="K289" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P289" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="290" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A290" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B290" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D290" t="s">
+        <v>15</v>
+      </c>
+      <c r="K290" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P290" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="291" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A291" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B291" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D291" t="s">
+        <v>15</v>
+      </c>
+      <c r="K291" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P291" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="292" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A292" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B292" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D292" t="s">
+        <v>15</v>
+      </c>
+      <c r="K292" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P292" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="293" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A293" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B293" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D293" t="s">
+        <v>15</v>
+      </c>
+      <c r="K293" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P293" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="294" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A294" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B294" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D294" t="s">
+        <v>15</v>
+      </c>
+      <c r="K294" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P294" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="295" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A295" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B295" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D295" t="s">
+        <v>15</v>
+      </c>
+      <c r="K295" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P295" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="296" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A296" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B296" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D296" t="s">
+        <v>15</v>
+      </c>
+      <c r="K296" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P296" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="297" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A297" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B297" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D297" t="s">
+        <v>15</v>
+      </c>
+      <c r="K297" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P297" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="298" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A298" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B298" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D298" t="s">
+        <v>15</v>
+      </c>
+      <c r="K298" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P298" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="299" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A299" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B299" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D299" t="s">
+        <v>15</v>
+      </c>
+      <c r="K299" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P299" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="300" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A300" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B300" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D300" t="s">
+        <v>15</v>
+      </c>
+      <c r="K300" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P300" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="301" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A301" s="1" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B301" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D301" t="s">
+        <v>15</v>
+      </c>
+      <c r="K301" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P301" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="302" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A302" s="1" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B302" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D302" t="s">
+        <v>15</v>
+      </c>
+      <c r="K302" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P302" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="303" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A303" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B303" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D303" t="s">
+        <v>15</v>
+      </c>
+      <c r="K303" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P303" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="304" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A304" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B304" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D304" t="s">
+        <v>15</v>
+      </c>
+      <c r="K304" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P304" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="305" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A305" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B305" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D305" t="s">
+        <v>15</v>
+      </c>
+      <c r="K305" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P305" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="306" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A306" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B306" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D306" t="s">
+        <v>15</v>
+      </c>
+      <c r="K306" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P306" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="307" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A307" s="1" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B307" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D307" t="s">
+        <v>15</v>
+      </c>
+      <c r="K307" t="s">
+        <v>1213</v>
+      </c>
+      <c r="P307" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="308" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A308" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="B308" t="s">
+        <v>2065</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D308" t="s">
+        <v>15</v>
+      </c>
+      <c r="K308" t="s">
+        <v>1538</v>
+      </c>
+      <c r="P308" t="s">
+        <v>2066</v>
+      </c>
+    </row>
+    <row r="309" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A309" s="1" t="s">
+        <v>2067</v>
+      </c>
+      <c r="B309" t="s">
+        <v>2065</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D309" t="s">
+        <v>15</v>
+      </c>
+      <c r="K309" t="s">
+        <v>1538</v>
+      </c>
+      <c r="P309" t="s">
+        <v>2068</v>
+      </c>
+    </row>
+    <row r="310" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A310" s="1" t="s">
+        <v>2069</v>
+      </c>
+      <c r="B310" t="s">
+        <v>2065</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D310" t="s">
+        <v>15</v>
+      </c>
+      <c r="K310" t="s">
+        <v>1538</v>
+      </c>
+      <c r="P310" t="s">
+        <v>2070</v>
+      </c>
+    </row>
+    <row r="311" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A311" s="1" t="s">
+        <v>2071</v>
+      </c>
+      <c r="B311" t="s">
+        <v>2065</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D311" t="s">
+        <v>15</v>
+      </c>
+      <c r="K311" t="s">
+        <v>1538</v>
+      </c>
+      <c r="P311" t="s">
+        <v>2072</v>
+      </c>
+    </row>
+    <row r="312" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A312" s="1" t="s">
+        <v>2073</v>
+      </c>
+      <c r="B312" t="s">
+        <v>2065</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D312" t="s">
+        <v>15</v>
+      </c>
+      <c r="K312" t="s">
+        <v>1538</v>
+      </c>
+      <c r="P312" t="s">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="313" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A313" s="1" t="s">
+        <v>2075</v>
+      </c>
+      <c r="B313" t="s">
+        <v>2065</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D313" t="s">
+        <v>15</v>
+      </c>
+      <c r="K313" t="s">
+        <v>1538</v>
+      </c>
+      <c r="P313" t="s">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="314" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A314" s="1" t="s">
+        <v>2077</v>
+      </c>
+      <c r="B314" t="s">
+        <v>2065</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D314" t="s">
+        <v>15</v>
+      </c>
+      <c r="K314" t="s">
+        <v>1538</v>
+      </c>
+      <c r="P314" t="s">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="315" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A315" s="1" t="s">
+        <v>2385</v>
+      </c>
+      <c r="B315" t="s">
+        <v>2386</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D315" t="s">
+        <v>571</v>
+      </c>
+      <c r="K315" t="s">
+        <v>369</v>
+      </c>
+      <c r="L315" t="s">
+        <v>192</v>
+      </c>
+      <c r="P315" t="s">
+        <v>2387</v>
+      </c>
+    </row>
+    <row r="316" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A316" s="1" t="s">
+        <v>2388</v>
+      </c>
+      <c r="B316" t="s">
+        <v>2386</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D316" t="s">
+        <v>571</v>
+      </c>
+      <c r="K316" t="s">
+        <v>369</v>
+      </c>
+      <c r="L316" t="s">
+        <v>192</v>
+      </c>
+      <c r="P316" t="s">
+        <v>2389</v>
+      </c>
+    </row>
+    <row r="317" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A317" s="1" t="s">
+        <v>2390</v>
+      </c>
+      <c r="B317" t="s">
+        <v>2386</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D317" t="s">
+        <v>571</v>
+      </c>
+      <c r="K317" t="s">
+        <v>369</v>
+      </c>
+      <c r="L317" t="s">
+        <v>192</v>
+      </c>
+      <c r="P317" t="s">
+        <v>2391</v>
+      </c>
+    </row>
+    <row r="318" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A318" s="1" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B318" t="s">
+        <v>2386</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D318" t="s">
+        <v>571</v>
+      </c>
+      <c r="K318" t="s">
+        <v>369</v>
+      </c>
+      <c r="L318" t="s">
+        <v>192</v>
+      </c>
+      <c r="P318" t="s">
+        <v>2393</v>
+      </c>
+    </row>
+    <row r="319" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A319" s="1" t="s">
+        <v>2844</v>
+      </c>
+      <c r="B319" t="s">
+        <v>2845</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D319" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K319" t="s">
+        <v>16</v>
+      </c>
+      <c r="P319" t="s">
+        <v>2846</v>
+      </c>
+    </row>
+    <row r="320" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A320" s="1" t="s">
+        <v>2847</v>
+      </c>
+      <c r="B320" t="s">
+        <v>2845</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D320" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K320" t="s">
+        <v>16</v>
+      </c>
+      <c r="P320" t="s">
+        <v>2848</v>
+      </c>
+    </row>
+    <row r="321" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A321" s="1" t="s">
+        <v>2849</v>
+      </c>
+      <c r="B321" t="s">
+        <v>2845</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D321" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K321" t="s">
+        <v>16</v>
+      </c>
+      <c r="P321" t="s">
+        <v>2850</v>
+      </c>
+    </row>
+    <row r="322" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A322" s="1" t="s">
+        <v>2851</v>
+      </c>
+      <c r="B322" t="s">
+        <v>2845</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D322" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K322" t="s">
+        <v>16</v>
+      </c>
+      <c r="P322" t="s">
+        <v>2852</v>
+      </c>
+    </row>
+    <row r="323" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A323" s="1" t="s">
+        <v>2853</v>
+      </c>
+      <c r="B323" t="s">
+        <v>2845</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D323" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K323" t="s">
+        <v>16</v>
+      </c>
+      <c r="P323" t="s">
+        <v>2854</v>
+      </c>
+    </row>
+    <row r="324" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A324" s="1" t="s">
+        <v>2855</v>
+      </c>
+      <c r="B324" t="s">
+        <v>2845</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D324" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K324" t="s">
+        <v>16</v>
+      </c>
+      <c r="P324" t="s">
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="325" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A325" s="1" t="s">
+        <v>2857</v>
+      </c>
+      <c r="B325" t="s">
+        <v>2845</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D325" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K325" t="s">
+        <v>16</v>
+      </c>
+      <c r="P325" t="s">
+        <v>2858</v>
+      </c>
+    </row>
+    <row r="326" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A326" s="1" t="s">
+        <v>2859</v>
+      </c>
+      <c r="B326" t="s">
+        <v>2845</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D326" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K326" t="s">
+        <v>16</v>
+      </c>
+      <c r="P326" t="s">
+        <v>2860</v>
+      </c>
+    </row>
+    <row r="327" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A327" s="1" t="s">
+        <v>2861</v>
+      </c>
+      <c r="B327" t="s">
+        <v>2845</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D327" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K327" t="s">
+        <v>16</v>
+      </c>
+      <c r="P327" t="s">
+        <v>2862</v>
+      </c>
+    </row>
+    <row r="328" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A328" s="1" t="s">
+        <v>2863</v>
+      </c>
+      <c r="B328" t="s">
+        <v>2845</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D328" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K328" t="s">
+        <v>16</v>
+      </c>
+      <c r="P328" t="s">
+        <v>2864</v>
+      </c>
+    </row>
+    <row r="329" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A329" s="1" t="s">
+        <v>2865</v>
+      </c>
+      <c r="B329" t="s">
+        <v>2845</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D329" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K329" t="s">
+        <v>16</v>
+      </c>
+      <c r="P329" t="s">
+        <v>2866</v>
+      </c>
+    </row>
+    <row r="330" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A330" s="1" t="s">
+        <v>2867</v>
+      </c>
+      <c r="B330" t="s">
+        <v>2845</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D330" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K330" t="s">
+        <v>16</v>
+      </c>
+      <c r="P330" t="s">
+        <v>2868</v>
+      </c>
+    </row>
+    <row r="331" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A331" s="1" t="s">
+        <v>2915</v>
+      </c>
+      <c r="B331" t="s">
+        <v>2916</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D331" t="s">
+        <v>525</v>
+      </c>
+      <c r="K331" t="s">
+        <v>369</v>
+      </c>
+      <c r="L331" t="s">
+        <v>363</v>
+      </c>
+      <c r="P331" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="332" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A332" s="1" t="s">
+        <v>2918</v>
+      </c>
+      <c r="B332" t="s">
+        <v>2916</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D332" t="s">
+        <v>525</v>
+      </c>
+      <c r="K332" t="s">
+        <v>369</v>
+      </c>
+      <c r="L332" t="s">
+        <v>363</v>
+      </c>
+      <c r="P332" t="s">
+        <v>2919</v>
+      </c>
+    </row>
+    <row r="333" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A333" s="1" t="s">
+        <v>2920</v>
+      </c>
+      <c r="B333" t="s">
+        <v>2916</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D333" t="s">
+        <v>525</v>
+      </c>
+      <c r="K333" t="s">
+        <v>369</v>
+      </c>
+      <c r="L333" t="s">
+        <v>363</v>
+      </c>
+      <c r="P333" t="s">
+        <v>2921</v>
+      </c>
+    </row>
+    <row r="334" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A334" s="1" t="s">
+        <v>2933</v>
+      </c>
+      <c r="B334" t="s">
+        <v>2934</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D334" t="s">
+        <v>5178</v>
+      </c>
+      <c r="K334" t="s">
+        <v>369</v>
+      </c>
+      <c r="L334" t="s">
+        <v>1534</v>
+      </c>
+      <c r="P334" t="s">
+        <v>2936</v>
+      </c>
+    </row>
+    <row r="335" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A335" s="1" t="s">
+        <v>2937</v>
+      </c>
+      <c r="B335" t="s">
+        <v>2934</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D335" t="s">
+        <v>5178</v>
+      </c>
+      <c r="K335" t="s">
+        <v>369</v>
+      </c>
+      <c r="L335" t="s">
+        <v>1534</v>
+      </c>
+      <c r="P335" t="s">
+        <v>2938</v>
+      </c>
+    </row>
+    <row r="336" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A336" s="1" t="s">
+        <v>2939</v>
+      </c>
+      <c r="B336" t="s">
+        <v>2940</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D336" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K336" t="s">
+        <v>369</v>
+      </c>
+      <c r="L336" t="s">
+        <v>388</v>
+      </c>
+      <c r="M336" t="s">
+        <v>1918</v>
+      </c>
+      <c r="P336" t="s">
+        <v>2941</v>
+      </c>
+    </row>
+    <row r="337" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A337" s="1" t="s">
+        <v>2942</v>
+      </c>
+      <c r="B337" t="s">
+        <v>2940</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D337" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K337" t="s">
+        <v>369</v>
+      </c>
+      <c r="L337" t="s">
+        <v>388</v>
+      </c>
+      <c r="M337" t="s">
+        <v>1918</v>
+      </c>
+      <c r="P337" t="s">
+        <v>2943</v>
+      </c>
+    </row>
+    <row r="338" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A338" s="1" t="s">
+        <v>2944</v>
+      </c>
+      <c r="B338" t="s">
+        <v>2940</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D338" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K338" t="s">
+        <v>369</v>
+      </c>
+      <c r="L338" t="s">
+        <v>388</v>
+      </c>
+      <c r="M338" t="s">
+        <v>1918</v>
+      </c>
+      <c r="P338" t="s">
+        <v>2945</v>
+      </c>
+    </row>
+    <row r="339" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A339" s="1" t="s">
+        <v>2946</v>
+      </c>
+      <c r="B339" t="s">
+        <v>2940</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D339" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K339" t="s">
+        <v>369</v>
+      </c>
+      <c r="L339" t="s">
+        <v>388</v>
+      </c>
+      <c r="M339" t="s">
+        <v>1918</v>
+      </c>
+      <c r="P339" t="s">
+        <v>2947</v>
+      </c>
+    </row>
+    <row r="340" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A340" s="1" t="s">
+        <v>3185</v>
+      </c>
+      <c r="B340" t="s">
+        <v>3186</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D340" t="s">
+        <v>525</v>
+      </c>
+      <c r="E340" t="s">
+        <v>15</v>
+      </c>
+      <c r="F340" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="K340" t="s">
+        <v>97</v>
+      </c>
+      <c r="L340" t="s">
+        <v>192</v>
+      </c>
+      <c r="P340" t="s">
+        <v>3187</v>
+      </c>
+    </row>
+    <row r="341" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A341" s="1" t="s">
+        <v>3225</v>
+      </c>
+      <c r="B341" t="s">
+        <v>3226</v>
+      </c>
+      <c r="C341" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D341" t="s">
+        <v>15</v>
+      </c>
+      <c r="K341" t="s">
+        <v>192</v>
+      </c>
+      <c r="L341" t="s">
+        <v>3198</v>
+      </c>
+      <c r="M341" t="s">
+        <v>852</v>
+      </c>
+      <c r="P341" t="s">
+        <v>3227</v>
+      </c>
+    </row>
+    <row r="342" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A342" s="1" t="s">
+        <v>3228</v>
+      </c>
+      <c r="B342" t="s">
+        <v>3226</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D342" t="s">
+        <v>15</v>
+      </c>
+      <c r="K342" t="s">
+        <v>192</v>
+      </c>
+      <c r="L342" t="s">
+        <v>3198</v>
+      </c>
+      <c r="M342" t="s">
+        <v>852</v>
+      </c>
+      <c r="P342" t="s">
+        <v>3229</v>
+      </c>
+    </row>
+    <row r="343" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A343" s="1" t="s">
+        <v>3240</v>
+      </c>
+      <c r="B343" t="s">
+        <v>3226</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D343" t="s">
+        <v>15</v>
+      </c>
+      <c r="K343" t="s">
+        <v>192</v>
+      </c>
+      <c r="L343" t="s">
+        <v>3198</v>
+      </c>
+      <c r="M343" t="s">
+        <v>852</v>
+      </c>
+      <c r="P343" t="s">
+        <v>3241</v>
+      </c>
+    </row>
+    <row r="344" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A344" s="1" t="s">
+        <v>3242</v>
+      </c>
+      <c r="B344" t="s">
+        <v>3226</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D344" t="s">
+        <v>15</v>
+      </c>
+      <c r="K344" t="s">
+        <v>192</v>
+      </c>
+      <c r="L344" t="s">
+        <v>3198</v>
+      </c>
+      <c r="M344" t="s">
+        <v>852</v>
+      </c>
+      <c r="P344" t="s">
+        <v>3243</v>
+      </c>
+    </row>
+    <row r="345" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A345" s="1" t="s">
+        <v>3281</v>
+      </c>
+      <c r="B345" t="s">
+        <v>3282</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D345" t="s">
+        <v>525</v>
+      </c>
+      <c r="K345" t="s">
+        <v>613</v>
+      </c>
+      <c r="P345" t="s">
+        <v>3283</v>
+      </c>
+    </row>
+    <row r="346" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A346" s="1" t="s">
+        <v>3284</v>
+      </c>
+      <c r="B346" t="s">
+        <v>3282</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D346" t="s">
+        <v>525</v>
+      </c>
+      <c r="K346" t="s">
+        <v>613</v>
+      </c>
+      <c r="P346" t="s">
+        <v>3285</v>
+      </c>
+    </row>
+    <row r="347" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A347" s="1" t="s">
+        <v>3286</v>
+      </c>
+      <c r="B347" t="s">
+        <v>3282</v>
+      </c>
+      <c r="C347" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D347" t="s">
+        <v>525</v>
+      </c>
+      <c r="K347" t="s">
+        <v>613</v>
+      </c>
+      <c r="P347" t="s">
+        <v>3287</v>
+      </c>
+    </row>
+    <row r="348" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A348" s="1" t="s">
+        <v>3288</v>
+      </c>
+      <c r="B348" t="s">
+        <v>3282</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D348" t="s">
+        <v>525</v>
+      </c>
+      <c r="K348" t="s">
+        <v>613</v>
+      </c>
+      <c r="P348" t="s">
+        <v>3289</v>
+      </c>
+    </row>
+    <row r="349" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A349" s="1" t="s">
+        <v>3304</v>
+      </c>
+      <c r="B349" t="s">
+        <v>3305</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>2960</v>
+      </c>
+      <c r="D349" t="s">
+        <v>15</v>
+      </c>
+      <c r="K349" t="s">
+        <v>369</v>
+      </c>
+      <c r="L349" t="s">
+        <v>2681</v>
+      </c>
+      <c r="P349" t="s">
+        <v>3306</v>
+      </c>
+    </row>
+    <row r="350" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A350" s="1" t="s">
+        <v>3307</v>
+      </c>
+      <c r="B350" t="s">
+        <v>3305</v>
+      </c>
+      <c r="C350" s="1" t="s">
+        <v>2960</v>
+      </c>
+      <c r="D350" t="s">
+        <v>15</v>
+      </c>
+      <c r="K350" t="s">
+        <v>369</v>
+      </c>
+      <c r="L350" t="s">
+        <v>2681</v>
+      </c>
+      <c r="P350" t="s">
+        <v>3308</v>
+      </c>
+    </row>
+    <row r="351" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A351" s="1" t="s">
+        <v>3309</v>
+      </c>
+      <c r="B351" t="s">
+        <v>3305</v>
+      </c>
+      <c r="C351" s="1" t="s">
+        <v>2960</v>
+      </c>
+      <c r="D351" t="s">
+        <v>15</v>
+      </c>
+      <c r="K351" t="s">
+        <v>369</v>
+      </c>
+      <c r="L351" t="s">
+        <v>2681</v>
+      </c>
+      <c r="P351" t="s">
+        <v>3310</v>
+      </c>
+    </row>
+    <row r="352" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A352" s="1" t="s">
+        <v>3311</v>
+      </c>
+      <c r="B352" t="s">
+        <v>3305</v>
+      </c>
+      <c r="C352" s="1" t="s">
+        <v>2960</v>
+      </c>
+      <c r="D352" t="s">
+        <v>15</v>
+      </c>
+      <c r="K352" t="s">
+        <v>369</v>
+      </c>
+      <c r="L352" t="s">
+        <v>2681</v>
+      </c>
+      <c r="P352" t="s">
+        <v>3312</v>
+      </c>
+    </row>
+    <row r="353" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A353" s="1" t="s">
+        <v>3313</v>
+      </c>
+      <c r="B353" t="s">
+        <v>3305</v>
+      </c>
+      <c r="C353" s="1" t="s">
+        <v>2960</v>
+      </c>
+      <c r="D353" t="s">
+        <v>15</v>
+      </c>
+      <c r="K353" t="s">
+        <v>369</v>
+      </c>
+      <c r="L353" t="s">
+        <v>2681</v>
+      </c>
+      <c r="P353" t="s">
+        <v>3314</v>
+      </c>
+    </row>
+    <row r="354" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A354" s="1" t="s">
+        <v>3576</v>
+      </c>
+      <c r="B354" t="s">
+        <v>3577</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="K354" t="s">
+        <v>107</v>
+      </c>
+      <c r="L354" t="s">
+        <v>451</v>
+      </c>
+      <c r="M354" t="s">
+        <v>192</v>
+      </c>
+      <c r="P354" t="s">
+        <v>3578</v>
+      </c>
+    </row>
+    <row r="355" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A355" s="1" t="s">
+        <v>3579</v>
+      </c>
+      <c r="B355" t="s">
+        <v>3577</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="K355" t="s">
+        <v>107</v>
+      </c>
+      <c r="L355" t="s">
+        <v>451</v>
+      </c>
+      <c r="M355" t="s">
+        <v>192</v>
+      </c>
+      <c r="P355" t="s">
+        <v>3580</v>
+      </c>
+    </row>
+    <row r="356" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A356" s="1" t="s">
+        <v>3581</v>
+      </c>
+      <c r="B356" t="s">
+        <v>3577</v>
+      </c>
+      <c r="C356" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="K356" t="s">
+        <v>107</v>
+      </c>
+      <c r="L356" t="s">
+        <v>451</v>
+      </c>
+      <c r="M356" t="s">
+        <v>192</v>
+      </c>
+      <c r="P356" t="s">
+        <v>3582</v>
+      </c>
+    </row>
+    <row r="357" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A357" s="1" t="s">
+        <v>3583</v>
+      </c>
+      <c r="B357" t="s">
+        <v>3577</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="K357" t="s">
+        <v>107</v>
+      </c>
+      <c r="L357" t="s">
+        <v>451</v>
+      </c>
+      <c r="M357" t="s">
+        <v>192</v>
+      </c>
+      <c r="P357" t="s">
+        <v>3584</v>
+      </c>
+    </row>
+    <row r="358" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A358" s="1" t="s">
+        <v>3585</v>
+      </c>
+      <c r="B358" t="s">
+        <v>3577</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D358" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K358" t="s">
+        <v>107</v>
+      </c>
+      <c r="P358" t="s">
+        <v>3586</v>
+      </c>
+    </row>
+    <row r="359" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A359" s="1" t="s">
+        <v>3587</v>
+      </c>
+      <c r="B359" t="s">
+        <v>3577</v>
+      </c>
+      <c r="C359" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D359" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K359" t="s">
+        <v>107</v>
+      </c>
+      <c r="P359" t="s">
+        <v>3588</v>
+      </c>
+    </row>
+    <row r="360" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A360" s="1" t="s">
+        <v>3589</v>
+      </c>
+      <c r="B360" t="s">
+        <v>3577</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D360" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K360" t="s">
+        <v>107</v>
+      </c>
+      <c r="P360" t="s">
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="361" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A361" s="1" t="s">
+        <v>3591</v>
+      </c>
+      <c r="B361" t="s">
+        <v>3577</v>
+      </c>
+      <c r="C361" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D361" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E361" t="s">
+        <v>15</v>
+      </c>
+      <c r="K361" t="s">
+        <v>1203</v>
+      </c>
+      <c r="L361" t="s">
+        <v>107</v>
+      </c>
+      <c r="P361" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="362" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A362" s="1" t="s">
+        <v>3593</v>
+      </c>
+      <c r="B362" t="s">
+        <v>3577</v>
+      </c>
+      <c r="C362" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D362" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E362" t="s">
+        <v>15</v>
+      </c>
+      <c r="K362" t="s">
+        <v>1203</v>
+      </c>
+      <c r="L362" t="s">
+        <v>107</v>
+      </c>
+      <c r="P362" t="s">
+        <v>3594</v>
+      </c>
+    </row>
+    <row r="363" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A363" s="1" t="s">
+        <v>3595</v>
+      </c>
+      <c r="B363" t="s">
+        <v>3577</v>
+      </c>
+      <c r="C363" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D363" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E363" t="s">
+        <v>15</v>
+      </c>
+      <c r="K363" t="s">
+        <v>1203</v>
+      </c>
+      <c r="L363" t="s">
+        <v>107</v>
+      </c>
+      <c r="P363" t="s">
+        <v>3596</v>
+      </c>
+    </row>
+    <row r="364" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A364" s="1" t="s">
+        <v>3597</v>
+      </c>
+      <c r="B364" t="s">
+        <v>3577</v>
+      </c>
+      <c r="C364" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D364" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K364" t="s">
+        <v>107</v>
+      </c>
+      <c r="P364" t="s">
+        <v>3598</v>
+      </c>
+    </row>
+    <row r="365" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A365" s="1" t="s">
+        <v>3599</v>
+      </c>
+      <c r="B365" t="s">
+        <v>3577</v>
+      </c>
+      <c r="C365" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D365" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K365" t="s">
+        <v>107</v>
+      </c>
+      <c r="P365" t="s">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="366" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A366" s="1" t="s">
+        <v>3601</v>
+      </c>
+      <c r="B366" t="s">
+        <v>3577</v>
+      </c>
+      <c r="C366" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D366" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K366" t="s">
+        <v>107</v>
+      </c>
+      <c r="P366" t="s">
+        <v>3602</v>
+      </c>
+    </row>
+    <row r="367" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A367" s="1" t="s">
+        <v>3661</v>
+      </c>
+      <c r="B367" t="s">
+        <v>3662</v>
+      </c>
+      <c r="C367" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="K367" t="s">
+        <v>3653</v>
+      </c>
+      <c r="L367" t="s">
+        <v>107</v>
+      </c>
+      <c r="P367" t="s">
+        <v>3663</v>
+      </c>
+    </row>
+    <row r="368" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A368" s="1" t="s">
+        <v>3664</v>
+      </c>
+      <c r="B368" t="s">
+        <v>3662</v>
+      </c>
+      <c r="C368" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="K368" t="s">
+        <v>3653</v>
+      </c>
+      <c r="L368" t="s">
+        <v>107</v>
+      </c>
+      <c r="P368" t="s">
+        <v>3665</v>
+      </c>
+    </row>
+    <row r="369" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A369" s="1" t="s">
+        <v>3674</v>
+      </c>
+      <c r="B369" t="s">
+        <v>3662</v>
+      </c>
+      <c r="C369" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="K369" t="s">
+        <v>3653</v>
+      </c>
+      <c r="L369" t="s">
+        <v>107</v>
+      </c>
+      <c r="P369" t="s">
+        <v>3675</v>
+      </c>
+    </row>
+    <row r="370" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A370" s="1" t="s">
+        <v>3678</v>
+      </c>
+      <c r="B370" t="s">
+        <v>3679</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="K370" t="s">
+        <v>3659</v>
+      </c>
+      <c r="P370" t="s">
+        <v>3680</v>
+      </c>
+    </row>
+    <row r="371" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A371" s="1" t="s">
+        <v>3681</v>
+      </c>
+      <c r="B371" t="s">
+        <v>3679</v>
+      </c>
+      <c r="C371" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="K371" t="s">
+        <v>3659</v>
+      </c>
+      <c r="P371" t="s">
+        <v>3682</v>
+      </c>
+    </row>
+    <row r="372" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A372" s="1" t="s">
+        <v>3683</v>
+      </c>
+      <c r="B372" t="s">
+        <v>3679</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="K372" t="s">
+        <v>3659</v>
+      </c>
+      <c r="P372" t="s">
+        <v>3684</v>
+      </c>
+    </row>
+    <row r="373" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A373" s="1" t="s">
+        <v>3685</v>
+      </c>
+      <c r="B373" t="s">
+        <v>3679</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="K373" t="s">
+        <v>3659</v>
+      </c>
+      <c r="P373" t="s">
+        <v>3686</v>
+      </c>
+    </row>
+    <row r="374" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A374" s="1" t="s">
+        <v>3687</v>
+      </c>
+      <c r="B374" t="s">
+        <v>3688</v>
+      </c>
+      <c r="C374" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D374" t="s">
+        <v>571</v>
+      </c>
+      <c r="K374" t="s">
+        <v>3689</v>
+      </c>
+      <c r="L374" t="s">
+        <v>1166</v>
+      </c>
+      <c r="P374" t="s">
+        <v>3690</v>
+      </c>
+    </row>
+    <row r="375" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A375" s="1" t="s">
+        <v>3691</v>
+      </c>
+      <c r="B375" t="s">
+        <v>3688</v>
+      </c>
+      <c r="C375" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D375" t="s">
+        <v>571</v>
+      </c>
+      <c r="K375" t="s">
+        <v>3689</v>
+      </c>
+      <c r="L375" t="s">
+        <v>1166</v>
+      </c>
+      <c r="P375" t="s">
+        <v>3692</v>
+      </c>
+    </row>
+    <row r="376" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A376" s="1" t="s">
+        <v>3693</v>
+      </c>
+      <c r="B376" t="s">
+        <v>3688</v>
+      </c>
+      <c r="C376" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D376" t="s">
+        <v>571</v>
+      </c>
+      <c r="K376" t="s">
+        <v>3689</v>
+      </c>
+      <c r="L376" t="s">
+        <v>1166</v>
+      </c>
+      <c r="P376" t="s">
+        <v>3694</v>
+      </c>
+    </row>
+    <row r="377" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A377" s="1" t="s">
+        <v>4214</v>
+      </c>
+      <c r="B377" t="s">
+        <v>4215</v>
+      </c>
+      <c r="C377" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D377" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K377" t="s">
+        <v>97</v>
+      </c>
+      <c r="P377" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="378" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A378" s="1" t="s">
+        <v>4217</v>
+      </c>
+      <c r="B378" t="s">
+        <v>4215</v>
+      </c>
+      <c r="C378" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D378" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K378" t="s">
+        <v>97</v>
+      </c>
+      <c r="P378" t="s">
+        <v>4218</v>
+      </c>
+    </row>
+    <row r="379" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A379" s="1" t="s">
+        <v>4219</v>
+      </c>
+      <c r="B379" t="s">
+        <v>4215</v>
+      </c>
+      <c r="C379" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D379" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K379" t="s">
+        <v>97</v>
+      </c>
+      <c r="P379" t="s">
+        <v>4220</v>
+      </c>
+    </row>
+    <row r="380" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A380" s="1" t="s">
+        <v>4221</v>
+      </c>
+      <c r="B380" t="s">
+        <v>4215</v>
+      </c>
+      <c r="C380" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D380" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K380" t="s">
+        <v>97</v>
+      </c>
+      <c r="P380" t="s">
+        <v>4222</v>
+      </c>
+    </row>
+    <row r="381" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A381" s="1" t="s">
+        <v>4237</v>
+      </c>
+      <c r="B381" t="s">
+        <v>4238</v>
+      </c>
+      <c r="C381" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="P381" t="s">
+        <v>4239</v>
+      </c>
+    </row>
+    <row r="382" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A382" s="1" t="s">
+        <v>4240</v>
+      </c>
+      <c r="B382" t="s">
+        <v>4238</v>
+      </c>
+      <c r="C382" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="P382" t="s">
+        <v>4241</v>
       </c>
     </row>
   </sheetData>
@@ -37354,8 +37354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A502" workbookViewId="0">
-      <selection activeCell="I521" sqref="I521"/>
+    <sheetView topLeftCell="E1171" workbookViewId="0">
+      <selection activeCell="P1187" sqref="P1187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>